<commit_message>
Save for Clovis PC
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -2925,13 +2925,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>236.000</v>
+        <v>232.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>131871.15</v>
+        <v>129636.04</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3237,13 +3237,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>2644.000</v>
+        <v>2640.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>27240.78</v>
+        <v>27199.57</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3887,13 +3887,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>2866.000</v>
+        <v>2856.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>74650.90</v>
+        <v>74390.43</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -4251,13 +4251,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>2637.000</v>
+        <v>2633.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>363233.60</v>
+        <v>362682.61</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4823,13 +4823,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>7451.000</v>
+        <v>7442.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>28807.22</v>
+        <v>28772.42</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -6253,13 +6253,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>1954.000</v>
+        <v>1950.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>36588.65</v>
+        <v>36513.75</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -7787,13 +7787,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>21212.300</v>
+        <v>21178.300</v>
       </c>
       <c r="G232" t="s">
         <v>438</v>
       </c>
       <c r="H232" s="3">
-        <v>48145.31</v>
+        <v>48068.14</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -8203,13 +8203,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>4581.000</v>
+        <v>4576.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>11499.90</v>
+        <v>11487.35</v>
       </c>
     </row>
     <row r="249" spans="1:8">

</xml_diff>

<commit_message>
Exclude troca por uma religada
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="545">
   <si>
     <t>4600041302</t>
   </si>
@@ -653,6 +653,12 @@
   </si>
   <si>
     <t>JUNTA FF BOL VAR DIA DEMAX250 X DEMIN200</t>
+  </si>
+  <si>
+    <t>30005604</t>
+  </si>
+  <si>
+    <t>JUNTA FF BOL VAR DIA DEMAX275 X DEMIN225</t>
   </si>
   <si>
     <t>30002952</t>
@@ -1746,7 +1752,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H266"/>
+  <dimension ref="A1:H267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,28 +1772,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1807,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>82.000</v>
+        <v>84.000</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3">
-        <v>22632.36</v>
+        <v>23184.37</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2151,7 +2157,7 @@
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>13440.90</v>
+        <v>13440.91</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2463,7 +2469,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>50.78</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2567,7 +2573,7 @@
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>542.22</v>
+        <v>542.21</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2925,13 +2931,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>232.000</v>
+        <v>281.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>129636.04</v>
+        <v>157016.05</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3061,7 +3067,7 @@
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>1937.55</v>
+        <v>2092.96</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3185,13 +3191,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>1294.000</v>
+        <v>1279.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>11790.87</v>
+        <v>11654.21</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3237,13 +3243,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>2640.000</v>
+        <v>3031.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>27199.57</v>
+        <v>31228.01</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3445,13 +3451,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>59.49</v>
+        <v>237.96</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3601,13 +3607,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>40.000</v>
+        <v>42.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>5018.74</v>
+        <v>5269.67</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3887,13 +3893,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>2856.000</v>
+        <v>2849.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>74390.43</v>
+        <v>74208.08</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3945,7 +3951,7 @@
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>651.70</v>
+        <v>651.71</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -4251,13 +4257,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>2633.000</v>
+        <v>2622.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>362682.61</v>
+        <v>361167.39</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4543,7 +4549,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>1166.57</v>
+        <v>1033.65</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4563,13 +4569,13 @@
         <v>217</v>
       </c>
       <c r="F108" s="2">
-        <v>8.000</v>
+        <v>2.000</v>
       </c>
       <c r="G108" t="s">
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>2825.06</v>
+        <v>1166.57</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4589,13 +4595,13 @@
         <v>219</v>
       </c>
       <c r="F109" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>91.20</v>
+        <v>2825.06</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4615,13 +4621,13 @@
         <v>221</v>
       </c>
       <c r="F110" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G110" t="s">
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>719.47</v>
+        <v>91.20</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4641,13 +4647,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>545.000</v>
+        <v>2.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>20225.32</v>
+        <v>719.47</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4667,13 +4673,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>352.000</v>
+        <v>545.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>23009.79</v>
+        <v>20225.32</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4693,13 +4699,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>993.000</v>
+        <v>352.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>32716.37</v>
+        <v>23009.79</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4719,13 +4725,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>176.000</v>
+        <v>993.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>9043.46</v>
+        <v>32716.37</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4745,13 +4751,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>61.000</v>
+        <v>176.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>6216.97</v>
+        <v>9043.46</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4777,7 +4783,7 @@
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>1519.40</v>
+        <v>4586.29</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4797,13 +4803,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>9.000</v>
+        <v>45.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>1675.75</v>
+        <v>1519.40</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4823,13 +4829,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>7442.000</v>
+        <v>9.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>28772.42</v>
+        <v>1675.75</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4849,13 +4855,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>2.000</v>
+        <v>7400.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>2463.85</v>
+        <v>28609.80</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4881,7 +4887,7 @@
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>4533.88</v>
+        <v>2463.85</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4901,13 +4907,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>6385.34</v>
+        <v>4533.88</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4927,13 +4933,13 @@
         <v>245</v>
       </c>
       <c r="F122" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>12368.67</v>
+        <v>6385.34</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4953,13 +4959,13 @@
         <v>247</v>
       </c>
       <c r="F123" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G123" t="s">
         <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>3260.53</v>
+        <v>12368.67</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4979,13 +4985,13 @@
         <v>249</v>
       </c>
       <c r="F124" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>3527.49</v>
+        <v>3260.53</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -5005,13 +5011,13 @@
         <v>251</v>
       </c>
       <c r="F125" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G125" t="s">
         <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>6294.26</v>
+        <v>3527.49</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5031,13 +5037,13 @@
         <v>253</v>
       </c>
       <c r="F126" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G126" t="s">
         <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>4585.00</v>
+        <v>6294.26</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5057,13 +5063,13 @@
         <v>255</v>
       </c>
       <c r="F127" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G127" t="s">
         <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>14225.45</v>
+        <v>4585.00</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -5083,13 +5089,13 @@
         <v>257</v>
       </c>
       <c r="F128" s="2">
-        <v>69.000</v>
+        <v>2.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>99523.18</v>
+        <v>14225.45</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5109,13 +5115,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>562.000</v>
+        <v>69.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>3181.36</v>
+        <v>99523.18</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5135,13 +5141,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>261.000</v>
+        <v>562.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>2053.88</v>
+        <v>3181.36</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5161,13 +5167,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>92.000</v>
+        <v>261.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>1442.37</v>
+        <v>2053.88</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5187,13 +5193,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>113.000</v>
+        <v>92.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>1540.59</v>
+        <v>1442.37</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5213,13 +5219,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>42.000</v>
+        <v>112.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1281.96</v>
+        <v>1526.96</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5239,13 +5245,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>28.000</v>
+        <v>42.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>3185.96</v>
+        <v>1281.96</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5265,13 +5271,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>1.000</v>
+        <v>26.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>194.13</v>
+        <v>2958.39</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5291,13 +5297,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>159.15</v>
+        <v>194.13</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5323,7 +5329,7 @@
         <v>5</v>
       </c>
       <c r="H137" s="3">
-        <v>499.74</v>
+        <v>159.15</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5343,13 +5349,13 @@
         <v>277</v>
       </c>
       <c r="F138" s="2">
-        <v>43.000</v>
+        <v>2.000</v>
       </c>
       <c r="G138" t="s">
         <v>5</v>
       </c>
       <c r="H138" s="3">
-        <v>3120.30</v>
+        <v>499.74</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5369,13 +5375,13 @@
         <v>279</v>
       </c>
       <c r="F139" s="2">
-        <v>15.000</v>
+        <v>43.000</v>
       </c>
       <c r="G139" t="s">
         <v>5</v>
       </c>
       <c r="H139" s="3">
-        <v>2283.44</v>
+        <v>3120.30</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5395,13 +5401,13 @@
         <v>281</v>
       </c>
       <c r="F140" s="2">
-        <v>12.000</v>
+        <v>15.000</v>
       </c>
       <c r="G140" t="s">
         <v>5</v>
       </c>
       <c r="H140" s="3">
-        <v>5668.76</v>
+        <v>2283.44</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5421,13 +5427,13 @@
         <v>283</v>
       </c>
       <c r="F141" s="2">
-        <v>10.000</v>
+        <v>12.000</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
       </c>
       <c r="H141" s="3">
-        <v>6951.09</v>
+        <v>5668.76</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5447,13 +5453,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G142" t="s">
         <v>5</v>
       </c>
       <c r="H142" s="3">
-        <v>5624.37</v>
+        <v>6951.09</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5473,13 +5479,13 @@
         <v>287</v>
       </c>
       <c r="F143" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G143" t="s">
         <v>5</v>
       </c>
       <c r="H143" s="3">
-        <v>5800.85</v>
+        <v>5624.37</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5499,13 +5505,13 @@
         <v>289</v>
       </c>
       <c r="F144" s="2">
-        <v>3.000</v>
+        <v>5.000</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
       </c>
       <c r="H144" s="3">
-        <v>5120.09</v>
+        <v>5800.85</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5525,13 +5531,13 @@
         <v>291</v>
       </c>
       <c r="F145" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G145" t="s">
         <v>5</v>
       </c>
       <c r="H145" s="3">
-        <v>1690.54</v>
+        <v>5120.09</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5551,13 +5557,13 @@
         <v>293</v>
       </c>
       <c r="F146" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
       </c>
       <c r="H146" s="3">
-        <v>1094.94</v>
+        <v>1690.54</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5577,13 +5583,13 @@
         <v>295</v>
       </c>
       <c r="F147" s="2">
-        <v>18.000</v>
+        <v>4.000</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
       </c>
       <c r="H147" s="3">
-        <v>5329.84</v>
+        <v>1094.94</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5603,13 +5609,13 @@
         <v>297</v>
       </c>
       <c r="F148" s="2">
-        <v>3.000</v>
+        <v>18.000</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
       </c>
       <c r="H148" s="3">
-        <v>162.71</v>
+        <v>5329.84</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5629,13 +5635,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>4.000</v>
+        <v>3.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>419.08</v>
+        <v>162.71</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5655,13 +5661,13 @@
         <v>301</v>
       </c>
       <c r="F150" s="2">
-        <v>30.000</v>
+        <v>4.000</v>
       </c>
       <c r="G150" t="s">
         <v>5</v>
       </c>
       <c r="H150" s="3">
-        <v>179.61</v>
+        <v>419.08</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5681,13 +5687,13 @@
         <v>303</v>
       </c>
       <c r="F151" s="2">
-        <v>6.000</v>
+        <v>30.000</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
       </c>
       <c r="H151" s="3">
-        <v>98.34</v>
+        <v>179.61</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5707,13 +5713,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>10.000</v>
+        <v>6.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>374.16</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5733,13 +5739,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>527.000</v>
+        <v>10.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>2332.70</v>
+        <v>374.16</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5759,13 +5765,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>16.000</v>
+        <v>527.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>1204.47</v>
+        <v>2332.70</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5785,13 +5791,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>2.000</v>
+        <v>16.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>270.71</v>
+        <v>1204.47</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5811,13 +5817,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>25.000</v>
+        <v>2.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>116.25</v>
+        <v>270.71</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5837,13 +5843,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>10.000</v>
+        <v>25.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>1194.56</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5863,13 +5869,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>35.000</v>
+        <v>10.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>3575.81</v>
+        <v>1194.56</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5889,13 +5895,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>52.000</v>
+        <v>35.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>6942.47</v>
+        <v>3575.81</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5915,13 +5921,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>1.000</v>
+        <v>52.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>40.71</v>
+        <v>6942.47</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5938,16 +5944,16 @@
         <v>322</v>
       </c>
       <c r="E161" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F161" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>317.81</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5961,19 +5967,19 @@
         <v>2</v>
       </c>
       <c r="D162" t="s">
+        <v>324</v>
+      </c>
+      <c r="E162" t="s">
         <v>323</v>
       </c>
-      <c r="E162" t="s">
-        <v>324</v>
-      </c>
       <c r="F162" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>483.20</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5999,7 +6005,7 @@
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>45.92</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6019,13 +6025,13 @@
         <v>328</v>
       </c>
       <c r="F164" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G164" t="s">
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>303.12</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6051,7 +6057,7 @@
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>266.42</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6071,13 +6077,13 @@
         <v>332</v>
       </c>
       <c r="F166" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G166" t="s">
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>1141.60</v>
+        <v>266.42</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6097,13 +6103,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>3.000</v>
+        <v>8.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>1028.70</v>
+        <v>1141.60</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6123,13 +6129,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>9.000</v>
+        <v>3.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>543.81</v>
+        <v>1028.70</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6149,13 +6155,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>2.000</v>
+        <v>9.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>412.45</v>
+        <v>543.81</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6175,13 +6181,13 @@
         <v>340</v>
       </c>
       <c r="F170" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>24.27</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6201,13 +6207,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>214.33</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6227,13 +6233,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>15.000</v>
+        <v>9.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>3032.79</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6253,13 +6259,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>1950.000</v>
+        <v>15.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>36513.75</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6279,13 +6285,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>37.000</v>
+        <v>2249.000</v>
       </c>
       <c r="G174" t="s">
-        <v>349</v>
+        <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>55.41</v>
+        <v>42112.53</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6299,19 +6305,19 @@
         <v>2</v>
       </c>
       <c r="D175" t="s">
+        <v>349</v>
+      </c>
+      <c r="E175" t="s">
         <v>350</v>
       </c>
-      <c r="E175" t="s">
+      <c r="F175" s="2">
+        <v>12.000</v>
+      </c>
+      <c r="G175" t="s">
         <v>351</v>
       </c>
-      <c r="F175" s="2">
-        <v>103.000</v>
-      </c>
-      <c r="G175" t="s">
-        <v>5</v>
-      </c>
       <c r="H175" s="3">
-        <v>3671.30</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6331,13 +6337,13 @@
         <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>12.000</v>
+        <v>103.000</v>
       </c>
       <c r="G176" t="s">
         <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>2296.07</v>
+        <v>3671.30</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6357,13 +6363,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>651.000</v>
+        <v>36.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>113675.74</v>
+        <v>6888.20</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6383,13 +6389,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>7.000</v>
+        <v>663.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>1219.43</v>
+        <v>115771.14</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6409,13 +6415,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>11.000</v>
+        <v>13.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>145.79</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6435,13 +6441,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>22.000</v>
+        <v>11.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>10363.87</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6461,13 +6467,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>58.000</v>
+        <v>22.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>26897.75</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6487,13 +6493,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>26.000</v>
+        <v>92.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>1587.82</v>
+        <v>42665.40</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6513,13 +6519,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>87.000</v>
+        <v>22.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>12699.18</v>
+        <v>1343.54</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6539,13 +6545,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>1.000</v>
+        <v>87.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>1218.18</v>
+        <v>12699.17</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6571,7 +6577,7 @@
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>1720.00</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6591,13 +6597,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>184.000</v>
+        <v>1.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>6147.25</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6617,13 +6623,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>28.000</v>
+        <v>184.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>1119.31</v>
+        <v>6147.25</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6643,13 +6649,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>459.000</v>
+        <v>28.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>7175.20</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6669,13 +6675,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>59.000</v>
+        <v>459.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>1003.06</v>
+        <v>7175.20</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6695,13 +6701,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>491.000</v>
+        <v>59.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>9947.66</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6721,13 +6727,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>44.000</v>
+        <v>491.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>1021.95</v>
+        <v>9947.66</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6747,13 +6753,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>96.000</v>
+        <v>44.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>6840.48</v>
+        <v>1021.95</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6773,13 +6779,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>16.000</v>
+        <v>96.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>1789.69</v>
+        <v>6840.48</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6799,13 +6805,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>1.000</v>
+        <v>16.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>189.22</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6825,13 +6831,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>19.000</v>
+        <v>1.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>1201.67</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6851,13 +6857,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>272.000</v>
+        <v>19.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>18834.64</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6877,13 +6883,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>2.000</v>
+        <v>272.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>651.09</v>
+        <v>18834.64</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6903,13 +6909,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>562.67</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6935,7 +6941,7 @@
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>1125.55</v>
+        <v>562.67</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6955,13 +6961,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>718.30</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6981,13 +6987,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>266.26</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7013,7 +7019,7 @@
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>257.36</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7033,13 +7039,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>961.64</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7059,13 +7065,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>726.22</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7085,13 +7091,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>662.53</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7111,13 +7117,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>2.000</v>
+        <v>5.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>493.11</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7137,13 +7143,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>7.000</v>
+        <v>2.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>885.89</v>
+        <v>493.11</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7163,13 +7169,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>40.000</v>
+        <v>7.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>5509.90</v>
+        <v>885.89</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7189,13 +7195,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>1.000</v>
+        <v>40.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>4700.00</v>
+        <v>5509.90</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7221,7 +7227,7 @@
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>8560.17</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7241,13 +7247,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>40.000</v>
+        <v>1.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>506.58</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7267,13 +7273,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>1.000</v>
+        <v>40.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>23.34</v>
+        <v>506.58</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7293,13 +7299,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>11.000</v>
+        <v>1.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>418.00</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7319,13 +7325,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>24.000</v>
+        <v>11.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>1584.75</v>
+        <v>418.00</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7345,13 +7351,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>1.000</v>
+        <v>24.000</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
       </c>
       <c r="H215" s="3">
-        <v>29.64</v>
+        <v>1584.75</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7377,7 +7383,7 @@
         <v>5</v>
       </c>
       <c r="H216" s="3">
-        <v>685.11</v>
+        <v>29.64</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7397,13 +7403,13 @@
         <v>435</v>
       </c>
       <c r="F217" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G217" t="s">
         <v>5</v>
       </c>
       <c r="H217" s="3">
-        <v>8149.76</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7423,13 +7429,13 @@
         <v>437</v>
       </c>
       <c r="F218" s="2">
-        <v>4.800</v>
+        <v>2.000</v>
       </c>
       <c r="G218" t="s">
-        <v>438</v>
+        <v>5</v>
       </c>
       <c r="H218" s="3">
-        <v>1822.34</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7443,19 +7449,19 @@
         <v>2</v>
       </c>
       <c r="D219" t="s">
+        <v>438</v>
+      </c>
+      <c r="E219" t="s">
         <v>439</v>
       </c>
-      <c r="E219" t="s">
+      <c r="F219" s="2">
+        <v>4.800</v>
+      </c>
+      <c r="G219" t="s">
         <v>440</v>
       </c>
-      <c r="F219" s="2">
-        <v>16.000</v>
-      </c>
-      <c r="G219" t="s">
-        <v>438</v>
-      </c>
       <c r="H219" s="3">
-        <v>7011.29</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7475,13 +7481,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>17.000</v>
+        <v>16.000</v>
       </c>
       <c r="G220" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H220" s="3">
-        <v>2938.94</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7501,13 +7507,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>184.000</v>
+        <v>17.000</v>
       </c>
       <c r="G221" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H221" s="3">
-        <v>39969.93</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7527,13 +7533,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>1.090</v>
+        <v>184.000</v>
       </c>
       <c r="G222" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H222" s="3">
-        <v>250.66</v>
+        <v>39969.93</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7553,13 +7559,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>20.300</v>
+        <v>1.090</v>
       </c>
       <c r="G223" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H223" s="3">
-        <v>6816.84</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7579,13 +7585,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>13.000</v>
+        <v>20.300</v>
       </c>
       <c r="G224" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H224" s="3">
-        <v>3437.72</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7605,13 +7611,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>22.000</v>
+        <v>13.000</v>
       </c>
       <c r="G225" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H225" s="3">
-        <v>2084.93</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7631,13 +7637,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>345.400</v>
+        <v>22.000</v>
       </c>
       <c r="G226" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H226" s="3">
-        <v>3460.95</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7657,13 +7663,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>78.000</v>
+        <v>345.400</v>
       </c>
       <c r="G227" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H227" s="3">
-        <v>1687.76</v>
+        <v>3460.95</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7683,13 +7689,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>11.000</v>
+        <v>78.000</v>
       </c>
       <c r="G228" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H228" s="3">
-        <v>974.64</v>
+        <v>1687.76</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7709,13 +7715,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>84.000</v>
+        <v>11.000</v>
       </c>
       <c r="G229" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H229" s="3">
-        <v>13440.76</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7735,13 +7741,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>168.620</v>
+        <v>84.000</v>
       </c>
       <c r="G230" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H230" s="3">
-        <v>8798.84</v>
+        <v>13440.76</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7761,13 +7767,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>47.250</v>
+        <v>168.620</v>
       </c>
       <c r="G231" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H231" s="3">
-        <v>5148.59</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7787,13 +7793,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>21178.300</v>
+        <v>47.250</v>
       </c>
       <c r="G232" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H232" s="3">
-        <v>48068.14</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7813,13 +7819,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>2853.960</v>
+        <v>22158.300</v>
       </c>
       <c r="G233" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H233" s="3">
-        <v>12183.76</v>
+        <v>50292.42</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7839,13 +7845,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>29.390</v>
+        <v>2853.960</v>
       </c>
       <c r="G234" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H234" s="3">
-        <v>15217.18</v>
+        <v>12183.76</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7865,13 +7871,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>1198.180</v>
+        <v>29.390</v>
       </c>
       <c r="G235" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H235" s="3">
-        <v>45050.39</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7891,13 +7897,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>0.610</v>
+        <v>1198.180</v>
       </c>
       <c r="G236" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H236" s="3">
-        <v>6.23</v>
+        <v>45050.39</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7917,13 +7923,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>35.000</v>
+        <v>0.610</v>
       </c>
       <c r="G237" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H237" s="3">
-        <v>783.60</v>
+        <v>6.23</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7943,13 +7949,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>1061.580</v>
+        <v>34.000</v>
       </c>
       <c r="G238" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H238" s="3">
-        <v>33351.08</v>
+        <v>761.21</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7969,13 +7975,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>290.430</v>
+        <v>1561.960</v>
       </c>
       <c r="G239" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H239" s="3">
-        <v>26647.45</v>
+        <v>49071.25</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7995,13 +8001,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>59.100</v>
+        <v>270.420</v>
       </c>
       <c r="G240" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H240" s="3">
-        <v>9271.17</v>
+        <v>24811.50</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8021,13 +8027,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>241.900</v>
+        <v>59.100</v>
       </c>
       <c r="G241" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H241" s="3">
-        <v>7817.79</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8047,13 +8053,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>91.020</v>
+        <v>241.900</v>
       </c>
       <c r="G242" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H242" s="3">
-        <v>1685.63</v>
+        <v>7817.79</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8073,13 +8079,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>0.690</v>
+        <v>91.020</v>
       </c>
       <c r="G243" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H243" s="3">
-        <v>20.12</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8099,13 +8105,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>52.790</v>
+        <v>0.690</v>
       </c>
       <c r="G244" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H244" s="3">
-        <v>1134.03</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8125,13 +8131,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>78.310</v>
+        <v>52.790</v>
       </c>
       <c r="G245" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="H245" s="3">
-        <v>7083.14</v>
+        <v>1134.03</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8151,13 +8157,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>228.000</v>
+        <v>78.310</v>
       </c>
       <c r="G246" t="s">
-        <v>5</v>
+        <v>440</v>
       </c>
       <c r="H246" s="3">
-        <v>1334.94</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8177,13 +8183,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>75.000</v>
+        <v>228.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>413.17</v>
+        <v>1334.94</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8203,13 +8209,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>4576.000</v>
+        <v>75.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>11487.35</v>
+        <v>413.17</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8229,13 +8235,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>9.000</v>
+        <v>4573.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>3203.83</v>
+        <v>11479.82</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8255,13 +8261,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>556.74</v>
+        <v>3203.83</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8281,13 +8287,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>11.000</v>
+        <v>1.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>4741.17</v>
+        <v>556.74</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8307,13 +8313,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>6.000</v>
+        <v>11.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>2371.80</v>
+        <v>4741.17</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8333,13 +8339,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>2323.99</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8359,13 +8365,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>1462.82</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8391,7 +8397,7 @@
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>6585.02</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8411,13 +8417,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>1694.29</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8437,13 +8443,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>38.000</v>
+        <v>6.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>17563.39</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8463,13 +8469,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>14.000</v>
+        <v>38.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>7926.12</v>
+        <v>17563.39</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8489,13 +8495,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>2.000</v>
+        <v>14.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>3443.46</v>
+        <v>7926.12</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8515,13 +8521,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>6821.40</v>
+        <v>3443.46</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8541,13 +8547,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>7220.40</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8567,13 +8573,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>7.000</v>
+        <v>2.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>2566.22</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8593,13 +8599,13 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>17.000</v>
+        <v>7.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>7823.48</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -8619,13 +8625,13 @@
         <v>530</v>
       </c>
       <c r="F264" s="2">
-        <v>7.000</v>
+        <v>17.000</v>
       </c>
       <c r="G264" t="s">
         <v>5</v>
       </c>
       <c r="H264" s="3">
-        <v>3943.24</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="265" spans="1:8">
@@ -8645,13 +8651,13 @@
         <v>532</v>
       </c>
       <c r="F265" s="2">
-        <v>5.000</v>
+        <v>7.000</v>
       </c>
       <c r="G265" t="s">
         <v>5</v>
       </c>
       <c r="H265" s="3">
-        <v>2725.89</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="266" spans="1:8">
@@ -8671,12 +8677,38 @@
         <v>534</v>
       </c>
       <c r="F266" s="2">
+        <v>5.000</v>
+      </c>
+      <c r="G266" t="s">
+        <v>5</v>
+      </c>
+      <c r="H266" s="3">
+        <v>2725.89</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8">
+      <c r="A267" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" t="s">
+        <v>1</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
+        <v>535</v>
+      </c>
+      <c r="E267" t="s">
+        <v>536</v>
+      </c>
+      <c r="F267" s="2">
         <v>3.000</v>
       </c>
-      <c r="G266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H266" s="3">
+      <c r="G267" t="s">
+        <v>5</v>
+      </c>
+      <c r="H267" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: ambigous boolean reposicao_geral variable
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="543">
   <si>
     <t>4600041302</t>
   </si>
@@ -67,6 +67,12 @@
     <t>ABRACADEIRA FF REPARO TUBO DN50 LMIN=150</t>
   </si>
   <si>
+    <t>30001122</t>
+  </si>
+  <si>
+    <t>ABRACADEIRA FF REPARO TUBO DN75 LMIN=150</t>
+  </si>
+  <si>
     <t>30000153</t>
   </si>
   <si>
@@ -1309,12 +1315,6 @@
     <t>TE PVC BBB JE ESG DN 200 X 200 JEI/ JERI</t>
   </si>
   <si>
-    <t>30008708</t>
-  </si>
-  <si>
-    <t>TE PVC JE DN 100X75 - FORA ESPECIFICAÇÃO</t>
-  </si>
-  <si>
     <t>30010469</t>
   </si>
   <si>
@@ -1520,12 +1520,6 @@
   </si>
   <si>
     <t>VALV GAV CM REV ELAST BB JE CAB FF DN 50</t>
-  </si>
-  <si>
-    <t>30007804</t>
-  </si>
-  <si>
-    <t>VALV GAV CM REV ELAST BB JE CAB FF DN 75</t>
   </si>
   <si>
     <t>30003852</t>
@@ -1752,7 +1746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H267"/>
+  <dimension ref="A1:H266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1772,28 +1766,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>543</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1813,13 +1807,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>84.000</v>
+        <v>81.000</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3">
-        <v>23184.37</v>
+        <v>22356.37</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1845,7 +1839,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>17904.37</v>
+        <v>17904.38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1891,13 +1885,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="3">
-        <v>6425.84</v>
+        <v>5140.67</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1995,13 +1989,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>8.000</v>
+        <v>10.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>1582.95</v>
+        <v>4275.79</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2021,13 +2015,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="2">
-        <v>3.000</v>
+        <v>8.000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
-        <v>750.47</v>
+        <v>1582.95</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2047,13 +2041,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>153.40</v>
+        <v>750.47</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2073,13 +2067,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>15.000</v>
+        <v>1.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>313.91</v>
+        <v>153.40</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2099,13 +2093,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2">
-        <v>9.000</v>
+        <v>15.000</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>878.23</v>
+        <v>313.91</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2125,13 +2119,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>19.000</v>
+        <v>9.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>723.49</v>
+        <v>878.23</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2151,13 +2145,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="2">
-        <v>142.000</v>
+        <v>19.000</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>13440.91</v>
+        <v>723.49</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2177,13 +2171,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>18.000</v>
+        <v>137.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>78.03</v>
+        <v>12967.64</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2203,13 +2197,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>623.000</v>
+        <v>18.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>1277.15</v>
+        <v>78.03</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2229,13 +2223,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>447.000</v>
+        <v>623.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>326.45</v>
+        <v>1277.15</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2255,13 +2249,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="2">
-        <v>98.000</v>
+        <v>447.000</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>125.14</v>
+        <v>326.45</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2281,13 +2275,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>136.000</v>
+        <v>98.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>607.32</v>
+        <v>125.14</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2307,13 +2301,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>60.000</v>
+        <v>136.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>227.27</v>
+        <v>607.32</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2333,13 +2327,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>4.000</v>
+        <v>60.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>48.64</v>
+        <v>227.27</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2359,13 +2353,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>11.000</v>
+        <v>4.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>6222.91</v>
+        <v>48.64</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2385,13 +2379,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>334.000</v>
+        <v>11.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>28520.40</v>
+        <v>6222.91</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2411,13 +2405,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>113.000</v>
+        <v>334.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>20496.57</v>
+        <v>28520.40</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2437,13 +2431,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>9.000</v>
+        <v>113.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>380.14</v>
+        <v>20496.57</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2463,13 +2457,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>59.98</v>
+        <v>380.14</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2489,13 +2483,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>103.20</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2515,13 +2509,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>197.65</v>
+        <v>103.20</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2541,13 +2535,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>618.66</v>
+        <v>197.65</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2567,13 +2561,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>542.21</v>
+        <v>618.66</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2593,13 +2587,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>10.000</v>
+        <v>2.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>201.79</v>
+        <v>542.21</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2619,13 +2613,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>339.93</v>
+        <v>201.79</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2645,13 +2639,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>14.000</v>
+        <v>6.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>566.79</v>
+        <v>339.93</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2671,13 +2665,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>15.000</v>
+        <v>13.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>675.15</v>
+        <v>526.30</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2697,13 +2691,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>17.000</v>
+        <v>15.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>553.16</v>
+        <v>675.15</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2723,13 +2717,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>22.000</v>
+        <v>17.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>1229.98</v>
+        <v>553.16</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2749,13 +2743,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>1.000</v>
+        <v>15.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>17.78</v>
+        <v>838.61</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2775,13 +2769,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>190.000</v>
+        <v>1.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>8925.11</v>
+        <v>17.78</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2801,13 +2795,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>2.000</v>
+        <v>185.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>4960.91</v>
+        <v>8690.25</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2827,13 +2821,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>1940.18</v>
+        <v>4960.91</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2859,7 +2853,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>2226.13</v>
+        <v>1940.18</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2879,13 +2873,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>253.000</v>
+        <v>1.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>7578.61</v>
+        <v>2226.13</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2905,13 +2899,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>275.000</v>
+        <v>241.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>43599.45</v>
+        <v>7219.15</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2931,13 +2925,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>281.000</v>
+        <v>200.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>157016.05</v>
+        <v>31708.86</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2957,13 +2951,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>3.000</v>
+        <v>209.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>308.38</v>
+        <v>116784.06</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2983,13 +2977,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>46.000</v>
+        <v>3.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>2898.44</v>
+        <v>308.38</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3009,13 +3003,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>2.000</v>
+        <v>46.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>603.23</v>
+        <v>2898.44</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3035,13 +3029,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>16.000</v>
+        <v>2.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>2244.02</v>
+        <v>603.23</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3061,13 +3055,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>10.000</v>
+        <v>16.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>2092.96</v>
+        <v>2244.02</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3087,13 +3081,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>8.000</v>
+        <v>10.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>2352.96</v>
+        <v>2092.96</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3113,13 +3107,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>9.000</v>
+        <v>8.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>3592.71</v>
+        <v>2352.96</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3139,13 +3133,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>863.17</v>
+        <v>3592.71</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3165,13 +3159,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>295.57</v>
+        <v>863.17</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3191,13 +3185,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>1279.000</v>
+        <v>3.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>11654.21</v>
+        <v>295.57</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3217,13 +3211,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>40.000</v>
+        <v>1070.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>641.18</v>
+        <v>9749.97</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3243,13 +3237,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3031.000</v>
+        <v>40.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>31228.01</v>
+        <v>641.18</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3269,13 +3263,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>11.000</v>
+        <v>2937.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>380.69</v>
+        <v>30259.77</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3295,13 +3289,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>9.000</v>
+        <v>11.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>334.55</v>
+        <v>380.69</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3321,13 +3315,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>5.000</v>
+        <v>9.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>1390.00</v>
+        <v>334.55</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3347,13 +3341,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>25.000</v>
+        <v>5.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>1165.08</v>
+        <v>1390.00</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3373,13 +3367,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>11.000</v>
+        <v>24.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>1357.53</v>
+        <v>1118.48</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3399,13 +3393,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>16.000</v>
+        <v>11.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>902.16</v>
+        <v>1357.53</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3425,13 +3419,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>29.000</v>
+        <v>16.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>2288.17</v>
+        <v>902.16</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3451,13 +3445,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>8.000</v>
+        <v>28.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>237.96</v>
+        <v>2209.27</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3477,13 +3471,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>37.000</v>
+        <v>8.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>2108.34</v>
+        <v>237.96</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3503,13 +3497,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>4.000</v>
+        <v>37.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>606.42</v>
+        <v>2108.34</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3529,13 +3523,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>1448.47</v>
+        <v>606.42</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3555,13 +3549,13 @@
         <v>139</v>
       </c>
       <c r="F69" s="2">
-        <v>638.000</v>
+        <v>1.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>3316.48</v>
+        <v>1448.47</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3581,13 +3575,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>23.000</v>
+        <v>823.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>1359.47</v>
+        <v>4278.14</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3607,13 +3601,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>42.000</v>
+        <v>23.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>5269.67</v>
+        <v>1359.47</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3633,13 +3627,13 @@
         <v>145</v>
       </c>
       <c r="F72" s="2">
-        <v>180.000</v>
+        <v>40.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>1598.49</v>
+        <v>5018.74</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3659,13 +3653,13 @@
         <v>147</v>
       </c>
       <c r="F73" s="2">
-        <v>15.000</v>
+        <v>180.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>851.70</v>
+        <v>1598.49</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3685,13 +3679,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>7.000</v>
+        <v>15.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>401.34</v>
+        <v>851.70</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3711,13 +3705,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>837.86</v>
+        <v>344.01</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3737,13 +3731,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>47.000</v>
+        <v>5.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>4841.34</v>
+        <v>837.86</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3763,13 +3757,13 @@
         <v>155</v>
       </c>
       <c r="F77" s="2">
-        <v>2.000</v>
+        <v>47.000</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>495.95</v>
+        <v>4841.34</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3789,13 +3783,13 @@
         <v>157</v>
       </c>
       <c r="F78" s="2">
-        <v>101.000</v>
+        <v>2.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>1876.55</v>
+        <v>495.95</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3815,13 +3809,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>1.000</v>
+        <v>93.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>131.57</v>
+        <v>1727.91</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3847,7 +3841,7 @@
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>72.70</v>
+        <v>131.57</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3867,13 +3861,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>1531.000</v>
+        <v>1.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>9497.17</v>
+        <v>72.70</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3893,13 +3887,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>2849.000</v>
+        <v>1490.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>74208.08</v>
+        <v>9243.03</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3919,13 +3913,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>5.000</v>
+        <v>2730.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>383.07</v>
+        <v>71108.99</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3945,13 +3939,13 @@
         <v>169</v>
       </c>
       <c r="F84" s="2">
-        <v>3.000</v>
+        <v>5.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>651.71</v>
+        <v>383.07</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3977,7 +3971,7 @@
         <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>1263.43</v>
+        <v>651.71</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3997,13 +3991,13 @@
         <v>173</v>
       </c>
       <c r="F86" s="2">
-        <v>15.000</v>
+        <v>3.000</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>2783.05</v>
+        <v>1263.43</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4023,13 +4017,13 @@
         <v>175</v>
       </c>
       <c r="F87" s="2">
-        <v>4.000</v>
+        <v>15.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>1008.05</v>
+        <v>2783.05</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4049,13 +4043,13 @@
         <v>177</v>
       </c>
       <c r="F88" s="2">
-        <v>14.000</v>
+        <v>4.000</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>1572.64</v>
+        <v>1008.05</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4075,13 +4069,13 @@
         <v>179</v>
       </c>
       <c r="F89" s="2">
-        <v>12.000</v>
+        <v>14.000</v>
       </c>
       <c r="G89" t="s">
         <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>5523.49</v>
+        <v>1572.64</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4101,13 +4095,13 @@
         <v>181</v>
       </c>
       <c r="F90" s="2">
-        <v>2.000</v>
+        <v>12.000</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>3671.99</v>
+        <v>5523.49</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4127,13 +4121,13 @@
         <v>183</v>
       </c>
       <c r="F91" s="2">
-        <v>149.000</v>
+        <v>2.000</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>5616.55</v>
+        <v>3671.99</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -4153,13 +4147,13 @@
         <v>185</v>
       </c>
       <c r="F92" s="2">
-        <v>2.000</v>
+        <v>140.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>560.27</v>
+        <v>5277.30</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -4179,13 +4173,13 @@
         <v>187</v>
       </c>
       <c r="F93" s="2">
-        <v>38.000</v>
+        <v>2.000</v>
       </c>
       <c r="G93" t="s">
         <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>3477.47</v>
+        <v>560.27</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -4205,13 +4199,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>1.000</v>
+        <v>38.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>2.97</v>
+        <v>3477.47</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4231,13 +4225,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>11.000</v>
+        <v>1.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>19946.36</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4257,13 +4251,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>2622.000</v>
+        <v>11.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>361167.39</v>
+        <v>19946.36</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4283,13 +4277,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>1.000</v>
+        <v>2370.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>2980.59</v>
+        <v>326455.65</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4315,7 +4309,7 @@
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>4463.84</v>
+        <v>2980.59</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4335,13 +4329,13 @@
         <v>199</v>
       </c>
       <c r="F99" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>1598.31</v>
+        <v>4463.84</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4361,13 +4355,13 @@
         <v>201</v>
       </c>
       <c r="F100" s="2">
-        <v>20.000</v>
+        <v>3.000</v>
       </c>
       <c r="G100" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>24666.05</v>
+        <v>1598.31</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4387,13 +4381,13 @@
         <v>203</v>
       </c>
       <c r="F101" s="2">
-        <v>6.000</v>
+        <v>20.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>10134.33</v>
+        <v>24666.05</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4413,13 +4407,13 @@
         <v>205</v>
       </c>
       <c r="F102" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>375.86</v>
+        <v>10134.33</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4445,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>279.59</v>
+        <v>375.86</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4465,13 +4459,13 @@
         <v>209</v>
       </c>
       <c r="F104" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>740.97</v>
+        <v>279.59</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4497,7 +4491,7 @@
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>902.80</v>
+        <v>740.97</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -4523,7 +4517,7 @@
         <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>994.54</v>
+        <v>902.80</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -4549,7 +4543,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>1033.65</v>
+        <v>994.54</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4575,7 +4569,7 @@
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>1166.57</v>
+        <v>1033.65</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4595,13 +4589,13 @@
         <v>219</v>
       </c>
       <c r="F109" s="2">
-        <v>8.000</v>
+        <v>2.000</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>2825.06</v>
+        <v>1166.57</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4621,13 +4615,13 @@
         <v>221</v>
       </c>
       <c r="F110" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G110" t="s">
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>91.20</v>
+        <v>2825.06</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4647,13 +4641,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>719.47</v>
+        <v>91.20</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4673,13 +4667,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>545.000</v>
+        <v>2.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>20225.32</v>
+        <v>719.47</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4699,13 +4693,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>352.000</v>
+        <v>534.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>23009.79</v>
+        <v>19817.18</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4725,13 +4719,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>993.000</v>
+        <v>352.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>32716.37</v>
+        <v>23009.79</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4751,13 +4745,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>176.000</v>
+        <v>955.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>9043.46</v>
+        <v>31464.35</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4777,13 +4771,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>45.000</v>
+        <v>174.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>4586.29</v>
+        <v>8940.70</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4803,13 +4797,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>45.000</v>
+        <v>39.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>1519.40</v>
+        <v>3974.78</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4829,13 +4823,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>9.000</v>
+        <v>45.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>1675.75</v>
+        <v>1519.40</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4855,13 +4849,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>7400.000</v>
+        <v>9.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>28609.80</v>
+        <v>1675.75</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4881,13 +4875,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>2.000</v>
+        <v>6608.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>2463.85</v>
+        <v>25546.41</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4913,7 +4907,7 @@
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>4533.88</v>
+        <v>2463.85</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4933,13 +4927,13 @@
         <v>245</v>
       </c>
       <c r="F122" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>6385.34</v>
+        <v>4533.88</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4959,13 +4953,13 @@
         <v>247</v>
       </c>
       <c r="F123" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G123" t="s">
         <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>12368.67</v>
+        <v>6385.34</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4985,13 +4979,13 @@
         <v>249</v>
       </c>
       <c r="F124" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>3260.53</v>
+        <v>12368.67</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -5011,13 +5005,13 @@
         <v>251</v>
       </c>
       <c r="F125" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G125" t="s">
         <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>3527.49</v>
+        <v>3260.53</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5037,13 +5031,13 @@
         <v>253</v>
       </c>
       <c r="F126" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G126" t="s">
         <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>6294.26</v>
+        <v>3527.49</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5063,13 +5057,13 @@
         <v>255</v>
       </c>
       <c r="F127" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G127" t="s">
         <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>4585.00</v>
+        <v>6294.26</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -5089,13 +5083,13 @@
         <v>257</v>
       </c>
       <c r="F128" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>14225.45</v>
+        <v>4585.00</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5115,13 +5109,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>69.000</v>
+        <v>2.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>99523.18</v>
+        <v>14225.45</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5141,13 +5135,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>562.000</v>
+        <v>52.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>3181.36</v>
+        <v>75002.98</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5167,13 +5161,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>261.000</v>
+        <v>562.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>2053.88</v>
+        <v>3181.37</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5193,13 +5187,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>92.000</v>
+        <v>257.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>1442.37</v>
+        <v>2022.40</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5219,13 +5213,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>112.000</v>
+        <v>92.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1526.96</v>
+        <v>1442.37</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5245,13 +5239,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>42.000</v>
+        <v>110.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>1281.96</v>
+        <v>1499.69</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5271,13 +5265,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>26.000</v>
+        <v>42.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>2958.39</v>
+        <v>1281.96</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5297,13 +5291,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>1.000</v>
+        <v>26.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>194.13</v>
+        <v>2958.39</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5323,13 +5317,13 @@
         <v>275</v>
       </c>
       <c r="F137" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G137" t="s">
         <v>5</v>
       </c>
       <c r="H137" s="3">
-        <v>159.15</v>
+        <v>194.13</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5355,7 +5349,7 @@
         <v>5</v>
       </c>
       <c r="H138" s="3">
-        <v>499.74</v>
+        <v>159.15</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5375,13 +5369,13 @@
         <v>279</v>
       </c>
       <c r="F139" s="2">
-        <v>43.000</v>
+        <v>2.000</v>
       </c>
       <c r="G139" t="s">
         <v>5</v>
       </c>
       <c r="H139" s="3">
-        <v>3120.30</v>
+        <v>499.74</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5401,13 +5395,13 @@
         <v>281</v>
       </c>
       <c r="F140" s="2">
-        <v>15.000</v>
+        <v>41.000</v>
       </c>
       <c r="G140" t="s">
         <v>5</v>
       </c>
       <c r="H140" s="3">
-        <v>2283.44</v>
+        <v>2975.17</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5427,13 +5421,13 @@
         <v>283</v>
       </c>
       <c r="F141" s="2">
-        <v>12.000</v>
+        <v>15.000</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
       </c>
       <c r="H141" s="3">
-        <v>5668.76</v>
+        <v>2283.44</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5453,13 +5447,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="2">
-        <v>10.000</v>
+        <v>12.000</v>
       </c>
       <c r="G142" t="s">
         <v>5</v>
       </c>
       <c r="H142" s="3">
-        <v>6951.09</v>
+        <v>5668.76</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5479,13 +5473,13 @@
         <v>287</v>
       </c>
       <c r="F143" s="2">
-        <v>6.000</v>
+        <v>9.000</v>
       </c>
       <c r="G143" t="s">
         <v>5</v>
       </c>
       <c r="H143" s="3">
-        <v>5624.37</v>
+        <v>6255.98</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5505,13 +5499,13 @@
         <v>289</v>
       </c>
       <c r="F144" s="2">
-        <v>5.000</v>
+        <v>6.000</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
       </c>
       <c r="H144" s="3">
-        <v>5800.85</v>
+        <v>5624.37</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5531,13 +5525,13 @@
         <v>291</v>
       </c>
       <c r="F145" s="2">
-        <v>3.000</v>
+        <v>5.000</v>
       </c>
       <c r="G145" t="s">
         <v>5</v>
       </c>
       <c r="H145" s="3">
-        <v>5120.09</v>
+        <v>5800.85</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5557,13 +5551,13 @@
         <v>293</v>
       </c>
       <c r="F146" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
       </c>
       <c r="H146" s="3">
-        <v>1690.54</v>
+        <v>5120.09</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5583,13 +5577,13 @@
         <v>295</v>
       </c>
       <c r="F147" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
       </c>
       <c r="H147" s="3">
-        <v>1094.94</v>
+        <v>1690.54</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5609,13 +5603,13 @@
         <v>297</v>
       </c>
       <c r="F148" s="2">
-        <v>18.000</v>
+        <v>9.000</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
       </c>
       <c r="H148" s="3">
-        <v>5329.84</v>
+        <v>2463.61</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5635,13 +5629,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>3.000</v>
+        <v>16.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>162.71</v>
+        <v>4737.64</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5661,13 +5655,13 @@
         <v>301</v>
       </c>
       <c r="F150" s="2">
-        <v>4.000</v>
+        <v>3.000</v>
       </c>
       <c r="G150" t="s">
         <v>5</v>
       </c>
       <c r="H150" s="3">
-        <v>419.08</v>
+        <v>162.71</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5687,13 +5681,13 @@
         <v>303</v>
       </c>
       <c r="F151" s="2">
-        <v>30.000</v>
+        <v>4.000</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
       </c>
       <c r="H151" s="3">
-        <v>179.61</v>
+        <v>419.08</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5713,13 +5707,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>6.000</v>
+        <v>30.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>98.34</v>
+        <v>179.61</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5739,13 +5733,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>10.000</v>
+        <v>6.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>374.16</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5765,13 +5759,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>527.000</v>
+        <v>10.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>2332.70</v>
+        <v>374.16</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5791,13 +5785,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>16.000</v>
+        <v>505.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>1204.47</v>
+        <v>2235.31</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5817,13 +5811,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>2.000</v>
+        <v>16.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>270.71</v>
+        <v>1204.47</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5843,13 +5837,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>25.000</v>
+        <v>2.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>116.25</v>
+        <v>270.71</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5869,13 +5863,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>10.000</v>
+        <v>25.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>1194.56</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5895,13 +5889,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>35.000</v>
+        <v>10.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>3575.81</v>
+        <v>1194.56</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5921,13 +5915,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>52.000</v>
+        <v>34.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>6942.47</v>
+        <v>3473.64</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5947,13 +5941,13 @@
         <v>323</v>
       </c>
       <c r="F161" s="2">
-        <v>1.000</v>
+        <v>55.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>40.71</v>
+        <v>7342.99</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5970,16 +5964,16 @@
         <v>324</v>
       </c>
       <c r="E162" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F162" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>317.81</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5993,19 +5987,19 @@
         <v>2</v>
       </c>
       <c r="D163" t="s">
+        <v>326</v>
+      </c>
+      <c r="E163" t="s">
         <v>325</v>
       </c>
-      <c r="E163" t="s">
-        <v>326</v>
-      </c>
       <c r="F163" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G163" t="s">
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>483.20</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6031,7 +6025,7 @@
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>45.92</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6051,13 +6045,13 @@
         <v>330</v>
       </c>
       <c r="F165" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G165" t="s">
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>303.12</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6083,7 +6077,7 @@
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>266.42</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6103,13 +6097,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>1141.60</v>
+        <v>266.42</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6129,13 +6123,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>3.000</v>
+        <v>8.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>1028.70</v>
+        <v>1141.60</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6155,13 +6149,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>9.000</v>
+        <v>3.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>543.81</v>
+        <v>1028.70</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6181,13 +6175,13 @@
         <v>340</v>
       </c>
       <c r="F170" s="2">
-        <v>2.000</v>
+        <v>9.000</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>412.45</v>
+        <v>543.81</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6207,13 +6201,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>24.27</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6233,13 +6227,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>214.33</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6259,13 +6253,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>15.000</v>
+        <v>9.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>3032.79</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6285,13 +6279,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>2249.000</v>
+        <v>15.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>42112.53</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6311,13 +6305,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>12.000</v>
+        <v>2445.000</v>
       </c>
       <c r="G175" t="s">
-        <v>351</v>
+        <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>17.99</v>
+        <v>45782.62</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6331,19 +6325,19 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
+        <v>351</v>
+      </c>
+      <c r="E176" t="s">
         <v>352</v>
       </c>
-      <c r="E176" t="s">
+      <c r="F176" s="2">
+        <v>12.000</v>
+      </c>
+      <c r="G176" t="s">
         <v>353</v>
       </c>
-      <c r="F176" s="2">
-        <v>103.000</v>
-      </c>
-      <c r="G176" t="s">
-        <v>5</v>
-      </c>
       <c r="H176" s="3">
-        <v>3671.30</v>
+        <v>18.02</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6363,13 +6357,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>36.000</v>
+        <v>101.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>6888.20</v>
+        <v>3600.02</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6389,13 +6383,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>663.000</v>
+        <v>35.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>115771.14</v>
+        <v>6696.86</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6415,13 +6409,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>13.000</v>
+        <v>671.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>2264.65</v>
+        <v>117168.07</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6441,13 +6435,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>11.000</v>
+        <v>13.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>145.79</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6467,13 +6461,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>22.000</v>
+        <v>11.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>10363.87</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6493,13 +6487,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>92.000</v>
+        <v>22.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>42665.40</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6519,13 +6513,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>22.000</v>
+        <v>63.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>1343.54</v>
+        <v>29216.54</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6545,13 +6539,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>87.000</v>
+        <v>21.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>12699.17</v>
+        <v>1282.47</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6571,13 +6565,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>1.000</v>
+        <v>87.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>1218.18</v>
+        <v>12699.17</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6603,7 +6597,7 @@
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1720.00</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6623,13 +6617,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>184.000</v>
+        <v>1.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>6147.25</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6649,13 +6643,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>28.000</v>
+        <v>184.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>1119.31</v>
+        <v>6147.25</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6675,13 +6669,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>459.000</v>
+        <v>28.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>7175.20</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6701,13 +6695,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>59.000</v>
+        <v>458.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>1003.06</v>
+        <v>7159.59</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6727,13 +6721,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>491.000</v>
+        <v>59.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>9947.66</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6753,13 +6747,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>44.000</v>
+        <v>488.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>1021.95</v>
+        <v>9886.88</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6779,13 +6773,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>96.000</v>
+        <v>44.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>6840.48</v>
+        <v>1021.95</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6805,13 +6799,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>16.000</v>
+        <v>96.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>1789.69</v>
+        <v>6840.48</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6831,13 +6825,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>1.000</v>
+        <v>16.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>189.22</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6857,13 +6851,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>19.000</v>
+        <v>1.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>1201.67</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6883,13 +6877,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>272.000</v>
+        <v>19.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>18834.64</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6909,13 +6903,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>2.000</v>
+        <v>261.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>651.09</v>
+        <v>18072.94</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6935,13 +6929,13 @@
         <v>399</v>
       </c>
       <c r="F199" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>562.67</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6967,7 +6961,7 @@
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>1125.55</v>
+        <v>562.67</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6987,13 +6981,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>718.30</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7013,13 +7007,13 @@
         <v>405</v>
       </c>
       <c r="F202" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G202" t="s">
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>266.26</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7045,7 +7039,7 @@
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>257.36</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7065,13 +7059,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>961.64</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7091,13 +7085,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>726.22</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7117,13 +7111,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>662.53</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7143,13 +7137,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>2.000</v>
+        <v>5.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>493.11</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7169,13 +7163,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>7.000</v>
+        <v>2.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>885.89</v>
+        <v>493.11</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7195,13 +7189,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>40.000</v>
+        <v>7.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>5509.90</v>
+        <v>885.89</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7221,13 +7215,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>1.000</v>
+        <v>38.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>4700.00</v>
+        <v>5234.40</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7253,7 +7247,7 @@
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>8560.17</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7273,13 +7267,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>40.000</v>
+        <v>1.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>506.58</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7299,13 +7293,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>1.000</v>
+        <v>40.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>23.34</v>
+        <v>506.58</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7325,13 +7319,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>11.000</v>
+        <v>1.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>418.00</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7351,13 +7345,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>24.000</v>
+        <v>11.000</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
       </c>
       <c r="H215" s="3">
-        <v>1584.75</v>
+        <v>418.00</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7377,13 +7371,13 @@
         <v>433</v>
       </c>
       <c r="F216" s="2">
-        <v>1.000</v>
+        <v>24.000</v>
       </c>
       <c r="G216" t="s">
         <v>5</v>
       </c>
       <c r="H216" s="3">
-        <v>29.64</v>
+        <v>1584.75</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7533,13 +7527,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>184.000</v>
+        <v>163.140</v>
       </c>
       <c r="G222" t="s">
         <v>440</v>
       </c>
       <c r="H222" s="3">
-        <v>39969.93</v>
+        <v>35438.55</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7689,13 +7683,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>78.000</v>
+        <v>1.860</v>
       </c>
       <c r="G228" t="s">
         <v>440</v>
       </c>
       <c r="H228" s="3">
-        <v>1687.76</v>
+        <v>40.25</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7819,13 +7813,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>22158.300</v>
+        <v>21657.800</v>
       </c>
       <c r="G233" t="s">
         <v>440</v>
       </c>
       <c r="H233" s="3">
-        <v>50292.42</v>
+        <v>49156.33</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7845,13 +7839,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>2853.960</v>
+        <v>2786.970</v>
       </c>
       <c r="G234" t="s">
         <v>440</v>
       </c>
       <c r="H234" s="3">
-        <v>12183.76</v>
+        <v>11897.77</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7897,13 +7891,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>1198.180</v>
+        <v>857.370</v>
       </c>
       <c r="G236" t="s">
         <v>440</v>
       </c>
       <c r="H236" s="3">
-        <v>45050.39</v>
+        <v>32236.27</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7923,13 +7917,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>0.610</v>
+        <v>615.610</v>
       </c>
       <c r="G237" t="s">
         <v>440</v>
       </c>
       <c r="H237" s="3">
-        <v>6.23</v>
+        <v>6281.47</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7949,13 +7943,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>34.000</v>
+        <v>25.800</v>
       </c>
       <c r="G238" t="s">
         <v>440</v>
       </c>
       <c r="H238" s="3">
-        <v>761.21</v>
+        <v>577.63</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7975,13 +7969,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>1561.960</v>
+        <v>542.080</v>
       </c>
       <c r="G239" t="s">
         <v>440</v>
       </c>
       <c r="H239" s="3">
-        <v>49071.25</v>
+        <v>17030.23</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -8183,13 +8177,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>228.000</v>
+        <v>218.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>1334.94</v>
+        <v>1276.39</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8209,13 +8203,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>75.000</v>
+        <v>73.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>413.17</v>
+        <v>402.15</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8235,13 +8229,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>4573.000</v>
+        <v>4539.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>11479.82</v>
+        <v>11394.48</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8287,13 +8281,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>556.74</v>
+        <v>3879.13</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8313,13 +8307,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>11.000</v>
+        <v>6.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>4741.17</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8339,13 +8333,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>2371.80</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8365,13 +8359,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>2323.99</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8397,7 +8391,7 @@
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>1462.82</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8417,13 +8411,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>6585.02</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8443,13 +8437,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>6.000</v>
+        <v>38.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>1694.29</v>
+        <v>17563.39</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8469,13 +8463,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>38.000</v>
+        <v>12.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>17563.39</v>
+        <v>6793.82</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8495,13 +8489,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>14.000</v>
+        <v>2.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>7926.12</v>
+        <v>3443.46</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8521,13 +8515,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>3443.46</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8547,13 +8541,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>6821.40</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8573,13 +8567,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>7220.40</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8599,13 +8593,13 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>7.000</v>
+        <v>17.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>2566.22</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -8625,13 +8619,13 @@
         <v>530</v>
       </c>
       <c r="F264" s="2">
-        <v>17.000</v>
+        <v>7.000</v>
       </c>
       <c r="G264" t="s">
         <v>5</v>
       </c>
       <c r="H264" s="3">
-        <v>7823.48</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="265" spans="1:8">
@@ -8651,13 +8645,13 @@
         <v>532</v>
       </c>
       <c r="F265" s="2">
-        <v>7.000</v>
+        <v>5.000</v>
       </c>
       <c r="G265" t="s">
         <v>5</v>
       </c>
       <c r="H265" s="3">
-        <v>3943.24</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="266" spans="1:8">
@@ -8677,38 +8671,12 @@
         <v>534</v>
       </c>
       <c r="F266" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G266" t="s">
         <v>5</v>
       </c>
       <c r="H266" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="267" spans="1:8">
-      <c r="A267" t="s">
-        <v>0</v>
-      </c>
-      <c r="B267" t="s">
-        <v>1</v>
-      </c>
-      <c r="C267" t="s">
-        <v>2</v>
-      </c>
-      <c r="D267" t="s">
-        <v>535</v>
-      </c>
-      <c r="E267" t="s">
-        <v>536</v>
-      </c>
-      <c r="F267" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G267" t="s">
-        <v>5</v>
-      </c>
-      <c r="H267" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: exclude troca pe cv preventivo by Ivan-Estevan
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -2951,13 +2951,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>209.000</v>
+        <v>207.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>116784.06</v>
+        <v>115666.50</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3211,13 +3211,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>1070.000</v>
+        <v>1068.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>9749.97</v>
+        <v>9731.75</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3263,13 +3263,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>2937.000</v>
+        <v>2936.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>30259.77</v>
+        <v>30249.47</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3575,13 +3575,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>823.000</v>
+        <v>821.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>4278.14</v>
+        <v>4267.74</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3809,13 +3809,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>93.000</v>
+        <v>91.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>1727.91</v>
+        <v>1690.75</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3887,13 +3887,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>1490.000</v>
+        <v>1482.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>9243.03</v>
+        <v>9193.41</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3913,13 +3913,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2730.000</v>
+        <v>2716.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>71108.99</v>
+        <v>70744.33</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4277,13 +4277,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>2370.000</v>
+        <v>2366.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>326455.65</v>
+        <v>325904.67</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4693,13 +4693,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>534.000</v>
+        <v>532.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>19817.18</v>
+        <v>19742.96</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4745,13 +4745,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>955.000</v>
+        <v>952.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>31464.35</v>
+        <v>31365.50</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4875,13 +4875,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>6608.000</v>
+        <v>6599.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>25546.41</v>
+        <v>25511.61</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -5187,13 +5187,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>257.000</v>
+        <v>251.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>2022.40</v>
+        <v>1975.18</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5785,13 +5785,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>505.000</v>
+        <v>497.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>2235.31</v>
+        <v>2199.90</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5941,13 +5941,13 @@
         <v>323</v>
       </c>
       <c r="F161" s="2">
-        <v>55.000</v>
+        <v>54.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>7342.99</v>
+        <v>7209.48</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -6305,13 +6305,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>2445.000</v>
+        <v>2444.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>45782.62</v>
+        <v>45763.90</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6383,13 +6383,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>35.000</v>
+        <v>30.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>6696.86</v>
+        <v>5740.16</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6409,13 +6409,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>671.000</v>
+        <v>668.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>117168.07</v>
+        <v>116644.22</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6903,13 +6903,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>261.000</v>
+        <v>257.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>18072.94</v>
+        <v>17795.97</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -7813,13 +7813,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>21657.800</v>
+        <v>21615.800</v>
       </c>
       <c r="G233" t="s">
         <v>440</v>
       </c>
       <c r="H233" s="3">
-        <v>49156.33</v>
+        <v>49061.00</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7917,13 +7917,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>615.610</v>
+        <v>564.600</v>
       </c>
       <c r="G237" t="s">
         <v>440</v>
       </c>
       <c r="H237" s="3">
-        <v>6281.47</v>
+        <v>5760.98</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -8229,13 +8229,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>4539.000</v>
+        <v>4538.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>11394.48</v>
+        <v>11391.96</v>
       </c>
     </row>
     <row r="250" spans="1:8">

</xml_diff>

<commit_message>
#fix: Close excel and remove hidro on main.rs
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="545">
   <si>
     <t>4600041302</t>
   </si>
@@ -1520,6 +1520,12 @@
   </si>
   <si>
     <t>VALV GAV CM REV ELAST BB JE CAB FF DN 50</t>
+  </si>
+  <si>
+    <t>30007804</t>
+  </si>
+  <si>
+    <t>VALV GAV CM REV ELAST BB JE CAB FF DN 75</t>
   </si>
   <si>
     <t>30003852</t>
@@ -1746,7 +1752,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H266"/>
+  <dimension ref="A1:H267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,28 +1772,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1807,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>81.000</v>
+        <v>80.000</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3">
-        <v>22356.37</v>
+        <v>22080.36</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1989,13 +1995,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>10.000</v>
+        <v>8.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>4275.79</v>
+        <v>3420.63</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2171,13 +2177,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>137.000</v>
+        <v>145.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>12967.64</v>
+        <v>13724.88</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2795,13 +2801,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>185.000</v>
+        <v>197.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>8690.25</v>
+        <v>9253.94</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2951,13 +2957,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>207.000</v>
+        <v>190.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>115666.50</v>
+        <v>106167.29</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3211,13 +3217,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>1068.000</v>
+        <v>1085.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>9731.75</v>
+        <v>9886.67</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3263,13 +3269,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>2936.000</v>
+        <v>2900.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>30249.47</v>
+        <v>29878.60</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3679,13 +3685,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>15.000</v>
+        <v>13.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>851.70</v>
+        <v>738.14</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3887,13 +3893,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>1482.000</v>
+        <v>1439.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>9193.41</v>
+        <v>8926.73</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3913,13 +3919,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2716.000</v>
+        <v>2811.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>70744.33</v>
+        <v>73218.78</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4147,13 +4153,13 @@
         <v>185</v>
       </c>
       <c r="F92" s="2">
-        <v>140.000</v>
+        <v>139.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>5277.30</v>
+        <v>5239.60</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -4277,13 +4283,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>2366.000</v>
+        <v>2298.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>325904.67</v>
+        <v>316538.01</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4693,13 +4699,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>532.000</v>
+        <v>554.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>19742.96</v>
+        <v>20559.40</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4719,13 +4725,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>352.000</v>
+        <v>348.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>23009.79</v>
+        <v>22748.31</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4745,13 +4751,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>952.000</v>
+        <v>965.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>31365.50</v>
+        <v>31793.79</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4797,13 +4803,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>39.000</v>
+        <v>36.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>3974.78</v>
+        <v>3669.03</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4875,13 +4881,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>6599.000</v>
+        <v>9461.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>25511.61</v>
+        <v>36575.88</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -5135,13 +5141,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>52.000</v>
+        <v>51.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>75002.98</v>
+        <v>73560.61</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5161,13 +5167,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>562.000</v>
+        <v>560.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>3181.37</v>
+        <v>3170.05</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5187,13 +5193,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>251.000</v>
+        <v>230.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>1975.18</v>
+        <v>1809.93</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5213,13 +5219,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>92.000</v>
+        <v>91.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1442.37</v>
+        <v>1426.69</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5785,13 +5791,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>497.000</v>
+        <v>472.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>2199.90</v>
+        <v>2089.24</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -6305,13 +6311,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>2444.000</v>
+        <v>2421.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>45763.90</v>
+        <v>45333.22</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6383,13 +6389,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>30.000</v>
+        <v>18.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>5740.16</v>
+        <v>3444.10</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6409,13 +6415,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>668.000</v>
+        <v>637.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>116644.22</v>
+        <v>111231.08</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6513,13 +6519,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>63.000</v>
+        <v>57.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>29216.54</v>
+        <v>26436.34</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6565,13 +6571,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>87.000</v>
+        <v>85.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>12699.17</v>
+        <v>12407.24</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6747,13 +6753,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>488.000</v>
+        <v>501.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>9886.88</v>
+        <v>10150.26</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6903,13 +6909,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>257.000</v>
+        <v>244.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>17795.97</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -7813,13 +7819,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>21615.800</v>
+        <v>21289.300</v>
       </c>
       <c r="G233" t="s">
         <v>440</v>
       </c>
       <c r="H233" s="3">
-        <v>49061.00</v>
+        <v>48319.93</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7917,13 +7923,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>564.600</v>
+        <v>366.100</v>
       </c>
       <c r="G237" t="s">
         <v>440</v>
       </c>
       <c r="H237" s="3">
-        <v>5760.98</v>
+        <v>3735.56</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7943,13 +7949,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>25.800</v>
+        <v>22.800</v>
       </c>
       <c r="G238" t="s">
         <v>440</v>
       </c>
       <c r="H238" s="3">
-        <v>577.63</v>
+        <v>510.46</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7969,13 +7975,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>542.080</v>
+        <v>521.080</v>
       </c>
       <c r="G239" t="s">
         <v>440</v>
       </c>
       <c r="H239" s="3">
-        <v>17030.23</v>
+        <v>16370.49</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -8125,13 +8131,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>52.790</v>
+        <v>48.790</v>
       </c>
       <c r="G245" t="s">
         <v>440</v>
       </c>
       <c r="H245" s="3">
-        <v>1134.03</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8177,13 +8183,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>218.000</v>
+        <v>233.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>1276.39</v>
+        <v>1364.22</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8229,13 +8235,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>4538.000</v>
+        <v>4834.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>11391.96</v>
+        <v>12135.03</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8281,13 +8287,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>9.000</v>
+        <v>6.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>3879.13</v>
+        <v>3340.44</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8307,13 +8313,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>6.000</v>
+        <v>9.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>2371.80</v>
+        <v>3879.13</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8333,13 +8339,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>2323.99</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8359,13 +8365,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>1462.82</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8391,7 +8397,7 @@
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>6585.02</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8411,13 +8417,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>1694.29</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8437,13 +8443,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>38.000</v>
+        <v>6.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>17563.39</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8463,13 +8469,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>12.000</v>
+        <v>38.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>6793.82</v>
+        <v>17563.39</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8489,13 +8495,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>2.000</v>
+        <v>12.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>3443.46</v>
+        <v>6793.82</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8515,13 +8521,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>6821.40</v>
+        <v>3443.46</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8541,13 +8547,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>7220.40</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8567,13 +8573,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>7.000</v>
+        <v>2.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>2566.22</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8593,13 +8599,13 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>17.000</v>
+        <v>7.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>7823.48</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -8619,13 +8625,13 @@
         <v>530</v>
       </c>
       <c r="F264" s="2">
-        <v>7.000</v>
+        <v>17.000</v>
       </c>
       <c r="G264" t="s">
         <v>5</v>
       </c>
       <c r="H264" s="3">
-        <v>3943.24</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="265" spans="1:8">
@@ -8645,13 +8651,13 @@
         <v>532</v>
       </c>
       <c r="F265" s="2">
-        <v>5.000</v>
+        <v>7.000</v>
       </c>
       <c r="G265" t="s">
         <v>5</v>
       </c>
       <c r="H265" s="3">
-        <v>2725.89</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="266" spans="1:8">
@@ -8671,12 +8677,38 @@
         <v>534</v>
       </c>
       <c r="F266" s="2">
+        <v>5.000</v>
+      </c>
+      <c r="G266" t="s">
+        <v>5</v>
+      </c>
+      <c r="H266" s="3">
+        <v>2725.89</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8">
+      <c r="A267" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" t="s">
+        <v>1</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2</v>
+      </c>
+      <c r="D267" t="s">
+        <v>535</v>
+      </c>
+      <c r="E267" t="s">
+        <v>536</v>
+      </c>
+      <c r="F267" s="2">
         <v>3.000</v>
       </c>
-      <c r="G266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H266" s="3">
+      <c r="G267" t="s">
+        <v>5</v>
+      </c>
+      <c r="H267" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#feat: escopo de materiais hidro plus saga
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="537">
   <si>
     <t>4600041302</t>
   </si>
@@ -259,24 +259,12 @@
     <t>CAVALETE PVC DN 20 (3/4) KIT COMPLETO-</t>
   </si>
   <si>
-    <t>30002194</t>
-  </si>
-  <si>
-    <t>COLAR TOM 200A400 MULTI FL DND 50</t>
-  </si>
-  <si>
     <t>30004691</t>
   </si>
   <si>
     <t>COLAR TOM 80A200 MULTI DND 80</t>
   </si>
   <si>
-    <t>30001075</t>
-  </si>
-  <si>
-    <t>COLAR TOM 80A200 MULTI FL DND 100</t>
-  </si>
-  <si>
     <t>30000287</t>
   </si>
   <si>
@@ -295,12 +283,6 @@
     <t>COLAR TOMADA ACO INOX DN50A150 X DNR20</t>
   </si>
   <si>
-    <t>30004703</t>
-  </si>
-  <si>
-    <t>COLAR TOMADA FF C.INOX DN200A300 X DNR20</t>
-  </si>
-  <si>
     <t>30002202</t>
   </si>
   <si>
@@ -595,6 +577,12 @@
     <t>HIDRANTE SUBT C/BASE FLANG DN 75 SIMPLES</t>
   </si>
   <si>
+    <t>50000108</t>
+  </si>
+  <si>
+    <t>HIDRO UNIJATO DN20 QN0,75 M³/H - PRE-EQ</t>
+  </si>
+  <si>
     <t>50000530</t>
   </si>
   <si>
@@ -1012,12 +1000,6 @@
     <t>REDUC CONC 225X110 TERMOF. PE 100 SDR 11</t>
   </si>
   <si>
-    <t>30006864</t>
-  </si>
-  <si>
-    <t>REDUCAO CONC ELETROF - DE 110 X 90</t>
-  </si>
-  <si>
     <t>30008609</t>
   </si>
   <si>
@@ -1211,12 +1193,6 @@
   </si>
   <si>
     <t>TE FF BOLSA JE2GS FLG DN150X75 PN10/16</t>
-  </si>
-  <si>
-    <t>30001891</t>
-  </si>
-  <si>
-    <t>TE FF BOLSA JE2GS FLG DN200X75 PN10/16</t>
   </si>
   <si>
     <t>30007308</t>
@@ -1752,7 +1728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H267"/>
+  <dimension ref="A1:H263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1772,28 +1748,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1813,13 +1789,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>80.000</v>
+        <v>75.000</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3">
-        <v>22080.36</v>
+        <v>20700.36</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1839,13 +1815,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="2">
-        <v>35.000</v>
+        <v>34.000</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>17904.38</v>
+        <v>17392.83</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1865,13 +1841,13 @@
         <v>9</v>
       </c>
       <c r="F4" s="2">
-        <v>23.000</v>
+        <v>21.000</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="3">
-        <v>20082.47</v>
+        <v>18336.17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1891,13 +1867,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>4.000</v>
+        <v>3.000</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="3">
-        <v>5140.67</v>
+        <v>3855.50</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1917,13 +1893,13 @@
         <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="3">
-        <v>13093.68</v>
+        <v>10474.94</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2001,7 +1977,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>3420.63</v>
+        <v>3420.62</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2177,13 +2153,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>145.000</v>
+        <v>147.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>13724.88</v>
+        <v>13914.19</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2229,13 +2205,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>623.000</v>
+        <v>622.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>1277.15</v>
+        <v>1275.10</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2411,13 +2387,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>334.000</v>
+        <v>324.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>28520.40</v>
+        <v>27666.50</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2495,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>59.98</v>
+        <v>61.38</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2645,13 +2621,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>339.93</v>
+        <v>460.48</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2697,13 +2673,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>15.000</v>
+        <v>14.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>675.15</v>
+        <v>630.14</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2723,13 +2699,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>17.000</v>
+        <v>16.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>553.16</v>
+        <v>520.62</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2749,13 +2725,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>15.000</v>
+        <v>13.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>838.61</v>
+        <v>726.80</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2801,13 +2777,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>197.000</v>
+        <v>134.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>9253.94</v>
+        <v>6294.60</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2827,13 +2803,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>4960.91</v>
+        <v>1940.18</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2853,13 +2829,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>1.000</v>
+        <v>234.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>1940.18</v>
+        <v>7009.47</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2879,13 +2855,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>1.000</v>
+        <v>170.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>2226.13</v>
+        <v>26952.61</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2905,13 +2881,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>241.000</v>
+        <v>90.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>7219.15</v>
+        <v>50289.75</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2931,13 +2907,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>200.000</v>
+        <v>46.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>31708.86</v>
+        <v>2898.44</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2957,13 +2933,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>190.000</v>
+        <v>2.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>106167.29</v>
+        <v>603.23</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2983,13 +2959,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>3.000</v>
+        <v>15.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>308.38</v>
+        <v>2103.77</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3009,13 +2985,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>46.000</v>
+        <v>9.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>2898.44</v>
+        <v>1883.67</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3035,13 +3011,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>603.23</v>
+        <v>2352.96</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3061,13 +3037,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>16.000</v>
+        <v>9.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>2244.02</v>
+        <v>3592.71</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3087,13 +3063,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>10.000</v>
+        <v>1.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>2092.96</v>
+        <v>863.17</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3113,13 +3089,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>8.000</v>
+        <v>3.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>2352.96</v>
+        <v>295.57</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3139,13 +3115,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>9.000</v>
+        <v>1058.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>3592.71</v>
+        <v>9622.30</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3165,13 +3141,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>1.000</v>
+        <v>40.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>863.17</v>
+        <v>641.18</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3191,13 +3167,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>3.000</v>
+        <v>2968.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>295.57</v>
+        <v>30516.09</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3217,13 +3193,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>1085.000</v>
+        <v>11.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>9886.67</v>
+        <v>380.69</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3243,13 +3219,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>40.000</v>
+        <v>9.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>641.18</v>
+        <v>334.55</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3269,13 +3245,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>2900.000</v>
+        <v>5.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>29878.60</v>
+        <v>1390.00</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3295,13 +3271,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>11.000</v>
+        <v>23.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>380.69</v>
+        <v>1071.88</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3321,13 +3297,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>9.000</v>
+        <v>11.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>334.55</v>
+        <v>1357.53</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3347,13 +3323,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>5.000</v>
+        <v>16.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>1390.00</v>
+        <v>902.16</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3373,13 +3349,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>24.000</v>
+        <v>28.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>1118.48</v>
+        <v>2209.27</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3399,13 +3375,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>11.000</v>
+        <v>14.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>1357.53</v>
+        <v>416.43</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3425,13 +3401,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>16.000</v>
+        <v>37.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>902.16</v>
+        <v>2108.34</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3451,13 +3427,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>28.000</v>
+        <v>4.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>2209.27</v>
+        <v>606.42</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3477,13 +3453,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>237.96</v>
+        <v>1448.47</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3503,13 +3479,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>37.000</v>
+        <v>1018.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>2108.34</v>
+        <v>5182.29</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3529,13 +3505,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>4.000</v>
+        <v>23.000</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>606.42</v>
+        <v>1359.47</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3555,13 +3531,13 @@
         <v>139</v>
       </c>
       <c r="F69" s="2">
-        <v>1.000</v>
+        <v>42.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>1448.47</v>
+        <v>5269.67</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3581,13 +3557,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>821.000</v>
+        <v>180.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>4267.74</v>
+        <v>1598.50</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3607,13 +3583,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>23.000</v>
+        <v>13.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>1359.47</v>
+        <v>738.14</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3633,13 +3609,13 @@
         <v>145</v>
       </c>
       <c r="F72" s="2">
-        <v>40.000</v>
+        <v>6.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>5018.74</v>
+        <v>344.01</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3659,13 +3635,13 @@
         <v>147</v>
       </c>
       <c r="F73" s="2">
-        <v>180.000</v>
+        <v>5.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>1598.49</v>
+        <v>837.86</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3685,13 +3661,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>13.000</v>
+        <v>47.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>738.14</v>
+        <v>4841.34</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3711,13 +3687,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>344.01</v>
+        <v>495.95</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3737,13 +3713,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>5.000</v>
+        <v>90.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>837.86</v>
+        <v>1672.17</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3763,13 +3739,13 @@
         <v>155</v>
       </c>
       <c r="F77" s="2">
-        <v>47.000</v>
+        <v>1.000</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>4841.34</v>
+        <v>131.57</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3789,13 +3765,13 @@
         <v>157</v>
       </c>
       <c r="F78" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>495.95</v>
+        <v>86.93</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3815,13 +3791,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>91.000</v>
+        <v>1381.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>1690.75</v>
+        <v>8569.11</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3841,13 +3817,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>1.000</v>
+        <v>2475.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>131.57</v>
+        <v>64468.32</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3867,13 +3843,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>72.70</v>
+        <v>383.07</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3893,13 +3869,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>1439.000</v>
+        <v>3.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>8926.73</v>
+        <v>651.71</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3919,13 +3895,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2811.000</v>
+        <v>3.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>73218.78</v>
+        <v>1263.43</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3945,13 +3921,13 @@
         <v>169</v>
       </c>
       <c r="F84" s="2">
-        <v>5.000</v>
+        <v>12.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>383.07</v>
+        <v>2226.44</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3971,13 +3947,13 @@
         <v>171</v>
       </c>
       <c r="F85" s="2">
-        <v>3.000</v>
+        <v>4.000</v>
       </c>
       <c r="G85" t="s">
         <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>651.71</v>
+        <v>1008.05</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3997,13 +3973,13 @@
         <v>173</v>
       </c>
       <c r="F86" s="2">
-        <v>3.000</v>
+        <v>14.000</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>1263.43</v>
+        <v>1572.64</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4023,13 +3999,13 @@
         <v>175</v>
       </c>
       <c r="F87" s="2">
-        <v>15.000</v>
+        <v>10.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>2783.05</v>
+        <v>4602.91</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4049,13 +4025,13 @@
         <v>177</v>
       </c>
       <c r="F88" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>1008.05</v>
+        <v>3671.99</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4075,13 +4051,13 @@
         <v>179</v>
       </c>
       <c r="F89" s="2">
-        <v>14.000</v>
+        <v>137.000</v>
       </c>
       <c r="G89" t="s">
         <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>1572.64</v>
+        <v>5164.21</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4101,13 +4077,13 @@
         <v>181</v>
       </c>
       <c r="F90" s="2">
-        <v>12.000</v>
+        <v>2.000</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>5523.49</v>
+        <v>560.27</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4127,13 +4103,13 @@
         <v>183</v>
       </c>
       <c r="F91" s="2">
-        <v>2.000</v>
+        <v>37.000</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>3671.99</v>
+        <v>3385.96</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -4153,13 +4129,13 @@
         <v>185</v>
       </c>
       <c r="F92" s="2">
-        <v>139.000</v>
+        <v>1.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>5239.60</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -4179,13 +4155,13 @@
         <v>187</v>
       </c>
       <c r="F93" s="2">
-        <v>2.000</v>
+        <v>10.000</v>
       </c>
       <c r="G93" t="s">
         <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>560.27</v>
+        <v>18133.05</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -4205,13 +4181,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>38.000</v>
+        <v>250.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>3477.47</v>
+        <v>21243.00</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4231,13 +4207,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>1.000</v>
+        <v>2361.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>2.97</v>
+        <v>325215.95</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4257,13 +4233,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>11.000</v>
+        <v>1.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>19946.36</v>
+        <v>2980.59</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4283,13 +4259,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>2298.000</v>
+        <v>1.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>316538.01</v>
+        <v>4463.84</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4309,13 +4285,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>2980.59</v>
+        <v>1598.31</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4335,13 +4311,13 @@
         <v>199</v>
       </c>
       <c r="F99" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>4463.84</v>
+        <v>23432.75</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4361,13 +4337,13 @@
         <v>201</v>
       </c>
       <c r="F100" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G100" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>1598.31</v>
+        <v>11241.86</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4387,13 +4363,13 @@
         <v>203</v>
       </c>
       <c r="F101" s="2">
-        <v>20.000</v>
+        <v>3.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>24666.05</v>
+        <v>1127.59</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4413,13 +4389,13 @@
         <v>205</v>
       </c>
       <c r="F102" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>10134.33</v>
+        <v>279.59</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4439,13 +4415,13 @@
         <v>207</v>
       </c>
       <c r="F103" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G103" t="s">
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>375.86</v>
+        <v>740.97</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4465,13 +4441,13 @@
         <v>209</v>
       </c>
       <c r="F104" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>279.59</v>
+        <v>902.80</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4497,7 +4473,7 @@
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>740.97</v>
+        <v>994.54</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -4523,7 +4499,7 @@
         <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>902.80</v>
+        <v>1033.65</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -4549,7 +4525,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>994.54</v>
+        <v>1166.57</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4569,13 +4545,13 @@
         <v>217</v>
       </c>
       <c r="F108" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G108" t="s">
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>1033.65</v>
+        <v>2825.06</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4595,13 +4571,13 @@
         <v>219</v>
       </c>
       <c r="F109" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>1166.57</v>
+        <v>91.20</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4621,13 +4597,13 @@
         <v>221</v>
       </c>
       <c r="F110" s="2">
-        <v>8.000</v>
+        <v>2.000</v>
       </c>
       <c r="G110" t="s">
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>2825.06</v>
+        <v>719.47</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4647,13 +4623,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>1.000</v>
+        <v>565.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>91.20</v>
+        <v>20967.62</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4673,13 +4649,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>2.000</v>
+        <v>343.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>719.47</v>
+        <v>22421.45</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4699,13 +4675,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>554.000</v>
+        <v>973.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>20559.40</v>
+        <v>32057.33</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4725,13 +4701,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>348.000</v>
+        <v>174.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>22748.31</v>
+        <v>8940.70</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4751,13 +4727,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>965.000</v>
+        <v>32.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>31793.79</v>
+        <v>3261.36</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4777,13 +4753,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>174.000</v>
+        <v>45.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>8940.70</v>
+        <v>1519.40</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4803,13 +4779,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>36.000</v>
+        <v>9.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>3669.03</v>
+        <v>1675.75</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4829,13 +4805,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>45.000</v>
+        <v>11172.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>1519.40</v>
+        <v>43365.52</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4855,13 +4831,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>9.000</v>
+        <v>2.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>1675.75</v>
+        <v>2463.85</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4881,13 +4857,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>9461.000</v>
+        <v>2.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>36575.88</v>
+        <v>4533.88</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4907,13 +4883,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>2463.85</v>
+        <v>6385.34</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4933,13 +4909,13 @@
         <v>245</v>
       </c>
       <c r="F122" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>4533.88</v>
+        <v>12368.67</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4959,13 +4935,13 @@
         <v>247</v>
       </c>
       <c r="F123" s="2">
-        <v>4.000</v>
+        <v>3.000</v>
       </c>
       <c r="G123" t="s">
         <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>6385.34</v>
+        <v>3260.53</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4985,13 +4961,13 @@
         <v>249</v>
       </c>
       <c r="F124" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>12368.67</v>
+        <v>3527.49</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -5017,7 +4993,7 @@
         <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>3260.53</v>
+        <v>6294.26</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5037,13 +5013,13 @@
         <v>253</v>
       </c>
       <c r="F126" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G126" t="s">
         <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>3527.49</v>
+        <v>4585.00</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5063,13 +5039,13 @@
         <v>255</v>
       </c>
       <c r="F127" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G127" t="s">
         <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>6294.26</v>
+        <v>14225.45</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -5089,13 +5065,13 @@
         <v>257</v>
       </c>
       <c r="F128" s="2">
-        <v>1.000</v>
+        <v>39.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>4585.00</v>
+        <v>56252.23</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5115,13 +5091,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>2.000</v>
+        <v>560.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>14225.45</v>
+        <v>3170.06</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5141,13 +5117,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>51.000</v>
+        <v>261.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>73560.61</v>
+        <v>2053.87</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5167,13 +5143,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>560.000</v>
+        <v>91.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>3170.05</v>
+        <v>1426.69</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5193,13 +5169,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>230.000</v>
+        <v>110.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>1809.93</v>
+        <v>1499.69</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5219,13 +5195,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>91.000</v>
+        <v>60.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1426.69</v>
+        <v>1831.37</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5245,13 +5221,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>110.000</v>
+        <v>26.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>1499.69</v>
+        <v>3249.51</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5271,13 +5247,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>42.000</v>
+        <v>1.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>1281.96</v>
+        <v>194.13</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5297,13 +5273,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>26.000</v>
+        <v>2.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>2958.39</v>
+        <v>159.15</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5323,13 +5299,13 @@
         <v>275</v>
       </c>
       <c r="F137" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G137" t="s">
         <v>5</v>
       </c>
       <c r="H137" s="3">
-        <v>194.13</v>
+        <v>499.74</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5349,13 +5325,13 @@
         <v>277</v>
       </c>
       <c r="F138" s="2">
-        <v>2.000</v>
+        <v>41.000</v>
       </c>
       <c r="G138" t="s">
         <v>5</v>
       </c>
       <c r="H138" s="3">
-        <v>159.15</v>
+        <v>2975.17</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5375,13 +5351,13 @@
         <v>279</v>
       </c>
       <c r="F139" s="2">
-        <v>2.000</v>
+        <v>11.000</v>
       </c>
       <c r="G139" t="s">
         <v>5</v>
       </c>
       <c r="H139" s="3">
-        <v>499.74</v>
+        <v>1674.52</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5401,13 +5377,13 @@
         <v>281</v>
       </c>
       <c r="F140" s="2">
-        <v>41.000</v>
+        <v>12.000</v>
       </c>
       <c r="G140" t="s">
         <v>5</v>
       </c>
       <c r="H140" s="3">
-        <v>2975.17</v>
+        <v>5671.40</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5427,13 +5403,13 @@
         <v>283</v>
       </c>
       <c r="F141" s="2">
-        <v>15.000</v>
+        <v>8.000</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
       </c>
       <c r="H141" s="3">
-        <v>2283.44</v>
+        <v>5567.25</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5453,13 +5429,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G142" t="s">
         <v>5</v>
       </c>
       <c r="H142" s="3">
-        <v>5668.76</v>
+        <v>5624.37</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5479,13 +5455,13 @@
         <v>287</v>
       </c>
       <c r="F143" s="2">
-        <v>9.000</v>
+        <v>5.000</v>
       </c>
       <c r="G143" t="s">
         <v>5</v>
       </c>
       <c r="H143" s="3">
-        <v>6255.98</v>
+        <v>5802.02</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5505,13 +5481,13 @@
         <v>289</v>
       </c>
       <c r="F144" s="2">
-        <v>6.000</v>
+        <v>3.000</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
       </c>
       <c r="H144" s="3">
-        <v>5624.37</v>
+        <v>5120.09</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5537,7 +5513,7 @@
         <v>5</v>
       </c>
       <c r="H145" s="3">
-        <v>5800.85</v>
+        <v>1690.54</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5557,13 +5533,13 @@
         <v>293</v>
       </c>
       <c r="F146" s="2">
-        <v>3.000</v>
+        <v>4.000</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
       </c>
       <c r="H146" s="3">
-        <v>5120.09</v>
+        <v>1094.94</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5583,13 +5559,13 @@
         <v>295</v>
       </c>
       <c r="F147" s="2">
-        <v>5.000</v>
+        <v>16.000</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
       </c>
       <c r="H147" s="3">
-        <v>1690.54</v>
+        <v>4737.64</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5609,13 +5585,13 @@
         <v>297</v>
       </c>
       <c r="F148" s="2">
-        <v>9.000</v>
+        <v>3.000</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
       </c>
       <c r="H148" s="3">
-        <v>2463.61</v>
+        <v>162.71</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5635,13 +5611,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>16.000</v>
+        <v>3.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>4737.64</v>
+        <v>314.31</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5661,13 +5637,13 @@
         <v>301</v>
       </c>
       <c r="F150" s="2">
-        <v>3.000</v>
+        <v>30.000</v>
       </c>
       <c r="G150" t="s">
         <v>5</v>
       </c>
       <c r="H150" s="3">
-        <v>162.71</v>
+        <v>179.62</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5687,13 +5663,13 @@
         <v>303</v>
       </c>
       <c r="F151" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
       </c>
       <c r="H151" s="3">
-        <v>419.08</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5713,13 +5689,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>30.000</v>
+        <v>10.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>179.61</v>
+        <v>374.15</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5739,13 +5715,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>6.000</v>
+        <v>468.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>98.34</v>
+        <v>2071.35</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5765,13 +5741,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>10.000</v>
+        <v>16.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>374.16</v>
+        <v>1204.47</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5791,13 +5767,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>472.000</v>
+        <v>1.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>2089.24</v>
+        <v>135.35</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5817,13 +5793,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>16.000</v>
+        <v>25.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>1204.47</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5843,13 +5819,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>270.71</v>
+        <v>955.65</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5869,13 +5845,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>25.000</v>
+        <v>33.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>116.25</v>
+        <v>3371.47</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5895,13 +5871,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>10.000</v>
+        <v>55.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>1194.56</v>
+        <v>7342.99</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5921,13 +5897,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>34.000</v>
+        <v>1.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>3473.64</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5944,16 +5920,16 @@
         <v>322</v>
       </c>
       <c r="E161" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F161" s="2">
-        <v>54.000</v>
+        <v>4.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>7209.48</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5967,19 +5943,19 @@
         <v>2</v>
       </c>
       <c r="D162" t="s">
+        <v>323</v>
+      </c>
+      <c r="E162" t="s">
         <v>324</v>
       </c>
-      <c r="E162" t="s">
-        <v>325</v>
-      </c>
       <c r="F162" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>40.71</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5993,19 +5969,19 @@
         <v>2</v>
       </c>
       <c r="D163" t="s">
+        <v>325</v>
+      </c>
+      <c r="E163" t="s">
         <v>326</v>
       </c>
-      <c r="E163" t="s">
-        <v>325</v>
-      </c>
       <c r="F163" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G163" t="s">
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>317.81</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6025,13 +6001,13 @@
         <v>328</v>
       </c>
       <c r="F164" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G164" t="s">
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>483.20</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6051,13 +6027,13 @@
         <v>330</v>
       </c>
       <c r="F165" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G165" t="s">
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>45.92</v>
+        <v>1141.60</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6077,13 +6053,13 @@
         <v>332</v>
       </c>
       <c r="F166" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G166" t="s">
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>303.12</v>
+        <v>1028.70</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6103,13 +6079,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>266.42</v>
+        <v>362.54</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6129,13 +6105,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>8.000</v>
+        <v>2.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>1141.60</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6155,13 +6131,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>1028.70</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6187,7 +6163,7 @@
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>543.81</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6207,13 +6183,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>2.000</v>
+        <v>15.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>412.45</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6233,13 +6209,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>1.000</v>
+        <v>2280.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>24.27</v>
+        <v>42693.00</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6259,13 +6235,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>9.000</v>
+        <v>123226.000</v>
       </c>
       <c r="G173" t="s">
-        <v>5</v>
+        <v>347</v>
       </c>
       <c r="H173" s="3">
-        <v>214.33</v>
+        <v>185533.15</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6279,19 +6255,19 @@
         <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E174" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F174" s="2">
-        <v>15.000</v>
+        <v>101.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>3032.79</v>
+        <v>3600.02</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6305,19 +6281,19 @@
         <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E175" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F175" s="2">
-        <v>2421.000</v>
+        <v>47.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>45333.22</v>
+        <v>8992.92</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6331,19 +6307,19 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E176" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>12.000</v>
+        <v>626.000</v>
       </c>
       <c r="G176" t="s">
-        <v>353</v>
+        <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>18.02</v>
+        <v>109310.27</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6363,13 +6339,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>101.000</v>
+        <v>13.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>3600.02</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6389,13 +6365,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>18.000</v>
+        <v>11.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>3444.10</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6415,13 +6391,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>637.000</v>
+        <v>22.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>111231.08</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6441,13 +6417,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>13.000</v>
+        <v>75.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>2264.65</v>
+        <v>34789.96</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6467,13 +6443,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>11.000</v>
+        <v>37.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>145.79</v>
+        <v>2259.59</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6493,13 +6469,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>22.000</v>
+        <v>80.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>10363.87</v>
+        <v>11677.39</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6519,13 +6495,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>57.000</v>
+        <v>1.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>26436.34</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6545,13 +6521,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>21.000</v>
+        <v>1.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>1282.47</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6571,13 +6547,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>85.000</v>
+        <v>182.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>12407.24</v>
+        <v>6080.43</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6597,13 +6573,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>1.000</v>
+        <v>28.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1218.18</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6623,13 +6599,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>1.000</v>
+        <v>441.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>1720.00</v>
+        <v>6893.88</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6649,13 +6625,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>184.000</v>
+        <v>59.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>6147.25</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6675,13 +6651,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>28.000</v>
+        <v>513.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>1119.31</v>
+        <v>10393.38</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6701,13 +6677,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>458.000</v>
+        <v>43.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>7159.59</v>
+        <v>998.72</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6727,13 +6703,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>59.000</v>
+        <v>93.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>1003.06</v>
+        <v>6626.71</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6753,13 +6729,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>501.000</v>
+        <v>16.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>10150.26</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6779,13 +6755,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>44.000</v>
+        <v>1.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>1021.95</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6805,13 +6781,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>96.000</v>
+        <v>19.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>6840.48</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6831,13 +6807,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>16.000</v>
+        <v>244.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>1789.69</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6857,13 +6833,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>189.22</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6883,13 +6859,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>19.000</v>
+        <v>1.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>1201.67</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6909,13 +6885,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>244.000</v>
+        <v>5.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>16895.78</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6935,13 +6911,13 @@
         <v>399</v>
       </c>
       <c r="F199" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>651.09</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6967,7 +6943,7 @@
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>562.67</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6987,13 +6963,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>1125.55</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7013,13 +6989,13 @@
         <v>405</v>
       </c>
       <c r="F202" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G202" t="s">
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>718.30</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7039,13 +7015,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>266.26</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7065,13 +7041,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>257.36</v>
+        <v>493.11</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7091,13 +7067,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>961.64</v>
+        <v>885.89</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7117,13 +7093,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>1.000</v>
+        <v>37.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>726.22</v>
+        <v>5096.66</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7143,13 +7119,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>662.53</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7169,13 +7145,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>493.11</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7195,13 +7171,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>7.000</v>
+        <v>38.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>885.89</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7221,13 +7197,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>38.000</v>
+        <v>1.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>5234.40</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7247,13 +7223,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>1.000</v>
+        <v>17.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>4700.00</v>
+        <v>646.00</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7273,13 +7249,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>1.000</v>
+        <v>24.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>8560.17</v>
+        <v>1584.75</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7299,13 +7275,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>40.000</v>
+        <v>1.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>506.58</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7325,13 +7301,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>23.34</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7351,13 +7327,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>11.000</v>
+        <v>4.800</v>
       </c>
       <c r="G215" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="H215" s="3">
-        <v>418.00</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7371,19 +7347,19 @@
         <v>2</v>
       </c>
       <c r="D216" t="s">
+        <v>433</v>
+      </c>
+      <c r="E216" t="s">
+        <v>434</v>
+      </c>
+      <c r="F216" s="2">
+        <v>16.000</v>
+      </c>
+      <c r="G216" t="s">
         <v>432</v>
       </c>
-      <c r="E216" t="s">
-        <v>433</v>
-      </c>
-      <c r="F216" s="2">
-        <v>24.000</v>
-      </c>
-      <c r="G216" t="s">
-        <v>5</v>
-      </c>
       <c r="H216" s="3">
-        <v>1584.75</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7397,19 +7373,19 @@
         <v>2</v>
       </c>
       <c r="D217" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E217" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F217" s="2">
-        <v>1.000</v>
+        <v>17.000</v>
       </c>
       <c r="G217" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="H217" s="3">
-        <v>685.11</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7423,19 +7399,19 @@
         <v>2</v>
       </c>
       <c r="D218" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E218" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F218" s="2">
-        <v>2.000</v>
+        <v>162.140</v>
       </c>
       <c r="G218" t="s">
-        <v>5</v>
+        <v>432</v>
       </c>
       <c r="H218" s="3">
-        <v>8149.76</v>
+        <v>35221.32</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7449,19 +7425,19 @@
         <v>2</v>
       </c>
       <c r="D219" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E219" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F219" s="2">
-        <v>4.800</v>
+        <v>1.090</v>
       </c>
       <c r="G219" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H219" s="3">
-        <v>1822.34</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7481,13 +7457,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>16.000</v>
+        <v>20.300</v>
       </c>
       <c r="G220" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H220" s="3">
-        <v>7011.29</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7507,13 +7483,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>17.000</v>
+        <v>13.000</v>
       </c>
       <c r="G221" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H221" s="3">
-        <v>2938.94</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7533,13 +7509,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>163.140</v>
+        <v>22.000</v>
       </c>
       <c r="G222" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H222" s="3">
-        <v>35438.55</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7559,13 +7535,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>1.090</v>
+        <v>343.600</v>
       </c>
       <c r="G223" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H223" s="3">
-        <v>250.66</v>
+        <v>3442.91</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7585,13 +7561,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>20.300</v>
+        <v>0.360</v>
       </c>
       <c r="G224" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H224" s="3">
-        <v>6816.84</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7611,13 +7587,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>13.000</v>
+        <v>11.000</v>
       </c>
       <c r="G225" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H225" s="3">
-        <v>3437.72</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7637,13 +7613,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>22.000</v>
+        <v>84.000</v>
       </c>
       <c r="G226" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H226" s="3">
-        <v>2084.93</v>
+        <v>13440.76</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7663,13 +7639,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>345.400</v>
+        <v>168.620</v>
       </c>
       <c r="G227" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H227" s="3">
-        <v>3460.95</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7689,13 +7665,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>1.860</v>
+        <v>47.250</v>
       </c>
       <c r="G228" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H228" s="3">
-        <v>40.25</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7715,13 +7691,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>11.000</v>
+        <v>20268.300</v>
       </c>
       <c r="G229" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H229" s="3">
-        <v>974.64</v>
+        <v>46002.35</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7741,13 +7717,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>84.000</v>
+        <v>2783.970</v>
       </c>
       <c r="G230" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H230" s="3">
-        <v>13440.76</v>
+        <v>11884.96</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7767,13 +7743,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>168.620</v>
+        <v>29.390</v>
       </c>
       <c r="G231" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H231" s="3">
-        <v>8798.84</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7793,13 +7769,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>47.250</v>
+        <v>856.370</v>
       </c>
       <c r="G232" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H232" s="3">
-        <v>5148.59</v>
+        <v>32198.67</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7819,13 +7795,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>21289.300</v>
+        <v>0.100</v>
       </c>
       <c r="G233" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H233" s="3">
-        <v>48319.93</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7845,13 +7821,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>2786.970</v>
+        <v>57.800</v>
       </c>
       <c r="G234" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H234" s="3">
-        <v>11897.77</v>
+        <v>1294.06</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7871,13 +7847,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>29.390</v>
+        <v>1191.970</v>
       </c>
       <c r="G235" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H235" s="3">
-        <v>15217.18</v>
+        <v>37447.47</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7897,13 +7873,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>857.370</v>
+        <v>270.420</v>
       </c>
       <c r="G236" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H236" s="3">
-        <v>32236.27</v>
+        <v>24811.50</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7923,13 +7899,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>366.100</v>
+        <v>59.100</v>
       </c>
       <c r="G237" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H237" s="3">
-        <v>3735.56</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7949,13 +7925,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>22.800</v>
+        <v>237.900</v>
       </c>
       <c r="G238" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H238" s="3">
-        <v>510.46</v>
+        <v>7688.51</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7975,13 +7951,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>521.080</v>
+        <v>91.020</v>
       </c>
       <c r="G239" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H239" s="3">
-        <v>16370.49</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -8001,13 +7977,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>270.420</v>
+        <v>0.690</v>
       </c>
       <c r="G240" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H240" s="3">
-        <v>24811.50</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8027,13 +8003,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>59.100</v>
+        <v>48.790</v>
       </c>
       <c r="G241" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H241" s="3">
-        <v>9271.17</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8053,13 +8029,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>241.900</v>
+        <v>78.310</v>
       </c>
       <c r="G242" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="H242" s="3">
-        <v>7817.79</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8079,13 +8055,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>91.020</v>
+        <v>216.000</v>
       </c>
       <c r="G243" t="s">
-        <v>440</v>
+        <v>5</v>
       </c>
       <c r="H243" s="3">
-        <v>1685.63</v>
+        <v>1264.68</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8105,13 +8081,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>0.690</v>
+        <v>73.000</v>
       </c>
       <c r="G244" t="s">
-        <v>440</v>
+        <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>20.12</v>
+        <v>402.15</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8131,13 +8107,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>48.790</v>
+        <v>4996.000</v>
       </c>
       <c r="G245" t="s">
-        <v>440</v>
+        <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>1048.10</v>
+        <v>12541.72</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8157,13 +8133,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>78.310</v>
+        <v>8.000</v>
       </c>
       <c r="G246" t="s">
-        <v>440</v>
+        <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>7083.14</v>
+        <v>2847.85</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8183,13 +8159,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>233.000</v>
+        <v>6.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>1364.22</v>
+        <v>3340.44</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8209,13 +8185,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>73.000</v>
+        <v>10.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>402.15</v>
+        <v>4310.15</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8235,13 +8211,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>4834.000</v>
+        <v>6.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>12135.03</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8261,13 +8237,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>9.000</v>
+        <v>2.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>3203.83</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8287,13 +8263,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>3340.44</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8313,13 +8289,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>3879.13</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8345,7 +8321,7 @@
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>2371.80</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8365,13 +8341,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>2.000</v>
+        <v>45.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>2323.99</v>
+        <v>20798.75</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8391,13 +8367,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>1462.82</v>
+        <v>4529.21</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8423,7 +8399,7 @@
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>6585.02</v>
+        <v>1721.73</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8443,13 +8419,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>1694.29</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8469,13 +8445,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>38.000</v>
+        <v>2.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>17563.39</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8495,13 +8471,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>12.000</v>
+        <v>7.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>6793.82</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8521,13 +8497,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>2.000</v>
+        <v>17.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>3443.46</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8547,13 +8523,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>4.000</v>
+        <v>7.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>6821.40</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8573,13 +8549,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>2.000</v>
+        <v>5.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>7220.40</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8599,116 +8575,12 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>7.000</v>
+        <v>3.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>2566.22</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8">
-      <c r="A264" t="s">
-        <v>0</v>
-      </c>
-      <c r="B264" t="s">
-        <v>1</v>
-      </c>
-      <c r="C264" t="s">
-        <v>2</v>
-      </c>
-      <c r="D264" t="s">
-        <v>529</v>
-      </c>
-      <c r="E264" t="s">
-        <v>530</v>
-      </c>
-      <c r="F264" s="2">
-        <v>17.000</v>
-      </c>
-      <c r="G264" t="s">
-        <v>5</v>
-      </c>
-      <c r="H264" s="3">
-        <v>7823.48</v>
-      </c>
-    </row>
-    <row r="265" spans="1:8">
-      <c r="A265" t="s">
-        <v>0</v>
-      </c>
-      <c r="B265" t="s">
-        <v>1</v>
-      </c>
-      <c r="C265" t="s">
-        <v>2</v>
-      </c>
-      <c r="D265" t="s">
-        <v>531</v>
-      </c>
-      <c r="E265" t="s">
-        <v>532</v>
-      </c>
-      <c r="F265" s="2">
-        <v>7.000</v>
-      </c>
-      <c r="G265" t="s">
-        <v>5</v>
-      </c>
-      <c r="H265" s="3">
-        <v>3943.24</v>
-      </c>
-    </row>
-    <row r="266" spans="1:8">
-      <c r="A266" t="s">
-        <v>0</v>
-      </c>
-      <c r="B266" t="s">
-        <v>1</v>
-      </c>
-      <c r="C266" t="s">
-        <v>2</v>
-      </c>
-      <c r="D266" t="s">
-        <v>533</v>
-      </c>
-      <c r="E266" t="s">
-        <v>534</v>
-      </c>
-      <c r="F266" s="2">
-        <v>5.000</v>
-      </c>
-      <c r="G266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H266" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="267" spans="1:8">
-      <c r="A267" t="s">
-        <v>0</v>
-      </c>
-      <c r="B267" t="s">
-        <v>1</v>
-      </c>
-      <c r="C267" t="s">
-        <v>2</v>
-      </c>
-      <c r="D267" t="s">
-        <v>535</v>
-      </c>
-      <c r="E267" t="s">
-        <v>536</v>
-      </c>
-      <c r="F267" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G267" t="s">
-        <v>5</v>
-      </c>
-      <c r="H267" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: multiple sessions instances
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -1123,16 +1123,16 @@
     <t>TE DE SELA ELETROF DE 355X110 TP FEMEA</t>
   </si>
   <si>
+    <t>30008677</t>
+  </si>
+  <si>
+    <t>TE DE SERV INTEGR ART DN 100 P/ DE 32</t>
+  </si>
+  <si>
     <t>30000211</t>
   </si>
   <si>
-    <t>TE DE SERV INTEGR ART DN 100 P/ DE 20</t>
-  </si>
-  <si>
-    <t>30008677</t>
-  </si>
-  <si>
-    <t>TE DE SERV INTEGR ART DN 100 P/ DE 32</t>
+    <t>TE DE SERV INTEGR ART DN 100-DE 110 X 20</t>
   </si>
   <si>
     <t>30007034</t>
@@ -1815,13 +1815,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="2">
-        <v>34.000</v>
+        <v>35.000</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>17392.83</v>
+        <v>17904.38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1971,13 +1971,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>8.000</v>
+        <v>6.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>3420.62</v>
+        <v>2565.46</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2543,13 +2543,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>4.000</v>
+        <v>3.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>618.66</v>
+        <v>463.99</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2777,13 +2777,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>134.000</v>
+        <v>122.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>6294.60</v>
+        <v>5730.91</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2855,13 +2855,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>170.000</v>
+        <v>111.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>26952.61</v>
+        <v>17598.49</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2881,13 +2881,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>90.000</v>
+        <v>74.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>50289.75</v>
+        <v>41349.35</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3115,13 +3115,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>1058.000</v>
+        <v>937.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>9622.30</v>
+        <v>8521.93</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3167,13 +3167,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>2968.000</v>
+        <v>2854.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>30516.09</v>
+        <v>29344.07</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3251,7 +3251,7 @@
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>1390.00</v>
+        <v>1454.70</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3479,13 +3479,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>1018.000</v>
+        <v>1187.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>5182.29</v>
+        <v>6042.61</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3641,7 +3641,7 @@
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>837.86</v>
+        <v>507.80</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3713,13 +3713,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>90.000</v>
+        <v>81.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>1672.17</v>
+        <v>1504.95</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3791,13 +3791,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>1381.000</v>
+        <v>1299.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>8569.11</v>
+        <v>7984.61</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3817,13 +3817,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>2475.000</v>
+        <v>2736.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>64468.32</v>
+        <v>71266.70</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -4103,13 +4103,13 @@
         <v>183</v>
       </c>
       <c r="F91" s="2">
-        <v>37.000</v>
+        <v>36.000</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>3385.96</v>
+        <v>3294.45</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -4181,13 +4181,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>250.000</v>
+        <v>255.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>21243.00</v>
+        <v>21667.90</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4207,13 +4207,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>2361.000</v>
+        <v>2341.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>325215.95</v>
+        <v>322461.05</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4337,13 +4337,13 @@
         <v>201</v>
       </c>
       <c r="F100" s="2">
-        <v>6.000</v>
+        <v>7.000</v>
       </c>
       <c r="G100" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>11241.86</v>
+        <v>13115.50</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4623,13 +4623,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>565.000</v>
+        <v>601.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>20967.62</v>
+        <v>22303.61</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4649,13 +4649,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>343.000</v>
+        <v>340.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>22421.45</v>
+        <v>22225.34</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4675,13 +4675,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>973.000</v>
+        <v>1037.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>32057.33</v>
+        <v>34165.86</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4701,13 +4701,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>174.000</v>
+        <v>173.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>8940.70</v>
+        <v>8889.31</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4727,13 +4727,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>32.000</v>
+        <v>29.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>3261.36</v>
+        <v>2955.61</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4753,13 +4753,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>45.000</v>
+        <v>51.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>1519.40</v>
+        <v>1721.99</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4805,13 +4805,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>11172.000</v>
+        <v>13105.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>43365.52</v>
+        <v>50868.90</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -5071,7 +5071,7 @@
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>56252.23</v>
+        <v>56252.24</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5091,13 +5091,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>560.000</v>
+        <v>558.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>3170.06</v>
+        <v>3158.74</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5117,13 +5117,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>261.000</v>
+        <v>351.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>2053.87</v>
+        <v>2885.88</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5195,13 +5195,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>60.000</v>
+        <v>66.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1831.37</v>
+        <v>2014.51</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5611,13 +5611,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>3.000</v>
+        <v>7.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>314.31</v>
+        <v>733.39</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5871,13 +5871,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>55.000</v>
+        <v>56.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>7342.99</v>
+        <v>7476.50</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -6209,13 +6209,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>2280.000</v>
+        <v>2473.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>42693.00</v>
+        <v>46306.92</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6235,13 +6235,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>123226.000</v>
+        <v>119121.000</v>
       </c>
       <c r="G173" t="s">
         <v>347</v>
       </c>
       <c r="H173" s="3">
-        <v>185533.15</v>
+        <v>180046.83</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6261,13 +6261,13 @@
         <v>349</v>
       </c>
       <c r="F174" s="2">
-        <v>101.000</v>
+        <v>100.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>3600.02</v>
+        <v>3564.38</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6287,13 +6287,13 @@
         <v>351</v>
       </c>
       <c r="F175" s="2">
-        <v>47.000</v>
+        <v>5.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>8992.92</v>
+        <v>956.69</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6313,13 +6313,13 @@
         <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>626.000</v>
+        <v>827.000</v>
       </c>
       <c r="G176" t="s">
         <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>109310.27</v>
+        <v>144408.28</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6417,13 +6417,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>75.000</v>
+        <v>136.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>34789.96</v>
+        <v>63085.79</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6443,13 +6443,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>37.000</v>
+        <v>52.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>2259.59</v>
+        <v>3175.64</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6475,7 +6475,7 @@
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>11677.39</v>
+        <v>11487.51</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6547,13 +6547,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>182.000</v>
+        <v>28.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>6080.43</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6573,13 +6573,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>28.000</v>
+        <v>182.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1119.31</v>
+        <v>6080.43</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6605,7 +6605,7 @@
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>6893.88</v>
+        <v>6893.89</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6651,13 +6651,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>513.000</v>
+        <v>556.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>10393.38</v>
+        <v>11264.56</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6677,13 +6677,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>43.000</v>
+        <v>47.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>998.72</v>
+        <v>1091.62</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -7691,13 +7691,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>20268.300</v>
+        <v>20174.300</v>
       </c>
       <c r="G229" t="s">
         <v>432</v>
       </c>
       <c r="H229" s="3">
-        <v>46002.35</v>
+        <v>45788.92</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7717,13 +7717,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>2783.970</v>
+        <v>2744.960</v>
       </c>
       <c r="G230" t="s">
         <v>432</v>
       </c>
       <c r="H230" s="3">
-        <v>11884.96</v>
+        <v>11718.42</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7795,13 +7795,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>0.100</v>
+        <v>539.600</v>
       </c>
       <c r="G233" t="s">
         <v>432</v>
       </c>
       <c r="H233" s="3">
-        <v>1.02</v>
+        <v>5388.40</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7821,13 +7821,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>57.800</v>
+        <v>45.800</v>
       </c>
       <c r="G234" t="s">
         <v>432</v>
       </c>
       <c r="H234" s="3">
-        <v>1294.06</v>
+        <v>1025.40</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7847,13 +7847,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>1191.970</v>
+        <v>2070.970</v>
       </c>
       <c r="G235" t="s">
         <v>432</v>
       </c>
       <c r="H235" s="3">
-        <v>37447.47</v>
+        <v>65062.53</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -8107,13 +8107,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>4996.000</v>
+        <v>5388.000</v>
       </c>
       <c r="G245" t="s">
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>12541.72</v>
+        <v>13525.79</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8185,13 +8185,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>10.000</v>
+        <v>12.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>4310.15</v>
+        <v>5172.18</v>
       </c>
     </row>
     <row r="249" spans="1:8">

</xml_diff>

<commit_message>
#fix: etapa on hidrometro material
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="535">
   <si>
     <t>4600041302</t>
   </si>
@@ -1061,12 +1061,6 @@
   </si>
   <si>
     <t>SELIM 90 G PVC DN 300 X 100 ENCAIXE</t>
-  </si>
-  <si>
-    <t>30007132</t>
-  </si>
-  <si>
-    <t>SELIM AJUST TUBO PVC E CER DN 150X100</t>
   </si>
   <si>
     <t>30003416</t>
@@ -1728,7 +1722,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H263"/>
+  <dimension ref="A1:H262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1748,28 +1742,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2855,13 +2849,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>111.000</v>
+        <v>110.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>17598.49</v>
+        <v>17439.95</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2881,13 +2875,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>74.000</v>
+        <v>71.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>41349.35</v>
+        <v>39673.02</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3115,13 +3109,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>937.000</v>
+        <v>909.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>8521.93</v>
+        <v>8267.29</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3167,13 +3161,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>2854.000</v>
+        <v>2822.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>29344.07</v>
+        <v>29015.08</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3479,13 +3473,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>1187.000</v>
+        <v>1185.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>6042.61</v>
+        <v>6032.43</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3713,13 +3707,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>81.000</v>
+        <v>79.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>1504.95</v>
+        <v>1467.79</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3791,13 +3785,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>1299.000</v>
+        <v>1289.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>7984.61</v>
+        <v>7923.13</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3817,13 +3811,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>2736.000</v>
+        <v>2705.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>71266.70</v>
+        <v>70459.14</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -4181,13 +4175,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>255.000</v>
+        <v>251.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>21667.90</v>
+        <v>21328.01</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4207,13 +4201,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>2341.000</v>
+        <v>2304.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>322461.05</v>
+        <v>317364.48</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4623,13 +4617,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>601.000</v>
+        <v>597.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>22303.61</v>
+        <v>22155.17</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4675,13 +4669,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>1037.000</v>
+        <v>1027.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>34165.86</v>
+        <v>33836.38</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4805,13 +4799,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>13105.000</v>
+        <v>13046.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>50868.90</v>
+        <v>50639.97</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -5117,13 +5111,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>351.000</v>
+        <v>347.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>2885.88</v>
+        <v>2852.99</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5279,7 +5273,7 @@
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>159.15</v>
+        <v>159.25</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -6209,13 +6203,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>2473.000</v>
+        <v>2443.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>46306.92</v>
+        <v>45745.17</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6235,13 +6229,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>119121.000</v>
+        <v>116421.000</v>
       </c>
       <c r="G173" t="s">
         <v>347</v>
       </c>
       <c r="H173" s="3">
-        <v>180046.83</v>
+        <v>175965.89</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6287,13 +6281,13 @@
         <v>351</v>
       </c>
       <c r="F175" s="2">
-        <v>5.000</v>
+        <v>820.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>956.69</v>
+        <v>143185.96</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6313,13 +6307,13 @@
         <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>827.000</v>
+        <v>13.000</v>
       </c>
       <c r="G176" t="s">
         <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>144408.28</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6339,13 +6333,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>13.000</v>
+        <v>11.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>2264.65</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6365,13 +6359,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>11.000</v>
+        <v>22.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>145.79</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6391,13 +6385,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>22.000</v>
+        <v>136.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>10363.87</v>
+        <v>63085.79</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6417,13 +6411,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>136.000</v>
+        <v>52.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>63085.79</v>
+        <v>3175.64</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6443,13 +6437,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>52.000</v>
+        <v>80.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>3175.64</v>
+        <v>11487.51</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6469,13 +6463,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>80.000</v>
+        <v>1.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>11487.51</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6501,7 +6495,7 @@
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>1218.18</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6521,13 +6515,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>1.000</v>
+        <v>28.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>1720.00</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6547,13 +6541,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>28.000</v>
+        <v>182.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>1119.31</v>
+        <v>6080.43</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6573,13 +6567,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>182.000</v>
+        <v>441.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>6080.43</v>
+        <v>6893.90</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6599,13 +6593,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>441.000</v>
+        <v>59.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>6893.89</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6625,13 +6619,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>59.000</v>
+        <v>529.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>1003.06</v>
+        <v>10717.54</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6651,13 +6645,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>556.000</v>
+        <v>47.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>11264.56</v>
+        <v>1091.62</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6677,13 +6671,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>47.000</v>
+        <v>93.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>1091.62</v>
+        <v>6626.71</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6703,13 +6697,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>93.000</v>
+        <v>16.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>6626.71</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6729,13 +6723,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>16.000</v>
+        <v>1.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>1789.69</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6755,13 +6749,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>189.22</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6781,13 +6775,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>19.000</v>
+        <v>244.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>1201.67</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6807,13 +6801,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>244.000</v>
+        <v>2.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>16895.78</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6833,13 +6827,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>651.09</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6859,13 +6853,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>1125.55</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6885,13 +6879,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>718.30</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6917,7 +6911,7 @@
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>266.26</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6937,13 +6931,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>257.36</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6963,13 +6957,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>961.64</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -6989,13 +6983,13 @@
         <v>405</v>
       </c>
       <c r="F202" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G202" t="s">
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>726.22</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7015,13 +7009,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>662.53</v>
+        <v>493.11</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7041,13 +7035,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>493.11</v>
+        <v>885.89</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7067,13 +7061,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>7.000</v>
+        <v>37.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>885.89</v>
+        <v>5096.66</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7093,13 +7087,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>37.000</v>
+        <v>1.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>5096.66</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7125,7 +7119,7 @@
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>4700.00</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7145,13 +7139,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>1.000</v>
+        <v>38.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>8560.17</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7171,13 +7165,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>38.000</v>
+        <v>1.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>481.25</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7197,13 +7191,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>1.000</v>
+        <v>17.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>23.34</v>
+        <v>646.00</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7223,13 +7217,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>17.000</v>
+        <v>24.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>646.00</v>
+        <v>1584.75</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7249,13 +7243,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>24.000</v>
+        <v>1.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>1584.75</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7275,13 +7269,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>685.11</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7301,13 +7295,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>2.000</v>
+        <v>4.800</v>
       </c>
       <c r="G214" t="s">
-        <v>5</v>
+        <v>430</v>
       </c>
       <c r="H214" s="3">
-        <v>8149.76</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7321,19 +7315,19 @@
         <v>2</v>
       </c>
       <c r="D215" t="s">
+        <v>431</v>
+      </c>
+      <c r="E215" t="s">
+        <v>432</v>
+      </c>
+      <c r="F215" s="2">
+        <v>16.000</v>
+      </c>
+      <c r="G215" t="s">
         <v>430</v>
       </c>
-      <c r="E215" t="s">
-        <v>431</v>
-      </c>
-      <c r="F215" s="2">
-        <v>4.800</v>
-      </c>
-      <c r="G215" t="s">
-        <v>432</v>
-      </c>
       <c r="H215" s="3">
-        <v>1822.34</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7353,13 +7347,13 @@
         <v>434</v>
       </c>
       <c r="F216" s="2">
-        <v>16.000</v>
+        <v>17.000</v>
       </c>
       <c r="G216" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H216" s="3">
-        <v>7011.29</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7379,13 +7373,13 @@
         <v>436</v>
       </c>
       <c r="F217" s="2">
-        <v>17.000</v>
+        <v>162.140</v>
       </c>
       <c r="G217" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H217" s="3">
-        <v>2938.94</v>
+        <v>35221.32</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7405,13 +7399,13 @@
         <v>438</v>
       </c>
       <c r="F218" s="2">
-        <v>162.140</v>
+        <v>1.090</v>
       </c>
       <c r="G218" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H218" s="3">
-        <v>35221.32</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7431,13 +7425,13 @@
         <v>440</v>
       </c>
       <c r="F219" s="2">
-        <v>1.090</v>
+        <v>20.300</v>
       </c>
       <c r="G219" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H219" s="3">
-        <v>250.66</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7457,13 +7451,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>20.300</v>
+        <v>13.000</v>
       </c>
       <c r="G220" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H220" s="3">
-        <v>6816.84</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7483,13 +7477,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>13.000</v>
+        <v>22.000</v>
       </c>
       <c r="G221" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H221" s="3">
-        <v>3437.72</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7509,13 +7503,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>22.000</v>
+        <v>343.600</v>
       </c>
       <c r="G222" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H222" s="3">
-        <v>2084.93</v>
+        <v>3442.91</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7535,13 +7529,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>343.600</v>
+        <v>0.360</v>
       </c>
       <c r="G223" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H223" s="3">
-        <v>3442.91</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7561,13 +7555,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>0.360</v>
+        <v>11.000</v>
       </c>
       <c r="G224" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H224" s="3">
-        <v>7.79</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7587,13 +7581,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>11.000</v>
+        <v>84.000</v>
       </c>
       <c r="G225" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H225" s="3">
-        <v>974.64</v>
+        <v>13440.76</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7613,13 +7607,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>84.000</v>
+        <v>168.620</v>
       </c>
       <c r="G226" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H226" s="3">
-        <v>13440.76</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7639,13 +7633,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>168.620</v>
+        <v>47.250</v>
       </c>
       <c r="G227" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H227" s="3">
-        <v>8798.84</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7665,13 +7659,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>47.250</v>
+        <v>19831.300</v>
       </c>
       <c r="G228" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H228" s="3">
-        <v>5148.59</v>
+        <v>45010.41</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7691,13 +7685,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>20174.300</v>
+        <v>2744.960</v>
       </c>
       <c r="G229" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H229" s="3">
-        <v>45788.92</v>
+        <v>11718.42</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7717,13 +7711,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>2744.960</v>
+        <v>29.390</v>
       </c>
       <c r="G230" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H230" s="3">
-        <v>11718.42</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7743,13 +7737,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>29.390</v>
+        <v>856.370</v>
       </c>
       <c r="G231" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H231" s="3">
-        <v>15217.18</v>
+        <v>32198.67</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7769,13 +7763,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>856.370</v>
+        <v>472.600</v>
       </c>
       <c r="G232" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H232" s="3">
-        <v>32198.67</v>
+        <v>4719.34</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7795,13 +7789,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>539.600</v>
+        <v>45.800</v>
       </c>
       <c r="G233" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H233" s="3">
-        <v>5388.40</v>
+        <v>1025.40</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7821,13 +7815,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>45.800</v>
+        <v>2070.970</v>
       </c>
       <c r="G234" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H234" s="3">
-        <v>1025.40</v>
+        <v>65062.53</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7847,13 +7841,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>2070.970</v>
+        <v>270.420</v>
       </c>
       <c r="G235" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H235" s="3">
-        <v>65062.53</v>
+        <v>24811.50</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7873,13 +7867,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>270.420</v>
+        <v>59.100</v>
       </c>
       <c r="G236" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H236" s="3">
-        <v>24811.50</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7899,13 +7893,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>59.100</v>
+        <v>237.900</v>
       </c>
       <c r="G237" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H237" s="3">
-        <v>9271.17</v>
+        <v>7688.51</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7925,13 +7919,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>237.900</v>
+        <v>91.020</v>
       </c>
       <c r="G238" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H238" s="3">
-        <v>7688.51</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7951,13 +7945,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>91.020</v>
+        <v>0.690</v>
       </c>
       <c r="G239" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H239" s="3">
-        <v>1685.63</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7977,13 +7971,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>0.690</v>
+        <v>48.790</v>
       </c>
       <c r="G240" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H240" s="3">
-        <v>20.12</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8003,13 +7997,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>48.790</v>
+        <v>78.310</v>
       </c>
       <c r="G241" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H241" s="3">
-        <v>1048.10</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8029,13 +8023,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>78.310</v>
+        <v>216.000</v>
       </c>
       <c r="G242" t="s">
-        <v>432</v>
+        <v>5</v>
       </c>
       <c r="H242" s="3">
-        <v>7083.14</v>
+        <v>1264.68</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8055,13 +8049,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>216.000</v>
+        <v>73.000</v>
       </c>
       <c r="G243" t="s">
         <v>5</v>
       </c>
       <c r="H243" s="3">
-        <v>1264.68</v>
+        <v>402.15</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8081,13 +8075,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>73.000</v>
+        <v>5380.000</v>
       </c>
       <c r="G244" t="s">
         <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>402.15</v>
+        <v>13505.71</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8107,13 +8101,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>5388.000</v>
+        <v>8.000</v>
       </c>
       <c r="G245" t="s">
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>13525.79</v>
+        <v>2847.85</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8133,13 +8127,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>8.000</v>
+        <v>6.000</v>
       </c>
       <c r="G246" t="s">
         <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>2847.85</v>
+        <v>3340.44</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8159,13 +8153,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>6.000</v>
+        <v>12.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>3340.44</v>
+        <v>5172.18</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8185,13 +8179,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>5172.18</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8211,13 +8205,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>2371.80</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8237,13 +8231,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>2323.99</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8269,7 +8263,7 @@
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>1462.82</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8289,13 +8283,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>6585.02</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8315,13 +8309,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>6.000</v>
+        <v>45.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>1694.29</v>
+        <v>20798.75</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8341,13 +8335,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>45.000</v>
+        <v>8.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>20798.75</v>
+        <v>4529.21</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8367,13 +8361,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>4529.21</v>
+        <v>1721.73</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8393,13 +8387,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>1721.73</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8419,13 +8413,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>6821.40</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8445,13 +8439,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>7220.40</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8471,13 +8465,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>7.000</v>
+        <v>17.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>2566.22</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8497,13 +8491,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>17.000</v>
+        <v>7.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>7823.48</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8523,13 +8517,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>7.000</v>
+        <v>5.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>3943.24</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8549,38 +8543,12 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="263" spans="1:8">
-      <c r="A263" t="s">
-        <v>0</v>
-      </c>
-      <c r="B263" t="s">
-        <v>1</v>
-      </c>
-      <c r="C263" t="s">
-        <v>2</v>
-      </c>
-      <c r="D263" t="s">
-        <v>527</v>
-      </c>
-      <c r="E263" t="s">
-        <v>528</v>
-      </c>
-      <c r="F263" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G263" t="s">
-        <v>5</v>
-      </c>
-      <c r="H263" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: start sessions on rust
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -67,12 +67,6 @@
     <t>ABRACADEIRA FF REPARO TUBO DN50 LMIN=150</t>
   </si>
   <si>
-    <t>30001122</t>
-  </si>
-  <si>
-    <t>ABRACADEIRA FF REPARO TUBO DN75 LMIN=150</t>
-  </si>
-  <si>
     <t>30000153</t>
   </si>
   <si>
@@ -491,6 +485,12 @@
   </si>
   <si>
     <t>CURVA 90GR PVC PB ESG DN100 CTA JEI/JERI</t>
+  </si>
+  <si>
+    <t>50000021</t>
+  </si>
+  <si>
+    <t>DISPOSITIVO MED METAL  DN 20</t>
   </si>
   <si>
     <t>50000178</t>
@@ -1965,13 +1965,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>2565.46</v>
+        <v>1582.95</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1991,13 +1991,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="2">
-        <v>8.000</v>
+        <v>3.000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
-        <v>1582.95</v>
+        <v>750.47</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2017,13 +2017,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>750.47</v>
+        <v>153.40</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2043,13 +2043,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>1.000</v>
+        <v>15.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>153.40</v>
+        <v>313.91</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2069,13 +2069,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2">
-        <v>15.000</v>
+        <v>9.000</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>313.91</v>
+        <v>878.23</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2095,13 +2095,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>9.000</v>
+        <v>19.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>878.23</v>
+        <v>723.49</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2121,13 +2121,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="2">
-        <v>19.000</v>
+        <v>147.000</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>723.49</v>
+        <v>13914.19</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2147,13 +2147,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>147.000</v>
+        <v>18.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>13914.19</v>
+        <v>78.03</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2173,13 +2173,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>18.000</v>
+        <v>620.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>78.03</v>
+        <v>1271.00</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2199,13 +2199,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>622.000</v>
+        <v>447.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>1275.10</v>
+        <v>326.45</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2225,13 +2225,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="2">
-        <v>447.000</v>
+        <v>98.000</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>326.45</v>
+        <v>125.14</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2251,13 +2251,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>98.000</v>
+        <v>136.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>125.14</v>
+        <v>607.32</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2277,13 +2277,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>136.000</v>
+        <v>60.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>607.32</v>
+        <v>227.27</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2303,13 +2303,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>60.000</v>
+        <v>4.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>227.27</v>
+        <v>48.64</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2329,13 +2329,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>4.000</v>
+        <v>11.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>48.64</v>
+        <v>6222.91</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2355,13 +2355,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>11.000</v>
+        <v>324.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>6222.91</v>
+        <v>27666.50</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2381,13 +2381,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>324.000</v>
+        <v>113.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>27666.50</v>
+        <v>20496.57</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2407,13 +2407,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>113.000</v>
+        <v>9.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>20496.57</v>
+        <v>380.14</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2433,13 +2433,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>380.14</v>
+        <v>61.38</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2459,13 +2459,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>61.38</v>
+        <v>103.20</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2485,13 +2485,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>103.20</v>
+        <v>197.65</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2511,13 +2511,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>197.65</v>
+        <v>463.99</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2537,13 +2537,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>463.99</v>
+        <v>542.21</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2563,13 +2563,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>2.000</v>
+        <v>10.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>542.21</v>
+        <v>201.79</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2589,13 +2589,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>10.000</v>
+        <v>8.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>201.79</v>
+        <v>460.48</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2615,13 +2615,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>8.000</v>
+        <v>13.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>460.48</v>
+        <v>526.30</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2641,13 +2641,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>13.000</v>
+        <v>14.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>526.30</v>
+        <v>630.14</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2667,13 +2667,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>14.000</v>
+        <v>16.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>630.14</v>
+        <v>520.62</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2693,13 +2693,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>16.000</v>
+        <v>13.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>520.62</v>
+        <v>726.80</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2719,13 +2719,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>13.000</v>
+        <v>1.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>726.80</v>
+        <v>17.78</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2745,13 +2745,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>1.000</v>
+        <v>122.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>17.78</v>
+        <v>5730.92</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2771,13 +2771,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>105.000</v>
+        <v>1.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>4932.35</v>
+        <v>1940.18</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2797,13 +2797,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>1.000</v>
+        <v>243.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>1940.18</v>
+        <v>5819.14</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2823,13 +2823,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>234.000</v>
+        <v>110.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>5603.63</v>
+        <v>17439.95</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2849,13 +2849,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>110.000</v>
+        <v>61.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>17439.95</v>
+        <v>34085.27</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2875,13 +2875,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>70.000</v>
+        <v>46.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>39114.25</v>
+        <v>2898.44</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2901,13 +2901,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>46.000</v>
+        <v>2.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>2898.44</v>
+        <v>603.23</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2927,13 +2927,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>2.000</v>
+        <v>14.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>603.23</v>
+        <v>1963.52</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2953,13 +2953,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>15.000</v>
+        <v>9.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>2103.77</v>
+        <v>1883.67</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2979,13 +2979,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>9.000</v>
+        <v>8.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>1883.67</v>
+        <v>2352.96</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3005,13 +3005,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>8.000</v>
+        <v>9.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>2352.96</v>
+        <v>3592.71</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3031,13 +3031,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>3592.71</v>
+        <v>863.17</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3057,13 +3057,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>863.17</v>
+        <v>295.57</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3083,13 +3083,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>3.000</v>
+        <v>754.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>295.57</v>
+        <v>6857.63</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3109,13 +3109,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>881.000</v>
+        <v>38.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>8012.67</v>
+        <v>609.12</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3135,13 +3135,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>40.000</v>
+        <v>2729.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>641.18</v>
+        <v>28058.98</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3161,13 +3161,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>2817.000</v>
+        <v>11.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>28963.69</v>
+        <v>380.69</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3187,13 +3187,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>11.000</v>
+        <v>9.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>380.69</v>
+        <v>334.55</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3213,13 +3213,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>9.000</v>
+        <v>5.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>334.55</v>
+        <v>1454.70</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3239,13 +3239,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>5.000</v>
+        <v>23.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>1454.70</v>
+        <v>1071.88</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3265,13 +3265,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>23.000</v>
+        <v>11.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>1071.88</v>
+        <v>1357.53</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3291,13 +3291,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>11.000</v>
+        <v>16.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>1357.53</v>
+        <v>902.16</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3317,13 +3317,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>16.000</v>
+        <v>28.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>902.16</v>
+        <v>2209.27</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3343,13 +3343,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>28.000</v>
+        <v>14.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>2209.27</v>
+        <v>416.43</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3369,13 +3369,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>14.000</v>
+        <v>36.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>416.43</v>
+        <v>2051.36</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3395,13 +3395,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>37.000</v>
+        <v>4.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>2108.34</v>
+        <v>606.42</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3421,13 +3421,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>606.42</v>
+        <v>1448.47</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3447,13 +3447,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>1.000</v>
+        <v>1197.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>1448.47</v>
+        <v>6093.54</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3473,13 +3473,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>1185.000</v>
+        <v>23.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>6032.43</v>
+        <v>1396.09</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3499,13 +3499,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>23.000</v>
+        <v>42.000</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>1359.47</v>
+        <v>6244.14</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3525,13 +3525,13 @@
         <v>139</v>
       </c>
       <c r="F69" s="2">
-        <v>42.000</v>
+        <v>180.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>5269.67</v>
+        <v>1598.50</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3551,13 +3551,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>180.000</v>
+        <v>13.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>1598.50</v>
+        <v>738.14</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3577,13 +3577,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>13.000</v>
+        <v>6.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>738.14</v>
+        <v>344.01</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3603,13 +3603,13 @@
         <v>145</v>
       </c>
       <c r="F72" s="2">
-        <v>6.000</v>
+        <v>5.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>344.01</v>
+        <v>507.80</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3629,13 +3629,13 @@
         <v>147</v>
       </c>
       <c r="F73" s="2">
-        <v>5.000</v>
+        <v>47.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>507.80</v>
+        <v>4841.34</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3655,13 +3655,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>47.000</v>
+        <v>2.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>4841.34</v>
+        <v>495.95</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3681,13 +3681,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>2.000</v>
+        <v>79.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>495.95</v>
+        <v>1467.79</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3707,13 +3707,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>79.000</v>
+        <v>1.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>1467.79</v>
+        <v>131.57</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3739,7 +3739,7 @@
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>131.57</v>
+        <v>86.93</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3759,13 +3759,13 @@
         <v>157</v>
       </c>
       <c r="F78" s="2">
-        <v>1.000</v>
+        <v>1358.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>86.93</v>
+        <v>8347.22</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3785,13 +3785,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>1286.000</v>
+        <v>13.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>7904.69</v>
+        <v>1024.36</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3811,13 +3811,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>2686.000</v>
+        <v>2730.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>69964.20</v>
+        <v>71110.22</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -4175,13 +4175,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>248.000</v>
+        <v>254.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>21073.10</v>
+        <v>21582.93</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4201,13 +4201,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>2257.000</v>
+        <v>2158.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>310890.47</v>
+        <v>297253.71</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4357,13 +4357,13 @@
         <v>203</v>
       </c>
       <c r="F101" s="2">
-        <v>3.000</v>
+        <v>5.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>1127.59</v>
+        <v>1879.31</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4617,13 +4617,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>597.000</v>
+        <v>607.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>22155.17</v>
+        <v>22526.28</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4643,13 +4643,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>340.000</v>
+        <v>342.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>22225.34</v>
+        <v>22356.08</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4669,13 +4669,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>1024.000</v>
+        <v>1113.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>33737.53</v>
+        <v>36669.80</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4695,13 +4695,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>173.000</v>
+        <v>174.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>8889.31</v>
+        <v>8940.70</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4721,13 +4721,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>29.000</v>
+        <v>33.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>2955.61</v>
+        <v>3363.28</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4799,13 +4799,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>12912.000</v>
+        <v>13154.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>50120.00</v>
+        <v>51059.50</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -5111,13 +5111,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>347.000</v>
+        <v>388.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>2852.99</v>
+        <v>3190.09</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5845,7 +5845,7 @@
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>3371.47</v>
+        <v>3473.41</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5871,7 +5871,7 @@
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>7476.50</v>
+        <v>7476.95</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -6203,13 +6203,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>2441.000</v>
+        <v>2402.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>45707.72</v>
+        <v>44977.45</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6229,13 +6229,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>115306.000</v>
+        <v>114886.000</v>
       </c>
       <c r="G173" t="s">
         <v>347</v>
       </c>
       <c r="H173" s="3">
-        <v>174280.60</v>
+        <v>173645.16</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6281,13 +6281,13 @@
         <v>351</v>
       </c>
       <c r="F175" s="2">
-        <v>817.000</v>
+        <v>798.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>142662.11</v>
+        <v>139344.38</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6391,7 +6391,7 @@
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>60302.59</v>
+        <v>60302.57</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6443,7 +6443,7 @@
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>11487.51</v>
+        <v>11488.53</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6573,7 +6573,7 @@
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>6893.90</v>
+        <v>6893.91</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6619,13 +6619,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>529.000</v>
+        <v>568.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>10717.54</v>
+        <v>11507.68</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -7015,7 +7015,7 @@
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>493.11</v>
+        <v>537.99</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7041,7 +7041,7 @@
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>885.89</v>
+        <v>909.52</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7067,7 +7067,7 @@
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>5096.66</v>
+        <v>5149.09</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7191,13 +7191,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>17.000</v>
+        <v>18.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>646.00</v>
+        <v>684.00</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7217,13 +7217,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>24.000</v>
+        <v>23.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>1584.75</v>
+        <v>1518.72</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7659,13 +7659,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>19804.300</v>
+        <v>19302.800</v>
       </c>
       <c r="G228" t="s">
         <v>430</v>
       </c>
       <c r="H228" s="3">
-        <v>44949.12</v>
+        <v>43815.85</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7685,13 +7685,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>2744.960</v>
+        <v>2724.960</v>
       </c>
       <c r="G229" t="s">
         <v>430</v>
       </c>
       <c r="H229" s="3">
-        <v>11718.42</v>
+        <v>11633.04</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7763,13 +7763,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>455.600</v>
+        <v>351.100</v>
       </c>
       <c r="G232" t="s">
         <v>430</v>
       </c>
       <c r="H232" s="3">
-        <v>4549.58</v>
+        <v>3506.07</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7815,13 +7815,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>2070.970</v>
+        <v>2063.970</v>
       </c>
       <c r="G234" t="s">
         <v>430</v>
       </c>
       <c r="H234" s="3">
-        <v>65062.53</v>
+        <v>64842.62</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -8023,13 +8023,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>216.000</v>
+        <v>207.000</v>
       </c>
       <c r="G242" t="s">
         <v>5</v>
       </c>
       <c r="H242" s="3">
-        <v>1264.68</v>
+        <v>1211.99</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8075,13 +8075,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>5368.000</v>
+        <v>5384.000</v>
       </c>
       <c r="G244" t="s">
         <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>13475.59</v>
+        <v>13515.77</v>
       </c>
     </row>
     <row r="245" spans="1:8">

</xml_diff>

<commit_message>
Set material for Rede agua
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -2789,13 +2789,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>118.000</v>
+        <v>117.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>5543.03</v>
+        <v>5496.05</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2847,7 +2847,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>6914.89</v>
+        <v>6914.88</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2893,13 +2893,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>50.000</v>
+        <v>49.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>27938.75</v>
+        <v>27379.98</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3153,13 +3153,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>720.000</v>
+        <v>716.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>6548.40</v>
+        <v>6512.02</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3205,13 +3205,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>2709.000</v>
+        <v>2707.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>27853.38</v>
+        <v>27832.83</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3523,7 +3523,7 @@
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>6017.22</v>
+        <v>6017.23</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3829,13 +3829,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>1259.000</v>
+        <v>1255.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>7738.61</v>
+        <v>7714.01</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3881,13 +3881,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>2670.000</v>
+        <v>2646.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>69547.21</v>
+        <v>68922.04</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -4245,13 +4245,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>249.000</v>
+        <v>248.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>21078.22</v>
+        <v>20993.57</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4271,13 +4271,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>2099.000</v>
+        <v>2082.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>289126.75</v>
+        <v>286785.09</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4687,13 +4687,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>597.000</v>
+        <v>596.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>22155.17</v>
+        <v>22118.06</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4739,13 +4739,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>1054.000</v>
+        <v>1051.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>34725.87</v>
+        <v>34627.03</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4869,13 +4869,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>12909.000</v>
+        <v>12877.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>50108.68</v>
+        <v>49984.49</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -6273,13 +6273,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>2456.000</v>
+        <v>2454.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>45988.60</v>
+        <v>45951.15</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6299,13 +6299,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>109786.000</v>
+        <v>109836.000</v>
       </c>
       <c r="G175" t="s">
         <v>351</v>
       </c>
       <c r="H175" s="3">
-        <v>166078.73</v>
+        <v>166154.32</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6377,13 +6377,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>780.000</v>
+        <v>775.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>136201.24</v>
+        <v>135328.15</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6481,13 +6481,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>130.000</v>
+        <v>126.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>60302.55</v>
+        <v>58447.08</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6669,7 +6669,7 @@
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>6893.92</v>
+        <v>6893.93</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -7755,13 +7755,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>20019.800</v>
+        <v>20012.800</v>
       </c>
       <c r="G231" t="s">
         <v>436</v>
       </c>
       <c r="H231" s="3">
-        <v>45430.85</v>
+        <v>45414.96</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7859,13 +7859,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>345.600</v>
+        <v>325.600</v>
       </c>
       <c r="G235" t="s">
         <v>436</v>
       </c>
       <c r="H235" s="3">
-        <v>3448.80</v>
+        <v>3249.21</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -8125,7 +8125,7 @@
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>1188.57</v>
+        <v>1188.56</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8171,13 +8171,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>5372.000</v>
+        <v>5364.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>13485.65</v>
+        <v>13465.57</v>
       </c>
     </row>
     <row r="248" spans="1:8">

</xml_diff>

<commit_message>
#fix: item cod for troca cv por uma novasp
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="541">
   <si>
     <t>4600041302</t>
   </si>
@@ -509,12 +509,6 @@
   </si>
   <si>
     <t>CURVA PVC 45GR LG PB JEI/JERI ESG DN100</t>
-  </si>
-  <si>
-    <t>50000021</t>
-  </si>
-  <si>
-    <t>DISPOSITIVO MED METAL  DN 20</t>
   </si>
   <si>
     <t>50000178</t>
@@ -1746,7 +1740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H266"/>
+  <dimension ref="A1:H265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,28 +1760,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>541</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1989,13 +1983,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>36.000</v>
+        <v>1.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>14916.97</v>
+        <v>427.58</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2905,7 +2899,7 @@
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>22909.78</v>
+        <v>22909.77</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2951,13 +2945,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>80.000</v>
+        <v>79.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>15195.71</v>
+        <v>15005.76</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3185,13 +3179,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>674.000</v>
+        <v>670.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>6116.27</v>
+        <v>6079.98</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3211,13 +3205,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>38.000</v>
+        <v>37.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>609.12</v>
+        <v>593.09</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3237,13 +3231,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3170.000</v>
+        <v>3166.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>32581.38</v>
+        <v>32540.26</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3913,13 +3907,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>1.000</v>
+        <v>2888.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>78.80</v>
+        <v>75225.39</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3939,13 +3933,13 @@
         <v>169</v>
       </c>
       <c r="F84" s="2">
-        <v>2892.000</v>
+        <v>5.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>75329.60</v>
+        <v>383.07</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3965,13 +3959,13 @@
         <v>171</v>
       </c>
       <c r="F85" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G85" t="s">
         <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>383.07</v>
+        <v>651.71</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3997,7 +3991,7 @@
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>651.71</v>
+        <v>1263.43</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4017,13 +4011,13 @@
         <v>175</v>
       </c>
       <c r="F87" s="2">
-        <v>3.000</v>
+        <v>12.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>1263.43</v>
+        <v>2226.44</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4043,13 +4037,13 @@
         <v>177</v>
       </c>
       <c r="F88" s="2">
-        <v>12.000</v>
+        <v>4.000</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>2226.44</v>
+        <v>1008.05</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4069,13 +4063,13 @@
         <v>179</v>
       </c>
       <c r="F89" s="2">
-        <v>4.000</v>
+        <v>14.000</v>
       </c>
       <c r="G89" t="s">
         <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>1008.05</v>
+        <v>1572.64</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4095,13 +4089,13 @@
         <v>181</v>
       </c>
       <c r="F90" s="2">
-        <v>14.000</v>
+        <v>10.000</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>1572.64</v>
+        <v>4255.32</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4121,13 +4115,13 @@
         <v>183</v>
       </c>
       <c r="F91" s="2">
-        <v>10.000</v>
+        <v>2.000</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>4255.32</v>
+        <v>3671.99</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -4147,13 +4141,13 @@
         <v>185</v>
       </c>
       <c r="F92" s="2">
-        <v>2.000</v>
+        <v>136.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>3671.99</v>
+        <v>5126.52</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -4173,13 +4167,13 @@
         <v>187</v>
       </c>
       <c r="F93" s="2">
-        <v>136.000</v>
+        <v>2.000</v>
       </c>
       <c r="G93" t="s">
         <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>5126.52</v>
+        <v>560.27</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -4199,13 +4193,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>2.000</v>
+        <v>36.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>560.27</v>
+        <v>3294.45</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4225,13 +4219,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>36.000</v>
+        <v>1.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>3294.45</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4251,13 +4245,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>1.000</v>
+        <v>10.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>2.97</v>
+        <v>18133.05</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4277,13 +4271,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>10.000</v>
+        <v>247.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>18133.05</v>
+        <v>20909.00</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4303,13 +4297,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>247.000</v>
+        <v>2035.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>20909.00</v>
+        <v>286174.81</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4329,13 +4323,13 @@
         <v>199</v>
       </c>
       <c r="F99" s="2">
-        <v>2042.000</v>
+        <v>1.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>287159.22</v>
+        <v>2980.59</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4361,7 +4355,7 @@
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>2980.59</v>
+        <v>4463.84</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4381,13 +4375,13 @@
         <v>203</v>
       </c>
       <c r="F101" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>4463.84</v>
+        <v>1598.31</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4407,13 +4401,13 @@
         <v>205</v>
       </c>
       <c r="F102" s="2">
-        <v>3.000</v>
+        <v>19.000</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>1598.31</v>
+        <v>23432.75</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4433,13 +4427,13 @@
         <v>207</v>
       </c>
       <c r="F103" s="2">
-        <v>19.000</v>
+        <v>7.000</v>
       </c>
       <c r="G103" t="s">
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>23432.75</v>
+        <v>13115.50</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4459,13 +4453,13 @@
         <v>209</v>
       </c>
       <c r="F104" s="2">
-        <v>7.000</v>
+        <v>5.000</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>13115.50</v>
+        <v>1877.21</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4485,13 +4479,13 @@
         <v>211</v>
       </c>
       <c r="F105" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G105" t="s">
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>1877.21</v>
+        <v>279.59</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -4511,13 +4505,13 @@
         <v>213</v>
       </c>
       <c r="F106" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G106" t="s">
         <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>279.59</v>
+        <v>740.97</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -4543,7 +4537,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>740.97</v>
+        <v>902.80</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4569,7 +4563,7 @@
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>902.80</v>
+        <v>994.54</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4595,7 +4589,7 @@
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>994.54</v>
+        <v>1033.65</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4621,7 +4615,7 @@
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>1033.65</v>
+        <v>1166.57</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4641,13 +4635,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>1166.57</v>
+        <v>2825.06</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4667,13 +4661,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>2825.06</v>
+        <v>91.20</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4693,13 +4687,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>91.20</v>
+        <v>719.47</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4719,13 +4713,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>2.000</v>
+        <v>629.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>719.47</v>
+        <v>23342.73</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4745,13 +4739,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>629.000</v>
+        <v>347.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>23342.73</v>
+        <v>22682.92</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4771,13 +4765,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>347.000</v>
+        <v>1010.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>22682.92</v>
+        <v>33276.11</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4797,13 +4791,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>1010.000</v>
+        <v>171.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>33276.11</v>
+        <v>8786.55</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4823,13 +4817,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>171.000</v>
+        <v>25.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>8786.55</v>
+        <v>2547.94</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4849,13 +4843,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>25.000</v>
+        <v>49.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>2547.94</v>
+        <v>1654.46</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4875,13 +4869,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>49.000</v>
+        <v>9.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>1654.46</v>
+        <v>1675.75</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4901,13 +4895,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>9.000</v>
+        <v>12688.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>1675.75</v>
+        <v>49251.06</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4927,13 +4921,13 @@
         <v>245</v>
       </c>
       <c r="F122" s="2">
-        <v>12725.000</v>
+        <v>2.000</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>49394.65</v>
+        <v>2463.85</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4959,7 +4953,7 @@
         <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>2463.85</v>
+        <v>4533.88</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4979,13 +4973,13 @@
         <v>249</v>
       </c>
       <c r="F124" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>4533.88</v>
+        <v>6385.34</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -5005,13 +4999,13 @@
         <v>251</v>
       </c>
       <c r="F125" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G125" t="s">
         <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>6385.34</v>
+        <v>12368.67</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5031,13 +5025,13 @@
         <v>253</v>
       </c>
       <c r="F126" s="2">
-        <v>6.000</v>
+        <v>3.000</v>
       </c>
       <c r="G126" t="s">
         <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>12368.67</v>
+        <v>3260.53</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5057,13 +5051,13 @@
         <v>255</v>
       </c>
       <c r="F127" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G127" t="s">
         <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>3260.53</v>
+        <v>3527.49</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -5083,13 +5077,13 @@
         <v>257</v>
       </c>
       <c r="F128" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>3527.49</v>
+        <v>6294.26</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5109,13 +5103,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>6294.26</v>
+        <v>4585.00</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5135,13 +5129,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>4585.00</v>
+        <v>14225.45</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5161,13 +5155,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>2.000</v>
+        <v>39.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>14225.45</v>
+        <v>56252.24</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5187,13 +5181,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>39.000</v>
+        <v>556.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>56252.24</v>
+        <v>3147.42</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5213,13 +5207,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>556.000</v>
+        <v>297.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>3147.42</v>
+        <v>2441.91</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5239,13 +5233,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>297.000</v>
+        <v>91.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>2441.91</v>
+        <v>1426.69</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5265,13 +5259,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>91.000</v>
+        <v>110.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>1426.69</v>
+        <v>1499.69</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5291,13 +5285,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>110.000</v>
+        <v>80.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>1499.69</v>
+        <v>2441.82</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5317,13 +5311,13 @@
         <v>275</v>
       </c>
       <c r="F137" s="2">
-        <v>80.000</v>
+        <v>26.000</v>
       </c>
       <c r="G137" t="s">
         <v>5</v>
       </c>
       <c r="H137" s="3">
-        <v>2441.82</v>
+        <v>3249.51</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5343,13 +5337,13 @@
         <v>277</v>
       </c>
       <c r="F138" s="2">
-        <v>26.000</v>
+        <v>1.000</v>
       </c>
       <c r="G138" t="s">
         <v>5</v>
       </c>
       <c r="H138" s="3">
-        <v>3249.51</v>
+        <v>194.13</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5369,13 +5363,13 @@
         <v>279</v>
       </c>
       <c r="F139" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G139" t="s">
         <v>5</v>
       </c>
       <c r="H139" s="3">
-        <v>194.13</v>
+        <v>159.25</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5401,7 +5395,7 @@
         <v>5</v>
       </c>
       <c r="H140" s="3">
-        <v>159.25</v>
+        <v>499.74</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5421,13 +5415,13 @@
         <v>283</v>
       </c>
       <c r="F141" s="2">
-        <v>2.000</v>
+        <v>41.000</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
       </c>
       <c r="H141" s="3">
-        <v>499.74</v>
+        <v>2975.17</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5447,13 +5441,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="2">
-        <v>41.000</v>
+        <v>12.000</v>
       </c>
       <c r="G142" t="s">
         <v>5</v>
       </c>
       <c r="H142" s="3">
-        <v>2975.17</v>
+        <v>1826.75</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5479,7 +5473,7 @@
         <v>5</v>
       </c>
       <c r="H143" s="3">
-        <v>1826.75</v>
+        <v>5671.40</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5499,13 +5493,13 @@
         <v>289</v>
       </c>
       <c r="F144" s="2">
-        <v>12.000</v>
+        <v>8.000</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
       </c>
       <c r="H144" s="3">
-        <v>5671.40</v>
+        <v>5567.25</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5525,13 +5519,13 @@
         <v>291</v>
       </c>
       <c r="F145" s="2">
-        <v>8.000</v>
+        <v>6.000</v>
       </c>
       <c r="G145" t="s">
         <v>5</v>
       </c>
       <c r="H145" s="3">
-        <v>5567.25</v>
+        <v>5624.37</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5551,13 +5545,13 @@
         <v>293</v>
       </c>
       <c r="F146" s="2">
-        <v>6.000</v>
+        <v>5.000</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
       </c>
       <c r="H146" s="3">
-        <v>5624.37</v>
+        <v>5802.02</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5577,13 +5571,13 @@
         <v>295</v>
       </c>
       <c r="F147" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
       </c>
       <c r="H147" s="3">
-        <v>5802.02</v>
+        <v>6826.78</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5603,13 +5597,13 @@
         <v>297</v>
       </c>
       <c r="F148" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
       </c>
       <c r="H148" s="3">
-        <v>6826.78</v>
+        <v>1690.54</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5629,13 +5623,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>5.000</v>
+        <v>4.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>1690.54</v>
+        <v>1094.94</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5655,13 +5649,13 @@
         <v>301</v>
       </c>
       <c r="F150" s="2">
-        <v>4.000</v>
+        <v>16.000</v>
       </c>
       <c r="G150" t="s">
         <v>5</v>
       </c>
       <c r="H150" s="3">
-        <v>1094.94</v>
+        <v>4737.64</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5681,13 +5675,13 @@
         <v>303</v>
       </c>
       <c r="F151" s="2">
-        <v>16.000</v>
+        <v>3.000</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
       </c>
       <c r="H151" s="3">
-        <v>4737.64</v>
+        <v>162.71</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5707,13 +5701,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>3.000</v>
+        <v>5.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>162.71</v>
+        <v>523.85</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5733,13 +5727,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>5.000</v>
+        <v>30.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>523.85</v>
+        <v>179.62</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5759,13 +5753,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>30.000</v>
+        <v>6.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>179.62</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5785,13 +5779,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>98.34</v>
+        <v>374.15</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5811,13 +5805,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>10.000</v>
+        <v>468.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>374.15</v>
+        <v>2071.35</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5837,13 +5831,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>468.000</v>
+        <v>16.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>2071.35</v>
+        <v>1467.58</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5863,13 +5857,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>16.000</v>
+        <v>1.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>1467.58</v>
+        <v>135.35</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5889,13 +5883,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>1.000</v>
+        <v>25.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>135.35</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5915,13 +5909,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>25.000</v>
+        <v>8.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>116.25</v>
+        <v>955.65</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5941,13 +5935,13 @@
         <v>323</v>
       </c>
       <c r="F161" s="2">
-        <v>8.000</v>
+        <v>33.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>955.65</v>
+        <v>3473.41</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5967,13 +5961,13 @@
         <v>325</v>
       </c>
       <c r="F162" s="2">
-        <v>33.000</v>
+        <v>55.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>3473.41</v>
+        <v>7343.43</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5993,13 +5987,13 @@
         <v>327</v>
       </c>
       <c r="F163" s="2">
-        <v>55.000</v>
+        <v>1.000</v>
       </c>
       <c r="G163" t="s">
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>7343.43</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6016,16 +6010,16 @@
         <v>328</v>
       </c>
       <c r="E164" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F164" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G164" t="s">
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>40.71</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6039,19 +6033,19 @@
         <v>2</v>
       </c>
       <c r="D165" t="s">
+        <v>329</v>
+      </c>
+      <c r="E165" t="s">
         <v>330</v>
       </c>
-      <c r="E165" t="s">
-        <v>329</v>
-      </c>
       <c r="F165" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G165" t="s">
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>317.81</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6077,7 +6071,7 @@
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>483.20</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6097,13 +6091,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>45.92</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6123,13 +6117,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>303.12</v>
+        <v>1128.58</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6149,13 +6143,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>8.000</v>
+        <v>3.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>1128.58</v>
+        <v>1054.62</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6175,13 +6169,13 @@
         <v>340</v>
       </c>
       <c r="F170" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>1054.62</v>
+        <v>362.54</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6201,13 +6195,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>362.54</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6227,13 +6221,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>412.45</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6253,13 +6247,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>24.27</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6279,13 +6273,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>9.000</v>
+        <v>15.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>214.33</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6305,13 +6299,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>15.000</v>
+        <v>2520.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>3032.79</v>
+        <v>47187.00</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6331,13 +6325,13 @@
         <v>352</v>
       </c>
       <c r="F176" s="2">
-        <v>2521.000</v>
+        <v>219146.000</v>
       </c>
       <c r="G176" t="s">
-        <v>5</v>
+        <v>353</v>
       </c>
       <c r="H176" s="3">
-        <v>47205.72</v>
+        <v>332215.83</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6351,19 +6345,19 @@
         <v>2</v>
       </c>
       <c r="D177" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E177" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>219196.000</v>
+        <v>100.000</v>
       </c>
       <c r="G177" t="s">
-        <v>355</v>
+        <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>332291.63</v>
+        <v>3564.38</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6383,13 +6377,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>100.000</v>
+        <v>726.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>3564.38</v>
+        <v>126771.90</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6409,13 +6403,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>726.000</v>
+        <v>13.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>126771.90</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6435,13 +6429,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>13.000</v>
+        <v>11.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>2264.65</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6461,13 +6455,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>11.000</v>
+        <v>22.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>145.79</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6487,13 +6481,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>22.000</v>
+        <v>90.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>10363.87</v>
+        <v>41747.85</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6513,13 +6507,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>90.000</v>
+        <v>53.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>41747.85</v>
+        <v>3236.71</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6539,13 +6533,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>53.000</v>
+        <v>75.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>3236.71</v>
+        <v>10771.46</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6565,13 +6559,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>75.000</v>
+        <v>1.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>10771.46</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6597,7 +6591,7 @@
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1218.18</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6617,13 +6611,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>1.000</v>
+        <v>28.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>1720.00</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6643,13 +6637,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>28.000</v>
+        <v>202.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>1119.31</v>
+        <v>6748.61</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6669,13 +6663,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>202.000</v>
+        <v>466.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>6748.61</v>
+        <v>7284.76</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6695,13 +6689,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>466.000</v>
+        <v>59.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>7284.76</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6721,13 +6715,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>59.000</v>
+        <v>565.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>1003.06</v>
+        <v>11446.90</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6747,13 +6741,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>568.000</v>
+        <v>46.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>11507.68</v>
+        <v>1068.40</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6773,13 +6767,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>47.000</v>
+        <v>93.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>1091.62</v>
+        <v>6626.71</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6799,13 +6793,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>93.000</v>
+        <v>16.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>6626.71</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6825,13 +6819,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>16.000</v>
+        <v>1.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>1789.69</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6851,13 +6845,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>189.22</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6877,13 +6871,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>19.000</v>
+        <v>244.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>1201.67</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6903,13 +6897,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>244.000</v>
+        <v>2.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>16895.78</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6929,13 +6923,13 @@
         <v>399</v>
       </c>
       <c r="F199" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>651.09</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6955,13 +6949,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>1125.55</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6981,13 +6975,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>718.30</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7013,7 +7007,7 @@
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>266.26</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7033,13 +7027,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>257.36</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7059,13 +7053,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>961.64</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7085,13 +7079,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>726.22</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7111,13 +7105,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>662.53</v>
+        <v>537.99</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7137,13 +7131,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>537.99</v>
+        <v>909.52</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7163,13 +7157,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>7.000</v>
+        <v>37.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>909.52</v>
+        <v>5149.09</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7189,13 +7183,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>37.000</v>
+        <v>1.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>5149.09</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7221,7 +7215,7 @@
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>4700.00</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7241,13 +7235,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>1.000</v>
+        <v>38.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>8560.17</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7267,13 +7261,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>38.000</v>
+        <v>1.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>481.25</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7293,13 +7287,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>1.000</v>
+        <v>17.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>23.34</v>
+        <v>646.00</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7319,13 +7313,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>17.000</v>
+        <v>22.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>646.00</v>
+        <v>1452.69</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7345,13 +7339,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>22.000</v>
+        <v>1.000</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
       </c>
       <c r="H215" s="3">
-        <v>1452.69</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7371,13 +7365,13 @@
         <v>433</v>
       </c>
       <c r="F216" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G216" t="s">
         <v>5</v>
       </c>
       <c r="H216" s="3">
-        <v>685.11</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7397,13 +7391,13 @@
         <v>435</v>
       </c>
       <c r="F217" s="2">
-        <v>2.000</v>
+        <v>4.800</v>
       </c>
       <c r="G217" t="s">
-        <v>5</v>
+        <v>436</v>
       </c>
       <c r="H217" s="3">
-        <v>8149.76</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7417,19 +7411,19 @@
         <v>2</v>
       </c>
       <c r="D218" t="s">
+        <v>437</v>
+      </c>
+      <c r="E218" t="s">
+        <v>438</v>
+      </c>
+      <c r="F218" s="2">
+        <v>16.000</v>
+      </c>
+      <c r="G218" t="s">
         <v>436</v>
       </c>
-      <c r="E218" t="s">
-        <v>437</v>
-      </c>
-      <c r="F218" s="2">
-        <v>4.800</v>
-      </c>
-      <c r="G218" t="s">
-        <v>438</v>
-      </c>
       <c r="H218" s="3">
-        <v>1822.34</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7449,13 +7443,13 @@
         <v>440</v>
       </c>
       <c r="F219" s="2">
-        <v>16.000</v>
+        <v>17.000</v>
       </c>
       <c r="G219" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H219" s="3">
-        <v>7011.29</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7475,13 +7469,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>17.000</v>
+        <v>162.140</v>
       </c>
       <c r="G220" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H220" s="3">
-        <v>2938.94</v>
+        <v>35221.32</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7501,13 +7495,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>162.140</v>
+        <v>1.090</v>
       </c>
       <c r="G221" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H221" s="3">
-        <v>35221.32</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7527,13 +7521,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>1.090</v>
+        <v>20.300</v>
       </c>
       <c r="G222" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H222" s="3">
-        <v>250.66</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7553,13 +7547,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>20.300</v>
+        <v>13.000</v>
       </c>
       <c r="G223" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H223" s="3">
-        <v>6816.84</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7579,13 +7573,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>13.000</v>
+        <v>22.000</v>
       </c>
       <c r="G224" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H224" s="3">
-        <v>3437.72</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7605,13 +7599,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>22.000</v>
+        <v>343.600</v>
       </c>
       <c r="G225" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H225" s="3">
-        <v>2084.93</v>
+        <v>3442.91</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7631,13 +7625,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>343.600</v>
+        <v>0.360</v>
       </c>
       <c r="G226" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H226" s="3">
-        <v>3442.91</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7657,13 +7651,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>0.360</v>
+        <v>11.000</v>
       </c>
       <c r="G227" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H227" s="3">
-        <v>7.79</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7683,13 +7677,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>11.000</v>
+        <v>150.000</v>
       </c>
       <c r="G228" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H228" s="3">
-        <v>974.64</v>
+        <v>24001.36</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7709,13 +7703,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>150.000</v>
+        <v>168.620</v>
       </c>
       <c r="G229" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H229" s="3">
-        <v>24001.36</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7735,13 +7729,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>168.620</v>
+        <v>47.250</v>
       </c>
       <c r="G230" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H230" s="3">
-        <v>8798.84</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7761,13 +7755,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>47.250</v>
+        <v>21194.800</v>
       </c>
       <c r="G231" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H231" s="3">
-        <v>5148.59</v>
+        <v>48097.22</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7787,13 +7781,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>21217.800</v>
+        <v>3217.960</v>
       </c>
       <c r="G232" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H232" s="3">
-        <v>48149.42</v>
+        <v>14122.61</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7813,13 +7807,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>3222.960</v>
+        <v>29.390</v>
       </c>
       <c r="G233" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H233" s="3">
-        <v>14144.56</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7839,13 +7833,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>29.390</v>
+        <v>856.370</v>
       </c>
       <c r="G234" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H234" s="3">
-        <v>15217.18</v>
+        <v>32198.67</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7865,13 +7859,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>856.370</v>
+        <v>1.600</v>
       </c>
       <c r="G235" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H235" s="3">
-        <v>32198.67</v>
+        <v>15.97</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7891,13 +7885,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>1.600</v>
+        <v>27.800</v>
       </c>
       <c r="G236" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H236" s="3">
-        <v>15.97</v>
+        <v>622.40</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7917,13 +7911,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>27.800</v>
+        <v>529.040</v>
       </c>
       <c r="G237" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H237" s="3">
-        <v>622.40</v>
+        <v>16620.56</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7943,13 +7937,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>529.040</v>
+        <v>211.090</v>
       </c>
       <c r="G238" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H238" s="3">
-        <v>16620.56</v>
+        <v>19367.87</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7969,13 +7963,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>211.090</v>
+        <v>59.100</v>
       </c>
       <c r="G239" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H239" s="3">
-        <v>19367.87</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7995,13 +7989,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>59.100</v>
+        <v>237.900</v>
       </c>
       <c r="G240" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H240" s="3">
-        <v>9271.17</v>
+        <v>7688.51</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8021,13 +8015,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>237.900</v>
+        <v>91.020</v>
       </c>
       <c r="G241" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H241" s="3">
-        <v>7688.51</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8047,13 +8041,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>91.020</v>
+        <v>0.690</v>
       </c>
       <c r="G242" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H242" s="3">
-        <v>1685.63</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8073,13 +8067,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>0.690</v>
+        <v>48.790</v>
       </c>
       <c r="G243" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H243" s="3">
-        <v>20.12</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8099,13 +8093,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>48.790</v>
+        <v>78.310</v>
       </c>
       <c r="G244" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H244" s="3">
-        <v>1048.10</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8125,13 +8119,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>78.310</v>
+        <v>203.000</v>
       </c>
       <c r="G245" t="s">
-        <v>438</v>
+        <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>7083.14</v>
+        <v>1188.57</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8151,13 +8145,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>203.000</v>
+        <v>73.000</v>
       </c>
       <c r="G246" t="s">
         <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>1188.57</v>
+        <v>402.15</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8177,13 +8171,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>73.000</v>
+        <v>5640.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>402.15</v>
+        <v>14158.44</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8203,13 +8197,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>5640.000</v>
+        <v>8.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>14158.44</v>
+        <v>2847.85</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8229,13 +8223,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>8.000</v>
+        <v>7.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>2847.85</v>
+        <v>3897.18</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8255,13 +8249,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>7.000</v>
+        <v>12.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>3897.18</v>
+        <v>5172.18</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8281,13 +8275,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>5172.18</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8307,13 +8301,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>2371.80</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8333,13 +8327,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>2323.99</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8365,7 +8359,7 @@
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>1462.82</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8385,13 +8379,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>6585.02</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8411,13 +8405,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>6.000</v>
+        <v>45.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>1694.29</v>
+        <v>20798.75</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8437,13 +8431,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>45.000</v>
+        <v>8.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>20798.75</v>
+        <v>4529.21</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8463,13 +8457,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>4529.21</v>
+        <v>1721.73</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8489,13 +8483,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>1721.73</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8515,13 +8509,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>6821.40</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8541,13 +8535,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>7220.40</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8567,13 +8561,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>7.000</v>
+        <v>17.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>2566.22</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8593,13 +8587,13 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>17.000</v>
+        <v>7.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>7823.48</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -8619,13 +8613,13 @@
         <v>530</v>
       </c>
       <c r="F264" s="2">
-        <v>7.000</v>
+        <v>5.000</v>
       </c>
       <c r="G264" t="s">
         <v>5</v>
       </c>
       <c r="H264" s="3">
-        <v>3943.24</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="265" spans="1:8">
@@ -8645,38 +8639,12 @@
         <v>532</v>
       </c>
       <c r="F265" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G265" t="s">
         <v>5</v>
       </c>
       <c r="H265" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="266" spans="1:8">
-      <c r="A266" t="s">
-        <v>0</v>
-      </c>
-      <c r="B266" t="s">
-        <v>1</v>
-      </c>
-      <c r="C266" t="s">
-        <v>2</v>
-      </c>
-      <c r="D266" t="s">
-        <v>533</v>
-      </c>
-      <c r="E266" t="s">
-        <v>534</v>
-      </c>
-      <c r="F266" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H266" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: excluding contratada material nosense
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="537">
   <si>
     <t>4600041302</t>
   </si>
@@ -925,12 +925,6 @@
     <t>LUVA CORRER FF DUCTIL BOLSAS JE - DN 80</t>
   </si>
   <si>
-    <t>30002813</t>
-  </si>
-  <si>
-    <t>LUVA CORRER FF DUCTIL BOLSAS JE2GS DN 75</t>
-  </si>
-  <si>
     <t>30005931</t>
   </si>
   <si>
@@ -1466,12 +1460,6 @@
   </si>
   <si>
     <t>TUBO PVC RIG PB JEI/JERI DN 50 CL 20.</t>
-  </si>
-  <si>
-    <t>30026318</t>
-  </si>
-  <si>
-    <t>TUBO PVC RIG PB JEI/JERI DN 75 CL. 20</t>
   </si>
   <si>
     <t>30007933</t>
@@ -1740,7 +1728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H265"/>
+  <dimension ref="A1:H263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1760,28 +1748,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>539</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1983,13 +1971,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>1.000</v>
+        <v>36.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>427.58</v>
+        <v>8671.49</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2165,13 +2153,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>145.000</v>
+        <v>132.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>13724.88</v>
+        <v>12494.38</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2737,13 +2725,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>13.000</v>
+        <v>11.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>726.80</v>
+        <v>614.98</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2789,13 +2777,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>174.000</v>
+        <v>164.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>8173.62</v>
+        <v>7703.88</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2841,13 +2829,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>263.000</v>
+        <v>363.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>7484.01</v>
+        <v>10329.63</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2867,13 +2855,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>109.000</v>
+        <v>108.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>17281.41</v>
+        <v>17122.86</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2893,13 +2881,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>41.000</v>
+        <v>27.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>22909.77</v>
+        <v>15086.93</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2945,13 +2933,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>79.000</v>
+        <v>47.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>15005.76</v>
+        <v>8927.45</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3179,13 +3167,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>670.000</v>
+        <v>561.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>6079.98</v>
+        <v>5090.90</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3231,13 +3219,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3166.000</v>
+        <v>3054.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>32540.26</v>
+        <v>31389.03</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3413,13 +3401,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>28.000</v>
+        <v>26.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>2209.27</v>
+        <v>2051.47</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3549,7 +3537,7 @@
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>6770.66</v>
+        <v>6770.70</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3595,13 +3583,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>42.000</v>
+        <v>41.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>6244.14</v>
+        <v>6095.47</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3627,7 +3615,7 @@
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>1598.50</v>
+        <v>1598.51</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3855,13 +3843,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>1318.000</v>
+        <v>1314.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>8101.11</v>
+        <v>8076.40</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3907,13 +3895,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2888.000</v>
+        <v>2800.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>75225.39</v>
+        <v>72933.04</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4069,7 +4057,7 @@
         <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>1572.64</v>
+        <v>1572.63</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4141,13 +4129,13 @@
         <v>185</v>
       </c>
       <c r="F92" s="2">
-        <v>136.000</v>
+        <v>134.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>5126.52</v>
+        <v>5051.13</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -4271,13 +4259,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>247.000</v>
+        <v>237.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>20909.00</v>
+        <v>20062.49</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4297,13 +4285,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>2035.000</v>
+        <v>2369.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>286174.81</v>
+        <v>333142.76</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4381,7 +4369,7 @@
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>1598.31</v>
+        <v>1598.30</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4713,13 +4701,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>629.000</v>
+        <v>626.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>23342.73</v>
+        <v>23231.39</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4739,13 +4727,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>347.000</v>
+        <v>342.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>22682.92</v>
+        <v>22356.07</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4765,13 +4753,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>1010.000</v>
+        <v>1008.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>33276.11</v>
+        <v>33210.21</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4791,13 +4779,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>171.000</v>
+        <v>170.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>8786.55</v>
+        <v>8735.16</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4817,13 +4805,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>25.000</v>
+        <v>21.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>2547.94</v>
+        <v>2140.27</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4895,13 +4883,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>12688.000</v>
+        <v>12280.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>49251.06</v>
+        <v>47667.73</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -5155,13 +5143,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>39.000</v>
+        <v>38.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>56252.24</v>
+        <v>54809.87</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5181,13 +5169,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>556.000</v>
+        <v>555.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>3147.42</v>
+        <v>3141.77</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5207,13 +5195,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>297.000</v>
+        <v>296.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>2441.91</v>
+        <v>2433.69</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5285,13 +5273,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>80.000</v>
+        <v>78.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>2441.82</v>
+        <v>2380.78</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5623,13 +5611,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>1094.94</v>
+        <v>547.47</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5701,13 +5689,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>5.000</v>
+        <v>30.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>523.85</v>
+        <v>181.80</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5727,13 +5715,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>30.000</v>
+        <v>6.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>179.62</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5753,13 +5741,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>6.000</v>
+        <v>10.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>98.34</v>
+        <v>374.15</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5779,13 +5767,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>10.000</v>
+        <v>468.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>374.15</v>
+        <v>2071.35</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5805,13 +5793,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>468.000</v>
+        <v>16.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>2071.35</v>
+        <v>1467.58</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5831,13 +5819,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>16.000</v>
+        <v>1.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>1467.58</v>
+        <v>135.35</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5857,13 +5845,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>1.000</v>
+        <v>25.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>135.35</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5883,13 +5871,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>25.000</v>
+        <v>8.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>116.25</v>
+        <v>955.65</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5909,13 +5897,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>8.000</v>
+        <v>33.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>955.65</v>
+        <v>3473.41</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5935,13 +5923,13 @@
         <v>323</v>
       </c>
       <c r="F161" s="2">
-        <v>33.000</v>
+        <v>50.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>3473.41</v>
+        <v>6675.84</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5961,13 +5949,13 @@
         <v>325</v>
       </c>
       <c r="F162" s="2">
-        <v>55.000</v>
+        <v>1.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>7343.43</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5984,16 +5972,16 @@
         <v>326</v>
       </c>
       <c r="E163" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F163" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G163" t="s">
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>40.71</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6007,19 +5995,19 @@
         <v>2</v>
       </c>
       <c r="D164" t="s">
+        <v>327</v>
+      </c>
+      <c r="E164" t="s">
         <v>328</v>
       </c>
-      <c r="E164" t="s">
-        <v>327</v>
-      </c>
       <c r="F164" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G164" t="s">
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>317.81</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6045,7 +6033,7 @@
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>483.20</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6065,13 +6053,13 @@
         <v>332</v>
       </c>
       <c r="F166" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G166" t="s">
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>45.92</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6091,13 +6079,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>303.12</v>
+        <v>1128.58</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6117,13 +6105,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>8.000</v>
+        <v>3.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>1128.58</v>
+        <v>1054.62</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6143,13 +6131,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>1054.62</v>
+        <v>362.54</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6169,13 +6157,13 @@
         <v>340</v>
       </c>
       <c r="F170" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>362.54</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6195,13 +6183,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>412.45</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6221,13 +6209,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>1.000</v>
+        <v>9.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>24.27</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6247,13 +6235,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>9.000</v>
+        <v>15.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>214.33</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6273,13 +6261,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>15.000</v>
+        <v>2444.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>3032.79</v>
+        <v>45763.90</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6299,13 +6287,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>2520.000</v>
+        <v>217951.000</v>
       </c>
       <c r="G175" t="s">
-        <v>5</v>
+        <v>351</v>
       </c>
       <c r="H175" s="3">
-        <v>47187.00</v>
+        <v>331019.92</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6319,19 +6307,19 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E176" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>219146.000</v>
+        <v>100.000</v>
       </c>
       <c r="G176" t="s">
-        <v>353</v>
+        <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>332215.83</v>
+        <v>3564.38</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6351,13 +6339,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>100.000</v>
+        <v>725.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>3564.38</v>
+        <v>126597.25</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6377,13 +6365,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>726.000</v>
+        <v>13.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>126771.90</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6403,13 +6391,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>13.000</v>
+        <v>11.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>2264.65</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6429,13 +6417,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>11.000</v>
+        <v>22.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>145.79</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6455,13 +6443,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>22.000</v>
+        <v>85.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>10363.87</v>
+        <v>39428.52</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6481,13 +6469,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>90.000</v>
+        <v>49.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>41747.85</v>
+        <v>2992.43</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6507,13 +6495,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>53.000</v>
+        <v>75.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>3236.71</v>
+        <v>10771.46</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6533,13 +6521,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>75.000</v>
+        <v>1.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>10771.46</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6565,7 +6553,7 @@
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>1218.18</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6585,13 +6573,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>1.000</v>
+        <v>28.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1720.00</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6611,13 +6599,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>28.000</v>
+        <v>202.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>1119.31</v>
+        <v>6748.61</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6637,13 +6625,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>202.000</v>
+        <v>464.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>6748.61</v>
+        <v>7253.53</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6663,13 +6651,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>466.000</v>
+        <v>59.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>7284.76</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6689,13 +6677,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>59.000</v>
+        <v>543.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>1003.06</v>
+        <v>11001.18</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6715,13 +6703,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>565.000</v>
+        <v>46.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>11446.90</v>
+        <v>1068.40</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6741,13 +6729,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>46.000</v>
+        <v>93.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>1068.40</v>
+        <v>6626.71</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6767,13 +6755,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>93.000</v>
+        <v>16.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>6626.71</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6793,13 +6781,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>16.000</v>
+        <v>1.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>1789.69</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6819,13 +6807,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>189.22</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6845,13 +6833,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>19.000</v>
+        <v>244.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>1201.67</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6871,13 +6859,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>244.000</v>
+        <v>2.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>16895.78</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6897,13 +6885,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>651.09</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6923,13 +6911,13 @@
         <v>399</v>
       </c>
       <c r="F199" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>1125.55</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6949,13 +6937,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>718.30</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6981,7 +6969,7 @@
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>266.26</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7001,13 +6989,13 @@
         <v>405</v>
       </c>
       <c r="F202" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G202" t="s">
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>257.36</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7027,13 +7015,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>961.64</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7053,13 +7041,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>726.22</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7079,13 +7067,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>662.53</v>
+        <v>537.99</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7105,13 +7093,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>537.99</v>
+        <v>909.52</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7131,13 +7119,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>7.000</v>
+        <v>32.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>909.52</v>
+        <v>4453.27</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7157,13 +7145,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>37.000</v>
+        <v>1.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>5149.09</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7189,7 +7177,7 @@
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>4700.00</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7209,13 +7197,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>1.000</v>
+        <v>38.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>8560.17</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7235,13 +7223,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>38.000</v>
+        <v>1.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>481.25</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7261,13 +7249,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>1.000</v>
+        <v>17.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>23.34</v>
+        <v>646.00</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7287,13 +7275,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>17.000</v>
+        <v>22.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>646.00</v>
+        <v>1452.69</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7313,13 +7301,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>22.000</v>
+        <v>1.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>1452.69</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7339,13 +7327,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
       </c>
       <c r="H215" s="3">
-        <v>685.11</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7365,13 +7353,13 @@
         <v>433</v>
       </c>
       <c r="F216" s="2">
-        <v>2.000</v>
+        <v>4.800</v>
       </c>
       <c r="G216" t="s">
-        <v>5</v>
+        <v>434</v>
       </c>
       <c r="H216" s="3">
-        <v>8149.76</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7385,19 +7373,19 @@
         <v>2</v>
       </c>
       <c r="D217" t="s">
+        <v>435</v>
+      </c>
+      <c r="E217" t="s">
+        <v>436</v>
+      </c>
+      <c r="F217" s="2">
+        <v>16.000</v>
+      </c>
+      <c r="G217" t="s">
         <v>434</v>
       </c>
-      <c r="E217" t="s">
-        <v>435</v>
-      </c>
-      <c r="F217" s="2">
-        <v>4.800</v>
-      </c>
-      <c r="G217" t="s">
-        <v>436</v>
-      </c>
       <c r="H217" s="3">
-        <v>1822.34</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7417,13 +7405,13 @@
         <v>438</v>
       </c>
       <c r="F218" s="2">
-        <v>16.000</v>
+        <v>17.000</v>
       </c>
       <c r="G218" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H218" s="3">
-        <v>7011.29</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7443,13 +7431,13 @@
         <v>440</v>
       </c>
       <c r="F219" s="2">
-        <v>17.000</v>
+        <v>162.140</v>
       </c>
       <c r="G219" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H219" s="3">
-        <v>2938.94</v>
+        <v>35221.32</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7469,13 +7457,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>162.140</v>
+        <v>1.090</v>
       </c>
       <c r="G220" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H220" s="3">
-        <v>35221.32</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7495,13 +7483,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>1.090</v>
+        <v>20.300</v>
       </c>
       <c r="G221" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H221" s="3">
-        <v>250.66</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7521,13 +7509,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>20.300</v>
+        <v>13.000</v>
       </c>
       <c r="G222" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H222" s="3">
-        <v>6816.84</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7547,13 +7535,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>13.000</v>
+        <v>22.000</v>
       </c>
       <c r="G223" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H223" s="3">
-        <v>3437.72</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7573,13 +7561,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>22.000</v>
+        <v>305.020</v>
       </c>
       <c r="G224" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H224" s="3">
-        <v>2084.93</v>
+        <v>3056.34</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7599,13 +7587,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>343.600</v>
+        <v>0.360</v>
       </c>
       <c r="G225" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H225" s="3">
-        <v>3442.91</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7625,13 +7613,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>0.360</v>
+        <v>11.000</v>
       </c>
       <c r="G226" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H226" s="3">
-        <v>7.79</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7651,13 +7639,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>11.000</v>
+        <v>150.000</v>
       </c>
       <c r="G227" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H227" s="3">
-        <v>974.64</v>
+        <v>24001.36</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7677,13 +7665,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>150.000</v>
+        <v>168.620</v>
       </c>
       <c r="G228" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H228" s="3">
-        <v>24001.36</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7703,13 +7691,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>168.620</v>
+        <v>47.250</v>
       </c>
       <c r="G229" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H229" s="3">
-        <v>8798.84</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7729,13 +7717,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>47.250</v>
+        <v>20310.800</v>
       </c>
       <c r="G230" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H230" s="3">
-        <v>5148.59</v>
+        <v>46091.11</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7755,13 +7743,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>21194.800</v>
+        <v>3217.960</v>
       </c>
       <c r="G231" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H231" s="3">
-        <v>48097.22</v>
+        <v>14122.61</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7781,13 +7769,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>3217.960</v>
+        <v>29.390</v>
       </c>
       <c r="G232" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H232" s="3">
-        <v>14122.61</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7807,13 +7795,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>29.390</v>
+        <v>856.370</v>
       </c>
       <c r="G233" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H233" s="3">
-        <v>15217.18</v>
+        <v>32198.67</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7833,13 +7821,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>856.370</v>
+        <v>0.100</v>
       </c>
       <c r="G234" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H234" s="3">
-        <v>32198.67</v>
+        <v>1.00</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7859,13 +7847,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>1.600</v>
+        <v>12.800</v>
       </c>
       <c r="G235" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H235" s="3">
-        <v>15.97</v>
+        <v>286.57</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7885,13 +7873,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>27.800</v>
+        <v>427.520</v>
       </c>
       <c r="G236" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H236" s="3">
-        <v>622.40</v>
+        <v>13431.16</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7911,13 +7899,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>529.040</v>
+        <v>211.090</v>
       </c>
       <c r="G237" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H237" s="3">
-        <v>16620.56</v>
+        <v>19367.87</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7937,13 +7925,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>211.090</v>
+        <v>59.100</v>
       </c>
       <c r="G238" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H238" s="3">
-        <v>19367.87</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7963,13 +7951,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>59.100</v>
+        <v>237.900</v>
       </c>
       <c r="G239" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H239" s="3">
-        <v>9271.17</v>
+        <v>7688.51</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7989,13 +7977,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>237.900</v>
+        <v>91.020</v>
       </c>
       <c r="G240" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H240" s="3">
-        <v>7688.51</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8015,13 +8003,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>91.020</v>
+        <v>48.790</v>
       </c>
       <c r="G241" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H241" s="3">
-        <v>1685.63</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8041,13 +8029,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>0.690</v>
+        <v>78.310</v>
       </c>
       <c r="G242" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H242" s="3">
-        <v>20.12</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8067,13 +8055,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>48.790</v>
+        <v>203.000</v>
       </c>
       <c r="G243" t="s">
-        <v>436</v>
+        <v>5</v>
       </c>
       <c r="H243" s="3">
-        <v>1048.10</v>
+        <v>1188.57</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8093,13 +8081,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>78.310</v>
+        <v>73.000</v>
       </c>
       <c r="G244" t="s">
-        <v>436</v>
+        <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>7083.14</v>
+        <v>402.15</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8119,13 +8107,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>203.000</v>
+        <v>5602.000</v>
       </c>
       <c r="G245" t="s">
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>1188.57</v>
+        <v>14063.07</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8145,13 +8133,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>73.000</v>
+        <v>8.000</v>
       </c>
       <c r="G246" t="s">
         <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>402.15</v>
+        <v>2847.85</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8171,13 +8159,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>5640.000</v>
+        <v>6.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>14158.44</v>
+        <v>3340.44</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8203,7 +8191,7 @@
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>2847.85</v>
+        <v>3448.12</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8223,13 +8211,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>7.000</v>
+        <v>6.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>3897.18</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8249,13 +8237,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>12.000</v>
+        <v>2.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>5172.18</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8275,13 +8263,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>2371.80</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8301,13 +8289,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>2323.99</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8327,13 +8315,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>1462.82</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8353,13 +8341,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>1.000</v>
+        <v>44.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>6585.02</v>
+        <v>20336.56</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8379,13 +8367,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>1694.29</v>
+        <v>4529.21</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8405,13 +8393,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>45.000</v>
+        <v>1.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>20798.75</v>
+        <v>1721.73</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8431,13 +8419,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>8.000</v>
+        <v>4.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>4529.21</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8457,13 +8445,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>1721.73</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8483,13 +8471,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>4.000</v>
+        <v>7.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>6821.40</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8509,13 +8497,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>2.000</v>
+        <v>16.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>7220.40</v>
+        <v>7363.28</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8541,7 +8529,7 @@
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>2566.22</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8561,13 +8549,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>17.000</v>
+        <v>5.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>7823.48</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8587,64 +8575,12 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
-        <v>7.000</v>
+        <v>3.000</v>
       </c>
       <c r="G263" t="s">
         <v>5</v>
       </c>
       <c r="H263" s="3">
-        <v>3943.24</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8">
-      <c r="A264" t="s">
-        <v>0</v>
-      </c>
-      <c r="B264" t="s">
-        <v>1</v>
-      </c>
-      <c r="C264" t="s">
-        <v>2</v>
-      </c>
-      <c r="D264" t="s">
-        <v>529</v>
-      </c>
-      <c r="E264" t="s">
-        <v>530</v>
-      </c>
-      <c r="F264" s="2">
-        <v>5.000</v>
-      </c>
-      <c r="G264" t="s">
-        <v>5</v>
-      </c>
-      <c r="H264" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="265" spans="1:8">
-      <c r="A265" t="s">
-        <v>0</v>
-      </c>
-      <c r="B265" t="s">
-        <v>1</v>
-      </c>
-      <c r="C265" t="s">
-        <v>2</v>
-      </c>
-      <c r="D265" t="s">
-        <v>531</v>
-      </c>
-      <c r="E265" t="s">
-        <v>532</v>
-      </c>
-      <c r="F265" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G265" t="s">
-        <v>5</v>
-      </c>
-      <c r="H265" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: pt2 - excluding contratada material nosense
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -2855,13 +2855,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>108.000</v>
+        <v>107.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>17122.86</v>
+        <v>16964.31</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2881,13 +2881,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>27.000</v>
+        <v>26.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>15086.93</v>
+        <v>14528.15</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2907,13 +2907,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>59.000</v>
+        <v>58.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>5201.25</v>
+        <v>5113.09</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3167,13 +3167,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>561.000</v>
+        <v>560.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>5090.90</v>
+        <v>5081.82</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3219,13 +3219,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3054.000</v>
+        <v>3050.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>31389.03</v>
+        <v>31347.92</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3849,7 +3849,7 @@
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>8076.40</v>
+        <v>8076.41</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3895,13 +3895,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2800.000</v>
+        <v>2796.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>72933.04</v>
+        <v>72828.85</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4285,13 +4285,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>2369.000</v>
+        <v>2365.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>333142.76</v>
+        <v>332579.30</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4883,13 +4883,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>12280.000</v>
+        <v>12271.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>47667.73</v>
+        <v>47632.80</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -6261,13 +6261,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>2444.000</v>
+        <v>2441.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>45763.90</v>
+        <v>45707.72</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6631,7 +6631,7 @@
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>7253.53</v>
+        <v>7253.54</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -7717,13 +7717,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>20310.800</v>
+        <v>20292.800</v>
       </c>
       <c r="G230" t="s">
         <v>434</v>
       </c>
       <c r="H230" s="3">
-        <v>46091.11</v>
+        <v>46050.26</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -8107,13 +8107,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>5602.000</v>
+        <v>5601.000</v>
       </c>
       <c r="G245" t="s">
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>14063.07</v>
+        <v>14060.56</v>
       </c>
     </row>
     <row r="246" spans="1:8">

</xml_diff>

<commit_message>
#feat: get all family without declare it
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="539">
   <si>
     <t>4600041302</t>
   </si>
@@ -1073,6 +1073,12 @@
   </si>
   <si>
     <t>SELIM 90 G PVC DN 300 X 100 ENCAIXE</t>
+  </si>
+  <si>
+    <t>30007132</t>
+  </si>
+  <si>
+    <t>SELIM AJUST TUBO PVC E CER DN 150X100</t>
   </si>
   <si>
     <t>30003416</t>
@@ -1728,7 +1734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H263"/>
+  <dimension ref="A1:H264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1748,28 +1754,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1971,13 +1977,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>36.000</v>
+        <v>25.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>8671.49</v>
+        <v>6113.38</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2153,13 +2159,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>132.000</v>
+        <v>129.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>12494.38</v>
+        <v>12210.43</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2777,13 +2783,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>164.000</v>
+        <v>163.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>7703.88</v>
+        <v>7656.91</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2829,13 +2835,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>363.000</v>
+        <v>360.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>10329.63</v>
+        <v>10244.25</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2881,13 +2887,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>26.000</v>
+        <v>16.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>14528.15</v>
+        <v>8940.40</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2933,13 +2939,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>47.000</v>
+        <v>40.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>8927.45</v>
+        <v>7597.83</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3167,13 +3173,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>560.000</v>
+        <v>557.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>5081.82</v>
+        <v>5054.61</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3219,13 +3225,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3050.000</v>
+        <v>3033.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>31347.92</v>
+        <v>31173.18</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3583,13 +3589,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>41.000</v>
+        <v>37.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>6095.47</v>
+        <v>5500.79</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3843,13 +3849,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>1314.000</v>
+        <v>1253.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>8076.41</v>
+        <v>7701.39</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3895,13 +3901,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2796.000</v>
+        <v>2770.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>72828.85</v>
+        <v>72151.59</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4259,13 +4265,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>237.000</v>
+        <v>233.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>20062.49</v>
+        <v>19723.88</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4285,13 +4291,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>2365.000</v>
+        <v>2346.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>332579.30</v>
+        <v>329904.67</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4701,13 +4707,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>626.000</v>
+        <v>625.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>23231.39</v>
+        <v>23194.28</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4753,13 +4759,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>1008.000</v>
+        <v>951.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>33210.21</v>
+        <v>31332.17</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4883,13 +4889,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>12271.000</v>
+        <v>12142.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>47632.80</v>
+        <v>47132.10</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -5143,13 +5149,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>38.000</v>
+        <v>37.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>54809.87</v>
+        <v>53367.50</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5169,13 +5175,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>555.000</v>
+        <v>554.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>3141.77</v>
+        <v>3136.11</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5195,13 +5201,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>296.000</v>
+        <v>240.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>2433.69</v>
+        <v>1973.27</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5903,7 +5909,7 @@
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>3473.41</v>
+        <v>3473.42</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -6261,13 +6267,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>2441.000</v>
+        <v>2425.000</v>
       </c>
       <c r="G174" t="s">
         <v>5</v>
       </c>
       <c r="H174" s="3">
-        <v>45707.72</v>
+        <v>45408.13</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6287,13 +6293,13 @@
         <v>350</v>
       </c>
       <c r="F175" s="2">
-        <v>217951.000</v>
+        <v>217001.000</v>
       </c>
       <c r="G175" t="s">
         <v>351</v>
       </c>
       <c r="H175" s="3">
-        <v>331019.92</v>
+        <v>329920.23</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6339,13 +6345,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>725.000</v>
+        <v>1.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>126597.25</v>
+        <v>191.34</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6365,13 +6371,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>13.000</v>
+        <v>664.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>2264.65</v>
+        <v>115945.60</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6391,13 +6397,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>11.000</v>
+        <v>13.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>145.79</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6417,13 +6423,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>22.000</v>
+        <v>11.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>10363.87</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6443,13 +6449,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>85.000</v>
+        <v>22.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>39428.52</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6469,13 +6475,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>49.000</v>
+        <v>85.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>2992.43</v>
+        <v>39428.52</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6495,13 +6501,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>75.000</v>
+        <v>49.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>10771.46</v>
+        <v>2992.43</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6521,13 +6527,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>1.000</v>
+        <v>75.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>1218.18</v>
+        <v>10771.46</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6553,7 +6559,7 @@
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>1720.00</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6573,13 +6579,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>28.000</v>
+        <v>1.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1119.31</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6599,13 +6605,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>202.000</v>
+        <v>28.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>6748.61</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6625,13 +6631,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>464.000</v>
+        <v>202.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>7253.54</v>
+        <v>6748.61</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6651,13 +6657,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>59.000</v>
+        <v>464.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>1003.06</v>
+        <v>7253.54</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6677,13 +6683,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>543.000</v>
+        <v>59.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>11001.18</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6703,13 +6709,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>46.000</v>
+        <v>537.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>1068.40</v>
+        <v>10879.62</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6729,13 +6735,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>93.000</v>
+        <v>46.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>6626.71</v>
+        <v>1068.40</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6755,13 +6761,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>16.000</v>
+        <v>93.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>1789.69</v>
+        <v>6626.71</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6781,13 +6787,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>1.000</v>
+        <v>16.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>189.22</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6807,13 +6813,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>19.000</v>
+        <v>1.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>1201.67</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6833,13 +6839,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>244.000</v>
+        <v>19.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>16895.78</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6859,13 +6865,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>2.000</v>
+        <v>244.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>651.09</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6885,13 +6891,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>1125.55</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6911,13 +6917,13 @@
         <v>399</v>
       </c>
       <c r="F199" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>718.30</v>
+        <v>1125.55</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6937,13 +6943,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>266.26</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6969,7 +6975,7 @@
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>257.36</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -6989,13 +6995,13 @@
         <v>405</v>
       </c>
       <c r="F202" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G202" t="s">
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>961.64</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7015,13 +7021,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>726.22</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7041,13 +7047,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>662.53</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7067,13 +7073,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>2.000</v>
+        <v>5.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>537.99</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7093,13 +7099,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>7.000</v>
+        <v>2.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>909.52</v>
+        <v>537.99</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7119,13 +7125,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>32.000</v>
+        <v>7.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>4453.27</v>
+        <v>909.52</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7145,13 +7151,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>1.000</v>
+        <v>32.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>4700.00</v>
+        <v>4453.27</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7177,7 +7183,7 @@
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>8560.17</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7197,13 +7203,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>38.000</v>
+        <v>1.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>481.25</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7223,13 +7229,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>1.000</v>
+        <v>38.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>23.34</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7249,13 +7255,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>17.000</v>
+        <v>1.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>646.00</v>
+        <v>23.34</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7275,13 +7281,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>22.000</v>
+        <v>17.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>1452.69</v>
+        <v>646.00</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7301,13 +7307,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>1.000</v>
+        <v>22.000</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
       </c>
       <c r="H214" s="3">
-        <v>685.11</v>
+        <v>1452.69</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7327,13 +7333,13 @@
         <v>431</v>
       </c>
       <c r="F215" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
       </c>
       <c r="H215" s="3">
-        <v>8149.76</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7353,13 +7359,13 @@
         <v>433</v>
       </c>
       <c r="F216" s="2">
-        <v>4.800</v>
+        <v>2.000</v>
       </c>
       <c r="G216" t="s">
-        <v>434</v>
+        <v>5</v>
       </c>
       <c r="H216" s="3">
-        <v>1822.34</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7373,19 +7379,19 @@
         <v>2</v>
       </c>
       <c r="D217" t="s">
+        <v>434</v>
+      </c>
+      <c r="E217" t="s">
         <v>435</v>
       </c>
-      <c r="E217" t="s">
+      <c r="F217" s="2">
+        <v>4.800</v>
+      </c>
+      <c r="G217" t="s">
         <v>436</v>
       </c>
-      <c r="F217" s="2">
-        <v>16.000</v>
-      </c>
-      <c r="G217" t="s">
-        <v>434</v>
-      </c>
       <c r="H217" s="3">
-        <v>7011.29</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7405,13 +7411,13 @@
         <v>438</v>
       </c>
       <c r="F218" s="2">
-        <v>17.000</v>
+        <v>16.000</v>
       </c>
       <c r="G218" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H218" s="3">
-        <v>2938.94</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7431,13 +7437,13 @@
         <v>440</v>
       </c>
       <c r="F219" s="2">
-        <v>162.140</v>
+        <v>17.000</v>
       </c>
       <c r="G219" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H219" s="3">
-        <v>35221.32</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7457,13 +7463,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>1.090</v>
+        <v>162.140</v>
       </c>
       <c r="G220" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H220" s="3">
-        <v>250.66</v>
+        <v>35221.32</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7483,13 +7489,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>20.300</v>
+        <v>1.090</v>
       </c>
       <c r="G221" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H221" s="3">
-        <v>6816.84</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7509,13 +7515,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>13.000</v>
+        <v>20.300</v>
       </c>
       <c r="G222" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H222" s="3">
-        <v>3437.72</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7535,13 +7541,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>22.000</v>
+        <v>13.000</v>
       </c>
       <c r="G223" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H223" s="3">
-        <v>2084.93</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7561,13 +7567,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>305.020</v>
+        <v>22.000</v>
       </c>
       <c r="G224" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H224" s="3">
-        <v>3056.34</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7587,13 +7593,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>0.360</v>
+        <v>305.020</v>
       </c>
       <c r="G225" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H225" s="3">
-        <v>7.79</v>
+        <v>3056.34</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7613,13 +7619,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>11.000</v>
+        <v>0.360</v>
       </c>
       <c r="G226" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H226" s="3">
-        <v>974.64</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7639,13 +7645,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>150.000</v>
+        <v>11.000</v>
       </c>
       <c r="G227" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H227" s="3">
-        <v>24001.36</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7665,13 +7671,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>168.620</v>
+        <v>150.000</v>
       </c>
       <c r="G228" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H228" s="3">
-        <v>8798.84</v>
+        <v>24001.36</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7691,13 +7697,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>47.250</v>
+        <v>168.620</v>
       </c>
       <c r="G229" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H229" s="3">
-        <v>5148.59</v>
+        <v>8798.84</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7717,13 +7723,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>20292.800</v>
+        <v>47.250</v>
       </c>
       <c r="G230" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H230" s="3">
-        <v>46050.26</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7743,13 +7749,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>3217.960</v>
+        <v>20140.800</v>
       </c>
       <c r="G231" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H231" s="3">
-        <v>14122.61</v>
+        <v>45705.31</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7769,13 +7775,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>29.390</v>
+        <v>3217.960</v>
       </c>
       <c r="G232" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H232" s="3">
-        <v>15217.18</v>
+        <v>14122.61</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7795,13 +7801,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>856.370</v>
+        <v>29.390</v>
       </c>
       <c r="G233" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H233" s="3">
-        <v>32198.67</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7821,13 +7827,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>0.100</v>
+        <v>856.370</v>
       </c>
       <c r="G234" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H234" s="3">
-        <v>1.00</v>
+        <v>32198.67</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7847,13 +7853,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>12.800</v>
+        <v>2.100</v>
       </c>
       <c r="G235" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H235" s="3">
-        <v>286.57</v>
+        <v>20.96</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7873,13 +7879,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>427.520</v>
+        <v>12.800</v>
       </c>
       <c r="G236" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H236" s="3">
-        <v>13431.16</v>
+        <v>286.57</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7899,13 +7905,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>211.090</v>
+        <v>427.520</v>
       </c>
       <c r="G237" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H237" s="3">
-        <v>19367.87</v>
+        <v>13431.16</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7925,13 +7931,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>59.100</v>
+        <v>211.090</v>
       </c>
       <c r="G238" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H238" s="3">
-        <v>9271.17</v>
+        <v>19367.87</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7951,13 +7957,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>237.900</v>
+        <v>59.100</v>
       </c>
       <c r="G239" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H239" s="3">
-        <v>7688.51</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7977,13 +7983,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>91.020</v>
+        <v>237.900</v>
       </c>
       <c r="G240" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H240" s="3">
-        <v>1685.63</v>
+        <v>7688.51</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8003,13 +8009,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>48.790</v>
+        <v>91.020</v>
       </c>
       <c r="G241" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H241" s="3">
-        <v>1048.10</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8029,13 +8035,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>78.310</v>
+        <v>48.790</v>
       </c>
       <c r="G242" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H242" s="3">
-        <v>7083.14</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8055,13 +8061,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>203.000</v>
+        <v>78.310</v>
       </c>
       <c r="G243" t="s">
-        <v>5</v>
+        <v>436</v>
       </c>
       <c r="H243" s="3">
-        <v>1188.57</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8081,13 +8087,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>73.000</v>
+        <v>203.000</v>
       </c>
       <c r="G244" t="s">
         <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>402.15</v>
+        <v>1188.57</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8107,13 +8113,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>5601.000</v>
+        <v>73.000</v>
       </c>
       <c r="G245" t="s">
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>14060.56</v>
+        <v>402.15</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8133,13 +8139,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>8.000</v>
+        <v>5597.000</v>
       </c>
       <c r="G246" t="s">
         <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>2847.85</v>
+        <v>14050.51</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8159,13 +8165,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>3340.44</v>
+        <v>2847.85</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8185,13 +8191,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>8.000</v>
+        <v>6.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>3448.12</v>
+        <v>3340.44</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8211,13 +8217,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>2371.80</v>
+        <v>3448.12</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8237,13 +8243,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>2323.99</v>
+        <v>2371.80</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8263,13 +8269,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>1462.82</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8295,7 +8301,7 @@
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>6585.02</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8315,13 +8321,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>1694.29</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8341,13 +8347,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>44.000</v>
+        <v>6.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>20336.56</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8367,13 +8373,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>8.000</v>
+        <v>44.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>4529.21</v>
+        <v>20336.56</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8393,13 +8399,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>1721.73</v>
+        <v>4529.21</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8419,13 +8425,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>6821.40</v>
+        <v>1721.73</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8445,13 +8451,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>7220.40</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8471,13 +8477,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>7.000</v>
+        <v>2.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>2566.22</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8497,13 +8503,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>16.000</v>
+        <v>7.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>7363.28</v>
+        <v>2566.22</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8523,13 +8529,13 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>7.000</v>
+        <v>16.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>3943.24</v>
+        <v>7363.28</v>
       </c>
     </row>
     <row r="262" spans="1:8">
@@ -8549,13 +8555,13 @@
         <v>526</v>
       </c>
       <c r="F262" s="2">
-        <v>5.000</v>
+        <v>7.000</v>
       </c>
       <c r="G262" t="s">
         <v>5</v>
       </c>
       <c r="H262" s="3">
-        <v>2725.89</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="263" spans="1:8">
@@ -8575,12 +8581,38 @@
         <v>528</v>
       </c>
       <c r="F263" s="2">
+        <v>5.000</v>
+      </c>
+      <c r="G263" t="s">
+        <v>5</v>
+      </c>
+      <c r="H263" s="3">
+        <v>2725.89</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8">
+      <c r="A264" t="s">
+        <v>0</v>
+      </c>
+      <c r="B264" t="s">
+        <v>1</v>
+      </c>
+      <c r="C264" t="s">
+        <v>2</v>
+      </c>
+      <c r="D264" t="s">
+        <v>529</v>
+      </c>
+      <c r="E264" t="s">
+        <v>530</v>
+      </c>
+      <c r="F264" s="2">
         <v>3.000</v>
       </c>
-      <c r="G263" t="s">
-        <v>5</v>
-      </c>
-      <c r="H263" s="3">
+      <c r="G264" t="s">
+        <v>5</v>
+      </c>
+      <c r="H264" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
family argument removed from main.rs
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="533">
   <si>
     <t>4600041302</t>
   </si>
@@ -67,12 +67,6 @@
     <t>ABRACADEIRA FF REPARO TUBO DN50 LMIN=150</t>
   </si>
   <si>
-    <t>30001122</t>
-  </si>
-  <si>
-    <t>ABRACADEIRA FF REPARO TUBO DN75 LMIN=150</t>
-  </si>
-  <si>
     <t>30000153</t>
   </si>
   <si>
@@ -487,12 +481,6 @@
     <t>CURVA 90 GR PVC PB JE/JERI ESG DN 100</t>
   </si>
   <si>
-    <t>30008324</t>
-  </si>
-  <si>
-    <t>CURVA 90GR FF BOLSAS JE DN200</t>
-  </si>
-  <si>
     <t>30000757</t>
   </si>
   <si>
@@ -907,12 +895,6 @@
     <t>LUVA CORRER FF C/BOLSAS JM DN50</t>
   </si>
   <si>
-    <t>30005924</t>
-  </si>
-  <si>
-    <t>LUVA CORRER FF C/BOLSAS JM DN75</t>
-  </si>
-  <si>
     <t>30002812</t>
   </si>
   <si>
@@ -1018,6 +1000,12 @@
     <t>REDUC CONC 225X110 TERMOF. PE 100 SDR 11</t>
   </si>
   <si>
+    <t>30001590</t>
+  </si>
+  <si>
+    <t>REDUCAO CONC ELETROF - DE 110 X 63</t>
+  </si>
+  <si>
     <t>30008609</t>
   </si>
   <si>
@@ -1081,12 +1069,6 @@
     <t>SELIM 90 G PVC DN 300 X 100 ENCAIXE</t>
   </si>
   <si>
-    <t>30007132</t>
-  </si>
-  <si>
-    <t>SELIM AJUST TUBO PVC E CER DN 150X100</t>
-  </si>
-  <si>
     <t>30003416</t>
   </si>
   <si>
@@ -1213,12 +1195,6 @@
     <t>TE FF BOLSA JE2GS FLG DN150X75 PN10/16</t>
   </si>
   <si>
-    <t>30007308</t>
-  </si>
-  <si>
-    <t>TE FF C/FLANGES DN 200 X 200 PN 16</t>
-  </si>
-  <si>
     <t>30003715</t>
   </si>
   <si>
@@ -1321,15 +1297,21 @@
     <t>TE RED. ELETROF DE 315 X 225 PE 100</t>
   </si>
   <si>
+    <t>30001797</t>
+  </si>
+  <si>
+    <t>TUBO FF K7 PONTA E BOLSA JE2GS DN200</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>30003896</t>
   </si>
   <si>
     <t>TUBO FF K7 PONTA E BOLSA JE2GS DN300</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>30000849</t>
   </si>
   <si>
@@ -1562,12 +1544,6 @@
   </si>
   <si>
     <t>VALV GAV CM REV ELAST FL CAB DN 100</t>
-  </si>
-  <si>
-    <t>30007809</t>
-  </si>
-  <si>
-    <t>VALV GAV CM REV ELAST FL CAB DN 200 PN10</t>
   </si>
   <si>
     <t>30008830</t>
@@ -1740,7 +1716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H265"/>
+  <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1760,28 +1736,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1879,13 +1855,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="2">
-        <v>3.000</v>
+        <v>4.000</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="3">
-        <v>3855.50</v>
+        <v>5140.66</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1983,13 +1959,13 @@
         <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>14.000</v>
+        <v>8.000</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>3423.49</v>
+        <v>1582.95</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2009,13 +1985,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="2">
-        <v>8.000</v>
+        <v>3.000</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="3">
-        <v>1582.95</v>
+        <v>750.47</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2035,13 +2011,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <v>750.47</v>
+        <v>153.40</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2061,13 +2037,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>1.000</v>
+        <v>15.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>153.40</v>
+        <v>313.91</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2087,13 +2063,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="2">
-        <v>15.000</v>
+        <v>13.000</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>313.91</v>
+        <v>1268.55</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2113,13 +2089,13 @@
         <v>29</v>
       </c>
       <c r="F14" s="2">
-        <v>9.000</v>
+        <v>17.000</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="3">
-        <v>878.23</v>
+        <v>647.33</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2139,13 +2115,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="2">
-        <v>19.000</v>
+        <v>128.000</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="3">
-        <v>723.49</v>
+        <v>12115.77</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2165,13 +2141,13 @@
         <v>33</v>
       </c>
       <c r="F16" s="2">
-        <v>129.000</v>
+        <v>18.000</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="3">
-        <v>12210.43</v>
+        <v>78.03</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2191,13 +2167,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>18.000</v>
+        <v>620.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>78.03</v>
+        <v>1271.00</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2217,13 +2193,13 @@
         <v>37</v>
       </c>
       <c r="F18" s="2">
-        <v>620.000</v>
+        <v>447.000</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3">
-        <v>1271.00</v>
+        <v>326.45</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2243,13 +2219,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="2">
-        <v>447.000</v>
+        <v>98.000</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="3">
-        <v>326.45</v>
+        <v>125.14</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2269,13 +2245,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="2">
-        <v>98.000</v>
+        <v>136.000</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>125.14</v>
+        <v>607.32</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2295,13 +2271,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="2">
-        <v>136.000</v>
+        <v>60.000</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>607.32</v>
+        <v>227.27</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2321,13 +2297,13 @@
         <v>45</v>
       </c>
       <c r="F22" s="2">
-        <v>60.000</v>
+        <v>4.000</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>227.27</v>
+        <v>48.64</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2347,13 +2323,13 @@
         <v>47</v>
       </c>
       <c r="F23" s="2">
-        <v>4.000</v>
+        <v>11.000</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>48.64</v>
+        <v>6222.91</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2373,13 +2349,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="2">
-        <v>11.000</v>
+        <v>324.000</v>
       </c>
       <c r="G24" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>6222.91</v>
+        <v>27666.50</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2399,13 +2375,13 @@
         <v>51</v>
       </c>
       <c r="F25" s="2">
-        <v>324.000</v>
+        <v>113.000</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="3">
-        <v>27666.50</v>
+        <v>20496.57</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2425,13 +2401,13 @@
         <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>113.000</v>
+        <v>9.000</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
-        <v>20496.57</v>
+        <v>380.14</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2451,13 +2427,13 @@
         <v>55</v>
       </c>
       <c r="F27" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="3">
-        <v>380.14</v>
+        <v>61.38</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2477,13 +2453,13 @@
         <v>57</v>
       </c>
       <c r="F28" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="3">
-        <v>61.38</v>
+        <v>103.20</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2503,13 +2479,13 @@
         <v>59</v>
       </c>
       <c r="F29" s="2">
-        <v>4.000</v>
+        <v>2.000</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="3">
-        <v>103.20</v>
+        <v>197.65</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2529,13 +2505,13 @@
         <v>61</v>
       </c>
       <c r="F30" s="2">
-        <v>2.000</v>
+        <v>3.000</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="3">
-        <v>197.65</v>
+        <v>463.99</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2555,13 +2531,13 @@
         <v>63</v>
       </c>
       <c r="F31" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>463.99</v>
+        <v>542.21</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2581,13 +2557,13 @@
         <v>65</v>
       </c>
       <c r="F32" s="2">
-        <v>2.000</v>
+        <v>10.000</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>542.21</v>
+        <v>201.79</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2607,13 +2583,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>10.000</v>
+        <v>8.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>201.79</v>
+        <v>460.48</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2633,13 +2609,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="2">
-        <v>8.000</v>
+        <v>13.000</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="3">
-        <v>460.48</v>
+        <v>526.30</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2659,13 +2635,13 @@
         <v>71</v>
       </c>
       <c r="F35" s="2">
-        <v>13.000</v>
+        <v>14.000</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3">
-        <v>526.30</v>
+        <v>630.14</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2685,13 +2661,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>14.000</v>
+        <v>16.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>630.14</v>
+        <v>520.62</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2711,13 +2687,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>16.000</v>
+        <v>5.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>520.62</v>
+        <v>279.52</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2737,13 +2713,13 @@
         <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="3">
-        <v>503.16</v>
+        <v>17.78</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2763,13 +2739,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>1.000</v>
+        <v>154.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>17.78</v>
+        <v>7234.15</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2789,13 +2765,13 @@
         <v>81</v>
       </c>
       <c r="F40" s="2">
-        <v>163.000</v>
+        <v>1.000</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="3">
-        <v>7656.91</v>
+        <v>1940.18</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2815,13 +2791,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>1.000</v>
+        <v>365.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>1940.18</v>
+        <v>10386.52</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2841,13 +2817,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>356.000</v>
+        <v>103.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>10130.42</v>
+        <v>16330.14</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2867,13 +2843,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>106.000</v>
+        <v>5.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>16805.77</v>
+        <v>2793.87</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2893,13 +2869,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>15.000</v>
+        <v>54.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>8381.62</v>
+        <v>4760.46</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2919,13 +2895,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>58.000</v>
+        <v>94.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>5113.09</v>
+        <v>17854.87</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2945,13 +2921,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>40.000</v>
+        <v>46.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>7597.83</v>
+        <v>2898.44</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2971,13 +2947,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>46.000</v>
+        <v>2.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>2898.44</v>
+        <v>603.23</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2997,13 +2973,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>2.000</v>
+        <v>14.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>603.23</v>
+        <v>1963.52</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3023,13 +2999,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>14.000</v>
+        <v>16.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>1963.52</v>
+        <v>3348.74</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3049,13 +3025,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>9.000</v>
+        <v>8.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>1883.67</v>
+        <v>2352.96</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3075,13 +3051,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>8.000</v>
+        <v>9.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>2352.96</v>
+        <v>3592.71</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3101,13 +3077,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>3592.71</v>
+        <v>863.17</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3127,13 +3103,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>863.17</v>
+        <v>295.57</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3153,13 +3129,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>3.000</v>
+        <v>917.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>295.57</v>
+        <v>8321.58</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3179,13 +3155,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>1057.000</v>
+        <v>37.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>9591.96</v>
+        <v>593.09</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3205,13 +3181,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>37.000</v>
+        <v>3514.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>593.09</v>
+        <v>36111.64</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3231,13 +3207,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>3632.000</v>
+        <v>11.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>37329.70</v>
+        <v>380.69</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3257,13 +3233,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>11.000</v>
+        <v>8.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>380.69</v>
+        <v>297.38</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3283,13 +3259,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>9.000</v>
+        <v>5.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>334.55</v>
+        <v>1454.70</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3309,13 +3285,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>5.000</v>
+        <v>23.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>1454.70</v>
+        <v>1071.88</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3335,13 +3311,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>23.000</v>
+        <v>11.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>1071.88</v>
+        <v>1357.53</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3361,13 +3337,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>11.000</v>
+        <v>16.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>1357.53</v>
+        <v>902.16</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3387,13 +3363,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>16.000</v>
+        <v>26.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>902.16</v>
+        <v>2051.47</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3413,13 +3389,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>26.000</v>
+        <v>19.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>2051.47</v>
+        <v>565.15</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3439,13 +3415,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>19.000</v>
+        <v>36.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>565.15</v>
+        <v>2051.36</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3465,13 +3441,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>36.000</v>
+        <v>4.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>2051.36</v>
+        <v>606.42</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3491,13 +3467,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>606.42</v>
+        <v>1448.47</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3517,13 +3493,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>1.000</v>
+        <v>1480.000</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>1448.47</v>
+        <v>7458.41</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3543,13 +3519,13 @@
         <v>139</v>
       </c>
       <c r="F69" s="2">
-        <v>1480.000</v>
+        <v>23.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>7534.31</v>
+        <v>1396.09</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3569,13 +3545,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>23.000</v>
+        <v>47.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>1396.09</v>
+        <v>6987.50</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3595,13 +3571,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>47.000</v>
+        <v>180.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>6987.50</v>
+        <v>1598.51</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3621,13 +3597,13 @@
         <v>145</v>
       </c>
       <c r="F72" s="2">
-        <v>180.000</v>
+        <v>13.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>1598.51</v>
+        <v>738.14</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3647,13 +3623,13 @@
         <v>147</v>
       </c>
       <c r="F73" s="2">
-        <v>13.000</v>
+        <v>6.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>738.14</v>
+        <v>344.01</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3673,13 +3649,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>6.000</v>
+        <v>18.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>344.01</v>
+        <v>1877.58</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3699,13 +3675,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>18.000</v>
+        <v>46.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>1877.58</v>
+        <v>4738.33</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3725,13 +3701,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>46.000</v>
+        <v>2.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>4738.33</v>
+        <v>495.95</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3751,13 +3727,13 @@
         <v>155</v>
       </c>
       <c r="F77" s="2">
-        <v>2.000</v>
+        <v>71.000</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>495.95</v>
+        <v>1319.15</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3777,13 +3753,13 @@
         <v>157</v>
       </c>
       <c r="F78" s="2">
-        <v>72.000</v>
+        <v>1.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>1337.73</v>
+        <v>86.93</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3803,13 +3779,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>1.000</v>
+        <v>1148.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>131.57</v>
+        <v>7055.88</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3829,13 +3805,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>86.93</v>
+        <v>207.19</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3855,13 +3831,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>1225.000</v>
+        <v>2865.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>7529.25</v>
+        <v>74626.01</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3881,13 +3857,13 @@
         <v>165</v>
       </c>
       <c r="F82" s="2">
-        <v>20.000</v>
+        <v>3.000</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>218.09</v>
+        <v>229.84</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3907,13 +3883,13 @@
         <v>167</v>
       </c>
       <c r="F83" s="2">
-        <v>2981.000</v>
+        <v>3.000</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>77647.61</v>
+        <v>651.71</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3933,13 +3909,13 @@
         <v>169</v>
       </c>
       <c r="F84" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>383.07</v>
+        <v>1263.43</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3959,13 +3935,13 @@
         <v>171</v>
       </c>
       <c r="F85" s="2">
-        <v>3.000</v>
+        <v>14.000</v>
       </c>
       <c r="G85" t="s">
         <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>651.71</v>
+        <v>2597.51</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -3985,13 +3961,13 @@
         <v>173</v>
       </c>
       <c r="F86" s="2">
-        <v>3.000</v>
+        <v>4.000</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>1263.43</v>
+        <v>1008.05</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4011,13 +3987,13 @@
         <v>175</v>
       </c>
       <c r="F87" s="2">
-        <v>12.000</v>
+        <v>14.000</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>2226.44</v>
+        <v>1572.63</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4037,13 +4013,13 @@
         <v>177</v>
       </c>
       <c r="F88" s="2">
-        <v>4.000</v>
+        <v>10.000</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>1008.05</v>
+        <v>4255.32</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4063,13 +4039,13 @@
         <v>179</v>
       </c>
       <c r="F89" s="2">
-        <v>14.000</v>
+        <v>2.000</v>
       </c>
       <c r="G89" t="s">
         <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>1572.63</v>
+        <v>3671.99</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4089,13 +4065,13 @@
         <v>181</v>
       </c>
       <c r="F90" s="2">
-        <v>10.000</v>
+        <v>134.000</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>4255.32</v>
+        <v>5051.13</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4121,7 +4097,7 @@
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>3671.99</v>
+        <v>560.27</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -4141,13 +4117,13 @@
         <v>185</v>
       </c>
       <c r="F92" s="2">
-        <v>134.000</v>
+        <v>36.000</v>
       </c>
       <c r="G92" t="s">
         <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>5051.13</v>
+        <v>3294.45</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -4167,13 +4143,13 @@
         <v>187</v>
       </c>
       <c r="F93" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G93" t="s">
         <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>560.27</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -4193,13 +4169,13 @@
         <v>189</v>
       </c>
       <c r="F94" s="2">
-        <v>36.000</v>
+        <v>10.000</v>
       </c>
       <c r="G94" t="s">
         <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>3294.45</v>
+        <v>18133.05</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4219,13 +4195,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>1.000</v>
+        <v>223.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>2.97</v>
+        <v>18877.36</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4245,13 +4221,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>10.000</v>
+        <v>2248.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>18133.05</v>
+        <v>316120.96</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4271,13 +4247,13 @@
         <v>195</v>
       </c>
       <c r="F97" s="2">
-        <v>233.000</v>
+        <v>1.000</v>
       </c>
       <c r="G97" t="s">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>19723.88</v>
+        <v>2980.59</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -4297,13 +4273,13 @@
         <v>197</v>
       </c>
       <c r="F98" s="2">
-        <v>2341.000</v>
+        <v>1.000</v>
       </c>
       <c r="G98" t="s">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>329199.71</v>
+        <v>4463.84</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -4323,13 +4299,13 @@
         <v>199</v>
       </c>
       <c r="F99" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G99" t="s">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>2980.59</v>
+        <v>1598.30</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4349,13 +4325,13 @@
         <v>201</v>
       </c>
       <c r="F100" s="2">
-        <v>1.000</v>
+        <v>19.000</v>
       </c>
       <c r="G100" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>4463.84</v>
+        <v>23432.75</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -4375,13 +4351,13 @@
         <v>203</v>
       </c>
       <c r="F101" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G101" t="s">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>1598.30</v>
+        <v>11241.86</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -4401,13 +4377,13 @@
         <v>205</v>
       </c>
       <c r="F102" s="2">
-        <v>19.000</v>
+        <v>6.000</v>
       </c>
       <c r="G102" t="s">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>23432.75</v>
+        <v>2252.65</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4427,13 +4403,13 @@
         <v>207</v>
       </c>
       <c r="F103" s="2">
-        <v>7.000</v>
+        <v>1.000</v>
       </c>
       <c r="G103" t="s">
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>13115.50</v>
+        <v>279.59</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4453,13 +4429,13 @@
         <v>209</v>
       </c>
       <c r="F104" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>1877.21</v>
+        <v>740.97</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -4479,13 +4455,13 @@
         <v>211</v>
       </c>
       <c r="F105" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G105" t="s">
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>279.59</v>
+        <v>902.80</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -4511,7 +4487,7 @@
         <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>740.97</v>
+        <v>994.54</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -4537,7 +4513,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>902.80</v>
+        <v>1033.65</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4563,7 +4539,7 @@
         <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>994.54</v>
+        <v>1166.57</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4583,13 +4559,13 @@
         <v>219</v>
       </c>
       <c r="F109" s="2">
-        <v>2.000</v>
+        <v>8.000</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>1033.65</v>
+        <v>2825.06</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4609,13 +4585,13 @@
         <v>221</v>
       </c>
       <c r="F110" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G110" t="s">
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>1166.57</v>
+        <v>91.20</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4635,13 +4611,13 @@
         <v>223</v>
       </c>
       <c r="F111" s="2">
-        <v>8.000</v>
+        <v>2.000</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>2825.06</v>
+        <v>719.47</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4661,13 +4637,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>1.000</v>
+        <v>651.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>91.20</v>
+        <v>24159.17</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4687,13 +4663,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>2.000</v>
+        <v>349.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>719.47</v>
+        <v>22813.65</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4713,13 +4689,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>662.000</v>
+        <v>920.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>24567.39</v>
+        <v>30310.68</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4739,13 +4715,13 @@
         <v>231</v>
       </c>
       <c r="F115" s="2">
-        <v>349.000</v>
+        <v>170.000</v>
       </c>
       <c r="G115" t="s">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>22813.65</v>
+        <v>8735.16</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -4765,13 +4741,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>924.000</v>
+        <v>24.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>30442.58</v>
+        <v>2538.29</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4791,13 +4767,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>170.000</v>
+        <v>49.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>8735.16</v>
+        <v>1654.46</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4817,13 +4793,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>29.000</v>
+        <v>9.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>2955.61</v>
+        <v>1675.75</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4843,13 +4819,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>49.000</v>
+        <v>11810.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>1654.46</v>
+        <v>45886.97</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -4869,13 +4845,13 @@
         <v>241</v>
       </c>
       <c r="F120" s="2">
-        <v>9.000</v>
+        <v>2.000</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>1675.75</v>
+        <v>2463.85</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -4895,13 +4871,13 @@
         <v>243</v>
       </c>
       <c r="F121" s="2">
-        <v>12137.000</v>
+        <v>2.000</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>47112.69</v>
+        <v>4533.88</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -4921,13 +4897,13 @@
         <v>245</v>
       </c>
       <c r="F122" s="2">
-        <v>2.000</v>
+        <v>4.000</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>2463.85</v>
+        <v>6385.34</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4947,13 +4923,13 @@
         <v>247</v>
       </c>
       <c r="F123" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G123" t="s">
         <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>4533.88</v>
+        <v>12368.67</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -4973,13 +4949,13 @@
         <v>249</v>
       </c>
       <c r="F124" s="2">
-        <v>4.000</v>
+        <v>3.000</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>6385.34</v>
+        <v>3260.53</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4999,13 +4975,13 @@
         <v>251</v>
       </c>
       <c r="F125" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G125" t="s">
         <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>12368.67</v>
+        <v>3527.49</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5031,7 +5007,7 @@
         <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>3260.53</v>
+        <v>6294.26</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5051,13 +5027,13 @@
         <v>255</v>
       </c>
       <c r="F127" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G127" t="s">
         <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>3527.49</v>
+        <v>4585.00</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -5077,13 +5053,13 @@
         <v>257</v>
       </c>
       <c r="F128" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G128" t="s">
         <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>6294.26</v>
+        <v>14225.45</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5103,13 +5079,13 @@
         <v>259</v>
       </c>
       <c r="F129" s="2">
-        <v>1.000</v>
+        <v>35.000</v>
       </c>
       <c r="G129" t="s">
         <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>4585.00</v>
+        <v>50482.77</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5129,13 +5105,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>2.000</v>
+        <v>554.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>14225.45</v>
+        <v>3136.11</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5155,13 +5131,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>36.000</v>
+        <v>171.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>51925.14</v>
+        <v>1405.96</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5181,13 +5157,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>554.000</v>
+        <v>91.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>3136.11</v>
+        <v>1426.69</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5207,13 +5183,13 @@
         <v>267</v>
       </c>
       <c r="F133" s="2">
-        <v>226.000</v>
+        <v>110.000</v>
       </c>
       <c r="G133" t="s">
         <v>5</v>
       </c>
       <c r="H133" s="3">
-        <v>1858.16</v>
+        <v>1499.69</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5233,13 +5209,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>91.000</v>
+        <v>78.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>1426.69</v>
+        <v>2380.78</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5259,13 +5235,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>110.000</v>
+        <v>26.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>1499.69</v>
+        <v>3249.51</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5285,13 +5261,13 @@
         <v>273</v>
       </c>
       <c r="F136" s="2">
-        <v>78.000</v>
+        <v>1.000</v>
       </c>
       <c r="G136" t="s">
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>2380.78</v>
+        <v>194.13</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5311,13 +5287,13 @@
         <v>275</v>
       </c>
       <c r="F137" s="2">
-        <v>26.000</v>
+        <v>2.000</v>
       </c>
       <c r="G137" t="s">
         <v>5</v>
       </c>
       <c r="H137" s="3">
-        <v>3249.51</v>
+        <v>159.25</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5337,13 +5313,13 @@
         <v>277</v>
       </c>
       <c r="F138" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G138" t="s">
         <v>5</v>
       </c>
       <c r="H138" s="3">
-        <v>194.13</v>
+        <v>499.74</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -5363,13 +5339,13 @@
         <v>279</v>
       </c>
       <c r="F139" s="2">
-        <v>2.000</v>
+        <v>41.000</v>
       </c>
       <c r="G139" t="s">
         <v>5</v>
       </c>
       <c r="H139" s="3">
-        <v>159.25</v>
+        <v>2975.17</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -5389,13 +5365,13 @@
         <v>281</v>
       </c>
       <c r="F140" s="2">
-        <v>2.000</v>
+        <v>16.000</v>
       </c>
       <c r="G140" t="s">
         <v>5</v>
       </c>
       <c r="H140" s="3">
-        <v>499.74</v>
+        <v>2435.67</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -5415,13 +5391,13 @@
         <v>283</v>
       </c>
       <c r="F141" s="2">
-        <v>41.000</v>
+        <v>12.000</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
       </c>
       <c r="H141" s="3">
-        <v>2975.17</v>
+        <v>5671.40</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -5441,13 +5417,13 @@
         <v>285</v>
       </c>
       <c r="F142" s="2">
-        <v>12.000</v>
+        <v>8.000</v>
       </c>
       <c r="G142" t="s">
         <v>5</v>
       </c>
       <c r="H142" s="3">
-        <v>1826.75</v>
+        <v>5567.25</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -5467,13 +5443,13 @@
         <v>287</v>
       </c>
       <c r="F143" s="2">
-        <v>12.000</v>
+        <v>6.000</v>
       </c>
       <c r="G143" t="s">
         <v>5</v>
       </c>
       <c r="H143" s="3">
-        <v>5671.40</v>
+        <v>5624.37</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -5493,13 +5469,13 @@
         <v>289</v>
       </c>
       <c r="F144" s="2">
-        <v>8.000</v>
+        <v>5.000</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
       </c>
       <c r="H144" s="3">
-        <v>5567.25</v>
+        <v>5802.02</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5519,13 +5495,13 @@
         <v>291</v>
       </c>
       <c r="F145" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G145" t="s">
         <v>5</v>
       </c>
       <c r="H145" s="3">
-        <v>5624.37</v>
+        <v>6826.78</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -5545,13 +5521,13 @@
         <v>293</v>
       </c>
       <c r="F146" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
       </c>
       <c r="H146" s="3">
-        <v>5802.02</v>
+        <v>1014.32</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -5571,13 +5547,13 @@
         <v>295</v>
       </c>
       <c r="F147" s="2">
-        <v>4.000</v>
+        <v>16.000</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
       </c>
       <c r="H147" s="3">
-        <v>6826.78</v>
+        <v>4737.64</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -5597,13 +5573,13 @@
         <v>297</v>
       </c>
       <c r="F148" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
       </c>
       <c r="H148" s="3">
-        <v>1690.54</v>
+        <v>108.47</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -5623,13 +5599,13 @@
         <v>299</v>
       </c>
       <c r="F149" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
       </c>
       <c r="H149" s="3">
-        <v>547.47</v>
+        <v>628.62</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5649,13 +5625,13 @@
         <v>301</v>
       </c>
       <c r="F150" s="2">
-        <v>16.000</v>
+        <v>30.000</v>
       </c>
       <c r="G150" t="s">
         <v>5</v>
       </c>
       <c r="H150" s="3">
-        <v>4737.64</v>
+        <v>181.79</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5675,13 +5651,13 @@
         <v>303</v>
       </c>
       <c r="F151" s="2">
-        <v>3.000</v>
+        <v>6.000</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
       </c>
       <c r="H151" s="3">
-        <v>162.71</v>
+        <v>98.34</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5701,13 +5677,13 @@
         <v>305</v>
       </c>
       <c r="F152" s="2">
-        <v>3.000</v>
+        <v>10.000</v>
       </c>
       <c r="G152" t="s">
         <v>5</v>
       </c>
       <c r="H152" s="3">
-        <v>314.31</v>
+        <v>374.15</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5727,13 +5703,13 @@
         <v>307</v>
       </c>
       <c r="F153" s="2">
-        <v>30.000</v>
+        <v>468.000</v>
       </c>
       <c r="G153" t="s">
         <v>5</v>
       </c>
       <c r="H153" s="3">
-        <v>181.80</v>
+        <v>2071.35</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5753,13 +5729,13 @@
         <v>309</v>
       </c>
       <c r="F154" s="2">
-        <v>6.000</v>
+        <v>16.000</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
       </c>
       <c r="H154" s="3">
-        <v>98.34</v>
+        <v>1467.58</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5779,13 +5755,13 @@
         <v>311</v>
       </c>
       <c r="F155" s="2">
-        <v>10.000</v>
+        <v>1.000</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
       </c>
       <c r="H155" s="3">
-        <v>374.15</v>
+        <v>135.35</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5805,13 +5781,13 @@
         <v>313</v>
       </c>
       <c r="F156" s="2">
-        <v>468.000</v>
+        <v>25.000</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
       </c>
       <c r="H156" s="3">
-        <v>2071.35</v>
+        <v>116.25</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5831,13 +5807,13 @@
         <v>315</v>
       </c>
       <c r="F157" s="2">
-        <v>16.000</v>
+        <v>8.000</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
       </c>
       <c r="H157" s="3">
-        <v>1467.58</v>
+        <v>955.65</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5857,13 +5833,13 @@
         <v>317</v>
       </c>
       <c r="F158" s="2">
-        <v>1.000</v>
+        <v>32.000</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
       </c>
       <c r="H158" s="3">
-        <v>135.35</v>
+        <v>3368.16</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5883,13 +5859,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>25.000</v>
+        <v>47.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>116.25</v>
+        <v>6275.29</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5909,13 +5885,13 @@
         <v>321</v>
       </c>
       <c r="F160" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
       </c>
       <c r="H160" s="3">
-        <v>955.65</v>
+        <v>40.71</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5932,16 +5908,16 @@
         <v>322</v>
       </c>
       <c r="E161" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F161" s="2">
-        <v>32.000</v>
+        <v>4.000</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
       </c>
       <c r="H161" s="3">
-        <v>3368.16</v>
+        <v>317.81</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5955,19 +5931,19 @@
         <v>2</v>
       </c>
       <c r="D162" t="s">
+        <v>323</v>
+      </c>
+      <c r="E162" t="s">
         <v>324</v>
       </c>
-      <c r="E162" t="s">
-        <v>325</v>
-      </c>
       <c r="F162" s="2">
-        <v>51.000</v>
+        <v>6.000</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
       </c>
       <c r="H162" s="3">
-        <v>6809.36</v>
+        <v>483.20</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5981,19 +5957,19 @@
         <v>2</v>
       </c>
       <c r="D163" t="s">
+        <v>325</v>
+      </c>
+      <c r="E163" t="s">
         <v>326</v>
       </c>
-      <c r="E163" t="s">
-        <v>327</v>
-      </c>
       <c r="F163" s="2">
-        <v>1.000</v>
+        <v>6.000</v>
       </c>
       <c r="G163" t="s">
         <v>5</v>
       </c>
       <c r="H163" s="3">
-        <v>40.71</v>
+        <v>45.92</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -6007,19 +5983,19 @@
         <v>2</v>
       </c>
       <c r="D164" t="s">
+        <v>327</v>
+      </c>
+      <c r="E164" t="s">
         <v>328</v>
       </c>
-      <c r="E164" t="s">
-        <v>327</v>
-      </c>
       <c r="F164" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G164" t="s">
         <v>5</v>
       </c>
       <c r="H164" s="3">
-        <v>317.81</v>
+        <v>303.12</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -6039,13 +6015,13 @@
         <v>330</v>
       </c>
       <c r="F165" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G165" t="s">
         <v>5</v>
       </c>
       <c r="H165" s="3">
-        <v>483.20</v>
+        <v>120.27</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -6065,13 +6041,13 @@
         <v>332</v>
       </c>
       <c r="F166" s="2">
-        <v>6.000</v>
+        <v>8.000</v>
       </c>
       <c r="G166" t="s">
         <v>5</v>
       </c>
       <c r="H166" s="3">
-        <v>45.92</v>
+        <v>1128.58</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -6091,13 +6067,13 @@
         <v>334</v>
       </c>
       <c r="F167" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G167" t="s">
         <v>5</v>
       </c>
       <c r="H167" s="3">
-        <v>303.12</v>
+        <v>1054.62</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -6117,13 +6093,13 @@
         <v>336</v>
       </c>
       <c r="F168" s="2">
-        <v>8.000</v>
+        <v>6.000</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
       </c>
       <c r="H168" s="3">
-        <v>1128.58</v>
+        <v>362.54</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -6143,13 +6119,13 @@
         <v>338</v>
       </c>
       <c r="F169" s="2">
-        <v>3.000</v>
+        <v>2.000</v>
       </c>
       <c r="G169" t="s">
         <v>5</v>
       </c>
       <c r="H169" s="3">
-        <v>1054.62</v>
+        <v>412.45</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -6169,13 +6145,13 @@
         <v>340</v>
       </c>
       <c r="F170" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
       </c>
       <c r="H170" s="3">
-        <v>362.54</v>
+        <v>24.27</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -6195,13 +6171,13 @@
         <v>342</v>
       </c>
       <c r="F171" s="2">
-        <v>2.000</v>
+        <v>9.000</v>
       </c>
       <c r="G171" t="s">
         <v>5</v>
       </c>
       <c r="H171" s="3">
-        <v>412.45</v>
+        <v>214.33</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -6221,13 +6197,13 @@
         <v>344</v>
       </c>
       <c r="F172" s="2">
-        <v>1.000</v>
+        <v>15.000</v>
       </c>
       <c r="G172" t="s">
         <v>5</v>
       </c>
       <c r="H172" s="3">
-        <v>24.27</v>
+        <v>3032.79</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -6247,13 +6223,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>9.000</v>
+        <v>2456.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>214.33</v>
+        <v>45988.60</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6273,13 +6249,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>15.000</v>
+        <v>215651.000</v>
       </c>
       <c r="G174" t="s">
-        <v>5</v>
+        <v>349</v>
       </c>
       <c r="H174" s="3">
-        <v>3032.79</v>
+        <v>327871.67</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6293,19 +6269,19 @@
         <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E175" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F175" s="2">
-        <v>2424.000</v>
+        <v>100.000</v>
       </c>
       <c r="G175" t="s">
         <v>5</v>
       </c>
       <c r="H175" s="3">
-        <v>45389.40</v>
+        <v>3564.38</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6319,19 +6295,19 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E176" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>217001.000</v>
+        <v>615.000</v>
       </c>
       <c r="G176" t="s">
-        <v>353</v>
+        <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>329918.19</v>
+        <v>107389.35</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6351,13 +6327,13 @@
         <v>355</v>
       </c>
       <c r="F177" s="2">
-        <v>100.000</v>
+        <v>13.000</v>
       </c>
       <c r="G177" t="s">
         <v>5</v>
       </c>
       <c r="H177" s="3">
-        <v>3564.38</v>
+        <v>2264.65</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6377,13 +6353,13 @@
         <v>357</v>
       </c>
       <c r="F178" s="2">
-        <v>1.000</v>
+        <v>11.000</v>
       </c>
       <c r="G178" t="s">
         <v>5</v>
       </c>
       <c r="H178" s="3">
-        <v>191.34</v>
+        <v>145.79</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6403,13 +6379,13 @@
         <v>359</v>
       </c>
       <c r="F179" s="2">
-        <v>636.000</v>
+        <v>22.000</v>
       </c>
       <c r="G179" t="s">
         <v>5</v>
       </c>
       <c r="H179" s="3">
-        <v>111056.32</v>
+        <v>10363.87</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6429,13 +6405,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>13.000</v>
+        <v>84.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>2264.65</v>
+        <v>38976.93</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6455,13 +6431,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>11.000</v>
+        <v>46.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>145.79</v>
+        <v>2809.22</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6481,13 +6457,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>22.000</v>
+        <v>75.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>10363.87</v>
+        <v>10771.45</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6507,13 +6483,13 @@
         <v>367</v>
       </c>
       <c r="F183" s="2">
-        <v>85.000</v>
+        <v>1.000</v>
       </c>
       <c r="G183" t="s">
         <v>5</v>
       </c>
       <c r="H183" s="3">
-        <v>39428.52</v>
+        <v>1218.18</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6533,13 +6509,13 @@
         <v>369</v>
       </c>
       <c r="F184" s="2">
-        <v>49.000</v>
+        <v>1.000</v>
       </c>
       <c r="G184" t="s">
         <v>5</v>
       </c>
       <c r="H184" s="3">
-        <v>2992.43</v>
+        <v>1720.00</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6559,13 +6535,13 @@
         <v>371</v>
       </c>
       <c r="F185" s="2">
-        <v>75.000</v>
+        <v>28.000</v>
       </c>
       <c r="G185" t="s">
         <v>5</v>
       </c>
       <c r="H185" s="3">
-        <v>10771.45</v>
+        <v>1119.31</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6585,13 +6561,13 @@
         <v>373</v>
       </c>
       <c r="F186" s="2">
-        <v>1.000</v>
+        <v>202.000</v>
       </c>
       <c r="G186" t="s">
         <v>5</v>
       </c>
       <c r="H186" s="3">
-        <v>1218.18</v>
+        <v>6748.61</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6611,13 +6587,13 @@
         <v>375</v>
       </c>
       <c r="F187" s="2">
-        <v>1.000</v>
+        <v>484.000</v>
       </c>
       <c r="G187" t="s">
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>1720.00</v>
+        <v>7566.20</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6637,13 +6613,13 @@
         <v>377</v>
       </c>
       <c r="F188" s="2">
-        <v>28.000</v>
+        <v>59.000</v>
       </c>
       <c r="G188" t="s">
         <v>5</v>
       </c>
       <c r="H188" s="3">
-        <v>1119.31</v>
+        <v>1003.06</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6663,13 +6639,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>202.000</v>
+        <v>509.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>6748.61</v>
+        <v>10312.34</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6689,13 +6665,13 @@
         <v>381</v>
       </c>
       <c r="F190" s="2">
-        <v>484.000</v>
+        <v>46.000</v>
       </c>
       <c r="G190" t="s">
         <v>5</v>
       </c>
       <c r="H190" s="3">
-        <v>7566.19</v>
+        <v>1068.40</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6715,13 +6691,13 @@
         <v>383</v>
       </c>
       <c r="F191" s="2">
-        <v>59.000</v>
+        <v>93.000</v>
       </c>
       <c r="G191" t="s">
         <v>5</v>
       </c>
       <c r="H191" s="3">
-        <v>1003.06</v>
+        <v>6626.71</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6741,13 +6717,13 @@
         <v>385</v>
       </c>
       <c r="F192" s="2">
-        <v>537.000</v>
+        <v>16.000</v>
       </c>
       <c r="G192" t="s">
         <v>5</v>
       </c>
       <c r="H192" s="3">
-        <v>10879.62</v>
+        <v>1789.69</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6767,13 +6743,13 @@
         <v>387</v>
       </c>
       <c r="F193" s="2">
-        <v>46.000</v>
+        <v>1.000</v>
       </c>
       <c r="G193" t="s">
         <v>5</v>
       </c>
       <c r="H193" s="3">
-        <v>1068.40</v>
+        <v>189.22</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -6793,13 +6769,13 @@
         <v>389</v>
       </c>
       <c r="F194" s="2">
-        <v>93.000</v>
+        <v>19.000</v>
       </c>
       <c r="G194" t="s">
         <v>5</v>
       </c>
       <c r="H194" s="3">
-        <v>6626.71</v>
+        <v>1201.67</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -6819,13 +6795,13 @@
         <v>391</v>
       </c>
       <c r="F195" s="2">
-        <v>16.000</v>
+        <v>244.000</v>
       </c>
       <c r="G195" t="s">
         <v>5</v>
       </c>
       <c r="H195" s="3">
-        <v>1789.69</v>
+        <v>16895.78</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -6845,13 +6821,13 @@
         <v>393</v>
       </c>
       <c r="F196" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G196" t="s">
         <v>5</v>
       </c>
       <c r="H196" s="3">
-        <v>189.22</v>
+        <v>651.09</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6871,13 +6847,13 @@
         <v>395</v>
       </c>
       <c r="F197" s="2">
-        <v>19.000</v>
+        <v>5.000</v>
       </c>
       <c r="G197" t="s">
         <v>5</v>
       </c>
       <c r="H197" s="3">
-        <v>1201.67</v>
+        <v>718.30</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -6897,13 +6873,13 @@
         <v>397</v>
       </c>
       <c r="F198" s="2">
-        <v>244.000</v>
+        <v>1.000</v>
       </c>
       <c r="G198" t="s">
         <v>5</v>
       </c>
       <c r="H198" s="3">
-        <v>16895.78</v>
+        <v>266.26</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -6923,13 +6899,13 @@
         <v>399</v>
       </c>
       <c r="F199" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G199" t="s">
         <v>5</v>
       </c>
       <c r="H199" s="3">
-        <v>651.09</v>
+        <v>257.36</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -6949,13 +6925,13 @@
         <v>401</v>
       </c>
       <c r="F200" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G200" t="s">
         <v>5</v>
       </c>
       <c r="H200" s="3">
-        <v>1125.55</v>
+        <v>961.64</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -6975,13 +6951,13 @@
         <v>403</v>
       </c>
       <c r="F201" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G201" t="s">
         <v>5</v>
       </c>
       <c r="H201" s="3">
-        <v>718.30</v>
+        <v>726.22</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -7001,13 +6977,13 @@
         <v>405</v>
       </c>
       <c r="F202" s="2">
-        <v>1.000</v>
+        <v>5.000</v>
       </c>
       <c r="G202" t="s">
         <v>5</v>
       </c>
       <c r="H202" s="3">
-        <v>266.26</v>
+        <v>662.53</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -7027,13 +7003,13 @@
         <v>407</v>
       </c>
       <c r="F203" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="G203" t="s">
         <v>5</v>
       </c>
       <c r="H203" s="3">
-        <v>257.36</v>
+        <v>537.99</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -7053,13 +7029,13 @@
         <v>409</v>
       </c>
       <c r="F204" s="2">
-        <v>2.000</v>
+        <v>7.000</v>
       </c>
       <c r="G204" t="s">
         <v>5</v>
       </c>
       <c r="H204" s="3">
-        <v>961.64</v>
+        <v>909.52</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -7079,13 +7055,13 @@
         <v>411</v>
       </c>
       <c r="F205" s="2">
-        <v>1.000</v>
+        <v>32.000</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
       </c>
       <c r="H205" s="3">
-        <v>726.22</v>
+        <v>4453.27</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -7105,13 +7081,13 @@
         <v>413</v>
       </c>
       <c r="F206" s="2">
-        <v>5.000</v>
+        <v>1.000</v>
       </c>
       <c r="G206" t="s">
         <v>5</v>
       </c>
       <c r="H206" s="3">
-        <v>662.53</v>
+        <v>4700.00</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -7131,13 +7107,13 @@
         <v>415</v>
       </c>
       <c r="F207" s="2">
-        <v>2.000</v>
+        <v>1.000</v>
       </c>
       <c r="G207" t="s">
         <v>5</v>
       </c>
       <c r="H207" s="3">
-        <v>537.99</v>
+        <v>8560.17</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -7157,13 +7133,13 @@
         <v>417</v>
       </c>
       <c r="F208" s="2">
-        <v>7.000</v>
+        <v>38.000</v>
       </c>
       <c r="G208" t="s">
         <v>5</v>
       </c>
       <c r="H208" s="3">
-        <v>909.52</v>
+        <v>481.25</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -7183,13 +7159,13 @@
         <v>419</v>
       </c>
       <c r="F209" s="2">
-        <v>32.000</v>
+        <v>5.000</v>
       </c>
       <c r="G209" t="s">
         <v>5</v>
       </c>
       <c r="H209" s="3">
-        <v>4453.27</v>
+        <v>116.72</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -7209,13 +7185,13 @@
         <v>421</v>
       </c>
       <c r="F210" s="2">
-        <v>1.000</v>
+        <v>17.000</v>
       </c>
       <c r="G210" t="s">
         <v>5</v>
       </c>
       <c r="H210" s="3">
-        <v>4700.00</v>
+        <v>646.00</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7235,13 +7211,13 @@
         <v>423</v>
       </c>
       <c r="F211" s="2">
-        <v>1.000</v>
+        <v>22.000</v>
       </c>
       <c r="G211" t="s">
         <v>5</v>
       </c>
       <c r="H211" s="3">
-        <v>8560.17</v>
+        <v>1452.69</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7261,13 +7237,13 @@
         <v>425</v>
       </c>
       <c r="F212" s="2">
-        <v>38.000</v>
+        <v>1.000</v>
       </c>
       <c r="G212" t="s">
         <v>5</v>
       </c>
       <c r="H212" s="3">
-        <v>481.25</v>
+        <v>685.11</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7287,13 +7263,13 @@
         <v>427</v>
       </c>
       <c r="F213" s="2">
-        <v>5.000</v>
+        <v>2.000</v>
       </c>
       <c r="G213" t="s">
         <v>5</v>
       </c>
       <c r="H213" s="3">
-        <v>116.72</v>
+        <v>8149.76</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7313,13 +7289,13 @@
         <v>429</v>
       </c>
       <c r="F214" s="2">
-        <v>17.000</v>
+        <v>1008.000</v>
       </c>
       <c r="G214" t="s">
-        <v>5</v>
+        <v>430</v>
       </c>
       <c r="H214" s="3">
-        <v>646.00</v>
+        <v>265339.36</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7333,19 +7309,19 @@
         <v>2</v>
       </c>
       <c r="D215" t="s">
+        <v>431</v>
+      </c>
+      <c r="E215" t="s">
+        <v>432</v>
+      </c>
+      <c r="F215" s="2">
+        <v>4.800</v>
+      </c>
+      <c r="G215" t="s">
         <v>430</v>
       </c>
-      <c r="E215" t="s">
-        <v>431</v>
-      </c>
-      <c r="F215" s="2">
-        <v>22.000</v>
-      </c>
-      <c r="G215" t="s">
-        <v>5</v>
-      </c>
       <c r="H215" s="3">
-        <v>1452.69</v>
+        <v>1822.34</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7359,19 +7335,19 @@
         <v>2</v>
       </c>
       <c r="D216" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E216" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F216" s="2">
-        <v>1.000</v>
+        <v>16.000</v>
       </c>
       <c r="G216" t="s">
-        <v>5</v>
+        <v>430</v>
       </c>
       <c r="H216" s="3">
-        <v>685.11</v>
+        <v>7011.29</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7385,19 +7361,19 @@
         <v>2</v>
       </c>
       <c r="D217" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E217" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F217" s="2">
-        <v>2.000</v>
+        <v>17.000</v>
       </c>
       <c r="G217" t="s">
-        <v>5</v>
+        <v>430</v>
       </c>
       <c r="H217" s="3">
-        <v>8149.76</v>
+        <v>2938.94</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7411,19 +7387,19 @@
         <v>2</v>
       </c>
       <c r="D218" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E218" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F218" s="2">
-        <v>4.800</v>
+        <v>161.140</v>
       </c>
       <c r="G218" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H218" s="3">
-        <v>1822.34</v>
+        <v>35004.10</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7443,13 +7419,13 @@
         <v>440</v>
       </c>
       <c r="F219" s="2">
-        <v>16.000</v>
+        <v>1.090</v>
       </c>
       <c r="G219" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H219" s="3">
-        <v>7011.29</v>
+        <v>250.66</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7469,13 +7445,13 @@
         <v>442</v>
       </c>
       <c r="F220" s="2">
-        <v>17.000</v>
+        <v>20.300</v>
       </c>
       <c r="G220" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H220" s="3">
-        <v>2938.94</v>
+        <v>6816.84</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7495,13 +7471,13 @@
         <v>444</v>
       </c>
       <c r="F221" s="2">
-        <v>162.140</v>
+        <v>13.000</v>
       </c>
       <c r="G221" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H221" s="3">
-        <v>35221.32</v>
+        <v>3437.72</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7521,13 +7497,13 @@
         <v>446</v>
       </c>
       <c r="F222" s="2">
-        <v>1.090</v>
+        <v>22.000</v>
       </c>
       <c r="G222" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H222" s="3">
-        <v>250.66</v>
+        <v>2084.93</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7547,13 +7523,13 @@
         <v>448</v>
       </c>
       <c r="F223" s="2">
-        <v>20.300</v>
+        <v>305.020</v>
       </c>
       <c r="G223" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H223" s="3">
-        <v>6816.84</v>
+        <v>3056.34</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -7573,13 +7549,13 @@
         <v>450</v>
       </c>
       <c r="F224" s="2">
-        <v>13.000</v>
+        <v>0.360</v>
       </c>
       <c r="G224" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H224" s="3">
-        <v>3437.72</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7599,13 +7575,13 @@
         <v>452</v>
       </c>
       <c r="F225" s="2">
-        <v>22.000</v>
+        <v>11.000</v>
       </c>
       <c r="G225" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H225" s="3">
-        <v>2084.93</v>
+        <v>974.64</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7625,13 +7601,13 @@
         <v>454</v>
       </c>
       <c r="F226" s="2">
-        <v>305.020</v>
+        <v>147.250</v>
       </c>
       <c r="G226" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H226" s="3">
-        <v>3056.34</v>
+        <v>24800.12</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -7651,13 +7627,13 @@
         <v>456</v>
       </c>
       <c r="F227" s="2">
-        <v>0.360</v>
+        <v>162.620</v>
       </c>
       <c r="G227" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H227" s="3">
-        <v>7.79</v>
+        <v>8485.75</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7677,13 +7653,13 @@
         <v>458</v>
       </c>
       <c r="F228" s="2">
-        <v>11.000</v>
+        <v>47.250</v>
       </c>
       <c r="G228" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H228" s="3">
-        <v>974.64</v>
+        <v>5148.59</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7703,13 +7679,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>150.000</v>
+        <v>19336.700</v>
       </c>
       <c r="G229" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H229" s="3">
-        <v>24001.36</v>
+        <v>43875.97</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7729,13 +7705,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>168.620</v>
+        <v>3213.960</v>
       </c>
       <c r="G230" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H230" s="3">
-        <v>8798.84</v>
+        <v>14105.06</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7755,13 +7731,13 @@
         <v>464</v>
       </c>
       <c r="F231" s="2">
-        <v>47.250</v>
+        <v>29.390</v>
       </c>
       <c r="G231" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H231" s="3">
-        <v>5148.59</v>
+        <v>15217.18</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7781,13 +7757,13 @@
         <v>466</v>
       </c>
       <c r="F232" s="2">
-        <v>20129.800</v>
+        <v>856.370</v>
       </c>
       <c r="G232" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H232" s="3">
-        <v>45675.62</v>
+        <v>32198.67</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7807,13 +7783,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>3217.960</v>
+        <v>56.100</v>
       </c>
       <c r="G233" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H233" s="3">
-        <v>14122.61</v>
+        <v>559.85</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7833,13 +7809,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>29.390</v>
+        <v>12.800</v>
       </c>
       <c r="G234" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H234" s="3">
-        <v>15217.18</v>
+        <v>286.57</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7859,13 +7835,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>856.370</v>
+        <v>1824.020</v>
       </c>
       <c r="G235" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H235" s="3">
-        <v>32198.67</v>
+        <v>57304.24</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7885,13 +7861,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>2.100</v>
+        <v>211.090</v>
       </c>
       <c r="G236" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H236" s="3">
-        <v>20.96</v>
+        <v>19367.87</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -7911,13 +7887,13 @@
         <v>476</v>
       </c>
       <c r="F237" s="2">
-        <v>12.800</v>
+        <v>59.100</v>
       </c>
       <c r="G237" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H237" s="3">
-        <v>286.57</v>
+        <v>9271.17</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7937,13 +7913,13 @@
         <v>478</v>
       </c>
       <c r="F238" s="2">
-        <v>427.520</v>
+        <v>237.900</v>
       </c>
       <c r="G238" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H238" s="3">
-        <v>13431.16</v>
+        <v>7688.51</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -7963,13 +7939,13 @@
         <v>480</v>
       </c>
       <c r="F239" s="2">
-        <v>211.090</v>
+        <v>91.020</v>
       </c>
       <c r="G239" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H239" s="3">
-        <v>19367.87</v>
+        <v>1685.63</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7989,13 +7965,13 @@
         <v>482</v>
       </c>
       <c r="F240" s="2">
-        <v>59.100</v>
+        <v>48.790</v>
       </c>
       <c r="G240" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H240" s="3">
-        <v>9271.17</v>
+        <v>1048.10</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8015,13 +7991,13 @@
         <v>484</v>
       </c>
       <c r="F241" s="2">
-        <v>237.900</v>
+        <v>78.310</v>
       </c>
       <c r="G241" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="H241" s="3">
-        <v>7688.51</v>
+        <v>7083.14</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -8041,13 +8017,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>91.020</v>
+        <v>203.000</v>
       </c>
       <c r="G242" t="s">
-        <v>438</v>
+        <v>5</v>
       </c>
       <c r="H242" s="3">
-        <v>1685.63</v>
+        <v>1188.56</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8067,13 +8043,13 @@
         <v>488</v>
       </c>
       <c r="F243" s="2">
-        <v>48.790</v>
+        <v>72.000</v>
       </c>
       <c r="G243" t="s">
-        <v>438</v>
+        <v>5</v>
       </c>
       <c r="H243" s="3">
-        <v>1048.10</v>
+        <v>396.64</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -8093,13 +8069,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>78.310</v>
+        <v>5851.000</v>
       </c>
       <c r="G244" t="s">
-        <v>438</v>
+        <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>7083.14</v>
+        <v>14688.16</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8119,13 +8095,13 @@
         <v>492</v>
       </c>
       <c r="F245" s="2">
-        <v>203.000</v>
+        <v>8.000</v>
       </c>
       <c r="G245" t="s">
         <v>5</v>
       </c>
       <c r="H245" s="3">
-        <v>1188.57</v>
+        <v>2847.85</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8145,13 +8121,13 @@
         <v>494</v>
       </c>
       <c r="F246" s="2">
-        <v>73.000</v>
+        <v>5.000</v>
       </c>
       <c r="G246" t="s">
         <v>5</v>
       </c>
       <c r="H246" s="3">
-        <v>402.15</v>
+        <v>2783.70</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -8171,13 +8147,13 @@
         <v>496</v>
       </c>
       <c r="F247" s="2">
-        <v>5594.000</v>
+        <v>8.000</v>
       </c>
       <c r="G247" t="s">
         <v>5</v>
       </c>
       <c r="H247" s="3">
-        <v>14042.98</v>
+        <v>3448.12</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -8197,13 +8173,13 @@
         <v>498</v>
       </c>
       <c r="F248" s="2">
-        <v>8.000</v>
+        <v>5.000</v>
       </c>
       <c r="G248" t="s">
         <v>5</v>
       </c>
       <c r="H248" s="3">
-        <v>2847.85</v>
+        <v>1976.50</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -8223,13 +8199,13 @@
         <v>500</v>
       </c>
       <c r="F249" s="2">
-        <v>6.000</v>
+        <v>2.000</v>
       </c>
       <c r="G249" t="s">
         <v>5</v>
       </c>
       <c r="H249" s="3">
-        <v>3340.44</v>
+        <v>2323.99</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -8249,13 +8225,13 @@
         <v>502</v>
       </c>
       <c r="F250" s="2">
-        <v>8.000</v>
+        <v>1.000</v>
       </c>
       <c r="G250" t="s">
         <v>5</v>
       </c>
       <c r="H250" s="3">
-        <v>3448.12</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -8275,13 +8251,13 @@
         <v>504</v>
       </c>
       <c r="F251" s="2">
-        <v>6.000</v>
+        <v>1.000</v>
       </c>
       <c r="G251" t="s">
         <v>5</v>
       </c>
       <c r="H251" s="3">
-        <v>2371.80</v>
+        <v>6585.02</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -8301,13 +8277,13 @@
         <v>506</v>
       </c>
       <c r="F252" s="2">
-        <v>2.000</v>
+        <v>6.000</v>
       </c>
       <c r="G252" t="s">
         <v>5</v>
       </c>
       <c r="H252" s="3">
-        <v>2323.99</v>
+        <v>1694.29</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -8327,13 +8303,13 @@
         <v>508</v>
       </c>
       <c r="F253" s="2">
-        <v>1.000</v>
+        <v>44.000</v>
       </c>
       <c r="G253" t="s">
         <v>5</v>
       </c>
       <c r="H253" s="3">
-        <v>1462.82</v>
+        <v>20336.56</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -8353,13 +8329,13 @@
         <v>510</v>
       </c>
       <c r="F254" s="2">
-        <v>1.000</v>
+        <v>8.000</v>
       </c>
       <c r="G254" t="s">
         <v>5</v>
       </c>
       <c r="H254" s="3">
-        <v>6585.02</v>
+        <v>4529.21</v>
       </c>
     </row>
     <row r="255" spans="1:8">
@@ -8379,13 +8355,13 @@
         <v>512</v>
       </c>
       <c r="F255" s="2">
-        <v>6.000</v>
+        <v>4.000</v>
       </c>
       <c r="G255" t="s">
         <v>5</v>
       </c>
       <c r="H255" s="3">
-        <v>1694.29</v>
+        <v>6821.40</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -8405,13 +8381,13 @@
         <v>514</v>
       </c>
       <c r="F256" s="2">
-        <v>44.000</v>
+        <v>2.000</v>
       </c>
       <c r="G256" t="s">
         <v>5</v>
       </c>
       <c r="H256" s="3">
-        <v>20336.56</v>
+        <v>7220.40</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -8431,13 +8407,13 @@
         <v>516</v>
       </c>
       <c r="F257" s="2">
-        <v>8.000</v>
+        <v>6.000</v>
       </c>
       <c r="G257" t="s">
         <v>5</v>
       </c>
       <c r="H257" s="3">
-        <v>4529.21</v>
+        <v>2199.61</v>
       </c>
     </row>
     <row r="258" spans="1:8">
@@ -8457,13 +8433,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>1.000</v>
+        <v>16.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>1721.73</v>
+        <v>7363.28</v>
       </c>
     </row>
     <row r="259" spans="1:8">
@@ -8483,13 +8459,13 @@
         <v>520</v>
       </c>
       <c r="F259" s="2">
-        <v>4.000</v>
+        <v>7.000</v>
       </c>
       <c r="G259" t="s">
         <v>5</v>
       </c>
       <c r="H259" s="3">
-        <v>6821.40</v>
+        <v>3943.24</v>
       </c>
     </row>
     <row r="260" spans="1:8">
@@ -8509,13 +8485,13 @@
         <v>522</v>
       </c>
       <c r="F260" s="2">
-        <v>2.000</v>
+        <v>5.000</v>
       </c>
       <c r="G260" t="s">
         <v>5</v>
       </c>
       <c r="H260" s="3">
-        <v>7220.40</v>
+        <v>2725.89</v>
       </c>
     </row>
     <row r="261" spans="1:8">
@@ -8535,116 +8511,12 @@
         <v>524</v>
       </c>
       <c r="F261" s="2">
-        <v>7.000</v>
+        <v>3.000</v>
       </c>
       <c r="G261" t="s">
         <v>5</v>
       </c>
       <c r="H261" s="3">
-        <v>2566.22</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8">
-      <c r="A262" t="s">
-        <v>0</v>
-      </c>
-      <c r="B262" t="s">
-        <v>1</v>
-      </c>
-      <c r="C262" t="s">
-        <v>2</v>
-      </c>
-      <c r="D262" t="s">
-        <v>525</v>
-      </c>
-      <c r="E262" t="s">
-        <v>526</v>
-      </c>
-      <c r="F262" s="2">
-        <v>16.000</v>
-      </c>
-      <c r="G262" t="s">
-        <v>5</v>
-      </c>
-      <c r="H262" s="3">
-        <v>7363.28</v>
-      </c>
-    </row>
-    <row r="263" spans="1:8">
-      <c r="A263" t="s">
-        <v>0</v>
-      </c>
-      <c r="B263" t="s">
-        <v>1</v>
-      </c>
-      <c r="C263" t="s">
-        <v>2</v>
-      </c>
-      <c r="D263" t="s">
-        <v>527</v>
-      </c>
-      <c r="E263" t="s">
-        <v>528</v>
-      </c>
-      <c r="F263" s="2">
-        <v>7.000</v>
-      </c>
-      <c r="G263" t="s">
-        <v>5</v>
-      </c>
-      <c r="H263" s="3">
-        <v>3943.24</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8">
-      <c r="A264" t="s">
-        <v>0</v>
-      </c>
-      <c r="B264" t="s">
-        <v>1</v>
-      </c>
-      <c r="C264" t="s">
-        <v>2</v>
-      </c>
-      <c r="D264" t="s">
-        <v>529</v>
-      </c>
-      <c r="E264" t="s">
-        <v>530</v>
-      </c>
-      <c r="F264" s="2">
-        <v>5.000</v>
-      </c>
-      <c r="G264" t="s">
-        <v>5</v>
-      </c>
-      <c r="H264" s="3">
-        <v>2725.89</v>
-      </c>
-    </row>
-    <row r="265" spans="1:8">
-      <c r="A265" t="s">
-        <v>0</v>
-      </c>
-      <c r="B265" t="s">
-        <v>1</v>
-      </c>
-      <c r="C265" t="s">
-        <v>2</v>
-      </c>
-      <c r="D265" t="s">
-        <v>531</v>
-      </c>
-      <c r="E265" t="s">
-        <v>532</v>
-      </c>
-      <c r="F265" s="2">
-        <v>3.000</v>
-      </c>
-      <c r="G265" t="s">
-        <v>5</v>
-      </c>
-      <c r="H265" s="3">
         <v>3602.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#fix: adjusted check Ordem status
</commit_message>
<xml_diff>
--- a/sheets/estoque_4600041302.XLSX
+++ b/sheets/estoque_4600041302.XLSX
@@ -271,12 +271,6 @@
     <t>COLAR TOMADA ACO INOX DN200A300 X DNR20</t>
   </si>
   <si>
-    <t>30004702</t>
-  </si>
-  <si>
-    <t>COLAR TOMADA ACO INOX DN50A150 X DNR20</t>
-  </si>
-  <si>
     <t>30004703</t>
   </si>
   <si>
@@ -521,6 +515,12 @@
   </si>
   <si>
     <t>EXTREMIDADE FF B JE2GS FLG DN300 PN10</t>
+  </si>
+  <si>
+    <t>30005514</t>
+  </si>
+  <si>
+    <t>EXTREMIDADE FF B JE2GS FLG DN75 PN10/16</t>
   </si>
   <si>
     <t>30005517</t>
@@ -1829,13 +1829,13 @@
         <v>9</v>
       </c>
       <c r="F4" s="2">
-        <v>15.000</v>
+        <v>14.000</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="3">
-        <v>13097.27</v>
+        <v>12224.12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2037,13 +2037,13 @@
         <v>25</v>
       </c>
       <c r="F12" s="2">
-        <v>15.000</v>
+        <v>35.000</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <v>313.91</v>
+        <v>732.45</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2167,13 +2167,13 @@
         <v>35</v>
       </c>
       <c r="F17" s="2">
-        <v>620.000</v>
+        <v>619.000</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="3">
-        <v>1271.00</v>
+        <v>1268.95</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2583,13 +2583,13 @@
         <v>67</v>
       </c>
       <c r="F33" s="2">
-        <v>8.000</v>
+        <v>5.000</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>460.48</v>
+        <v>287.80</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2661,13 +2661,13 @@
         <v>73</v>
       </c>
       <c r="F36" s="2">
-        <v>16.000</v>
+        <v>17.000</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="3">
-        <v>520.62</v>
+        <v>553.16</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2687,13 +2687,13 @@
         <v>75</v>
       </c>
       <c r="F37" s="2">
-        <v>5.000</v>
+        <v>3.000</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="3">
-        <v>279.52</v>
+        <v>167.71</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2739,13 +2739,13 @@
         <v>79</v>
       </c>
       <c r="F39" s="2">
-        <v>154.000</v>
+        <v>149.000</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>7234.15</v>
+        <v>6999.27</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2791,13 +2791,13 @@
         <v>83</v>
       </c>
       <c r="F41" s="2">
-        <v>365.000</v>
+        <v>401.000</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="3">
-        <v>10386.52</v>
+        <v>11410.94</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2817,13 +2817,13 @@
         <v>85</v>
       </c>
       <c r="F42" s="2">
-        <v>103.000</v>
+        <v>102.000</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="3">
-        <v>16330.14</v>
+        <v>16171.59</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2843,13 +2843,13 @@
         <v>87</v>
       </c>
       <c r="F43" s="2">
-        <v>5.000</v>
+        <v>53.000</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>2793.87</v>
+        <v>4672.30</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2869,13 +2869,13 @@
         <v>89</v>
       </c>
       <c r="F44" s="2">
-        <v>54.000</v>
+        <v>61.000</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="3">
-        <v>4760.46</v>
+        <v>11586.65</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2895,13 +2895,13 @@
         <v>91</v>
       </c>
       <c r="F45" s="2">
-        <v>94.000</v>
+        <v>46.000</v>
       </c>
       <c r="G45" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="3">
-        <v>17854.87</v>
+        <v>2898.44</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2921,13 +2921,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="2">
-        <v>46.000</v>
+        <v>2.000</v>
       </c>
       <c r="G46" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="3">
-        <v>2898.44</v>
+        <v>603.23</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2947,13 +2947,13 @@
         <v>95</v>
       </c>
       <c r="F47" s="2">
-        <v>2.000</v>
+        <v>17.000</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="3">
-        <v>603.23</v>
+        <v>2384.28</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2973,13 +2973,13 @@
         <v>97</v>
       </c>
       <c r="F48" s="2">
-        <v>14.000</v>
+        <v>16.000</v>
       </c>
       <c r="G48" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="3">
-        <v>1963.52</v>
+        <v>3348.74</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2999,13 +2999,13 @@
         <v>99</v>
       </c>
       <c r="F49" s="2">
-        <v>16.000</v>
+        <v>8.000</v>
       </c>
       <c r="G49" t="s">
         <v>5</v>
       </c>
       <c r="H49" s="3">
-        <v>3348.74</v>
+        <v>2352.96</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3025,13 +3025,13 @@
         <v>101</v>
       </c>
       <c r="F50" s="2">
-        <v>8.000</v>
+        <v>9.000</v>
       </c>
       <c r="G50" t="s">
         <v>5</v>
       </c>
       <c r="H50" s="3">
-        <v>2352.96</v>
+        <v>3592.71</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3051,13 +3051,13 @@
         <v>103</v>
       </c>
       <c r="F51" s="2">
-        <v>9.000</v>
+        <v>1.000</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
       </c>
       <c r="H51" s="3">
-        <v>3592.71</v>
+        <v>863.17</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3077,13 +3077,13 @@
         <v>105</v>
       </c>
       <c r="F52" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="G52" t="s">
         <v>5</v>
       </c>
       <c r="H52" s="3">
-        <v>863.17</v>
+        <v>295.57</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3103,13 +3103,13 @@
         <v>107</v>
       </c>
       <c r="F53" s="2">
-        <v>3.000</v>
+        <v>793.000</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
       </c>
       <c r="H53" s="3">
-        <v>295.57</v>
+        <v>7196.41</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3129,13 +3129,13 @@
         <v>109</v>
       </c>
       <c r="F54" s="2">
-        <v>917.000</v>
+        <v>37.000</v>
       </c>
       <c r="G54" t="s">
         <v>5</v>
       </c>
       <c r="H54" s="3">
-        <v>8321.58</v>
+        <v>593.09</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3155,13 +3155,13 @@
         <v>111</v>
       </c>
       <c r="F55" s="2">
-        <v>37.000</v>
+        <v>3824.000</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
       </c>
       <c r="H55" s="3">
-        <v>593.09</v>
+        <v>39297.13</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3181,13 +3181,13 @@
         <v>113</v>
       </c>
       <c r="F56" s="2">
-        <v>3514.000</v>
+        <v>11.000</v>
       </c>
       <c r="G56" t="s">
         <v>5</v>
       </c>
       <c r="H56" s="3">
-        <v>36111.64</v>
+        <v>380.69</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -3207,13 +3207,13 @@
         <v>115</v>
       </c>
       <c r="F57" s="2">
-        <v>11.000</v>
+        <v>8.000</v>
       </c>
       <c r="G57" t="s">
         <v>5</v>
       </c>
       <c r="H57" s="3">
-        <v>380.69</v>
+        <v>297.38</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3233,13 +3233,13 @@
         <v>117</v>
       </c>
       <c r="F58" s="2">
-        <v>8.000</v>
+        <v>5.000</v>
       </c>
       <c r="G58" t="s">
         <v>5</v>
       </c>
       <c r="H58" s="3">
-        <v>297.38</v>
+        <v>1454.70</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3259,13 +3259,13 @@
         <v>119</v>
       </c>
       <c r="F59" s="2">
-        <v>5.000</v>
+        <v>23.000</v>
       </c>
       <c r="G59" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="3">
-        <v>1454.70</v>
+        <v>1071.88</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3285,13 +3285,13 @@
         <v>121</v>
       </c>
       <c r="F60" s="2">
-        <v>23.000</v>
+        <v>11.000</v>
       </c>
       <c r="G60" t="s">
         <v>5</v>
       </c>
       <c r="H60" s="3">
-        <v>1071.88</v>
+        <v>1357.53</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3311,13 +3311,13 @@
         <v>123</v>
       </c>
       <c r="F61" s="2">
-        <v>11.000</v>
+        <v>16.000</v>
       </c>
       <c r="G61" t="s">
         <v>5</v>
       </c>
       <c r="H61" s="3">
-        <v>1357.53</v>
+        <v>902.16</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3337,13 +3337,13 @@
         <v>125</v>
       </c>
       <c r="F62" s="2">
-        <v>16.000</v>
+        <v>26.000</v>
       </c>
       <c r="G62" t="s">
         <v>5</v>
       </c>
       <c r="H62" s="3">
-        <v>902.16</v>
+        <v>2051.47</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3363,13 +3363,13 @@
         <v>127</v>
       </c>
       <c r="F63" s="2">
-        <v>26.000</v>
+        <v>19.000</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
       </c>
       <c r="H63" s="3">
-        <v>2051.47</v>
+        <v>565.15</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3389,13 +3389,13 @@
         <v>129</v>
       </c>
       <c r="F64" s="2">
-        <v>19.000</v>
+        <v>36.000</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
       </c>
       <c r="H64" s="3">
-        <v>565.15</v>
+        <v>2051.36</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3415,13 +3415,13 @@
         <v>131</v>
       </c>
       <c r="F65" s="2">
-        <v>36.000</v>
+        <v>4.000</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <v>2051.36</v>
+        <v>606.42</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3441,13 +3441,13 @@
         <v>133</v>
       </c>
       <c r="F66" s="2">
-        <v>4.000</v>
+        <v>1.000</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>606.42</v>
+        <v>1448.47</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3467,13 +3467,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2">
-        <v>1.000</v>
+        <v>1570.000</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
       </c>
       <c r="H67" s="3">
-        <v>1448.47</v>
+        <v>7911.96</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3493,13 +3493,13 @@
         <v>137</v>
       </c>
       <c r="F68" s="2">
-        <v>1480.000</v>
+        <v>23.000</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="3">
-        <v>7458.41</v>
+        <v>1396.09</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3519,13 +3519,13 @@
         <v>139</v>
       </c>
       <c r="F69" s="2">
-        <v>23.000</v>
+        <v>47.000</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
       </c>
       <c r="H69" s="3">
-        <v>1396.09</v>
+        <v>6987.50</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3545,13 +3545,13 @@
         <v>141</v>
       </c>
       <c r="F70" s="2">
-        <v>47.000</v>
+        <v>180.000</v>
       </c>
       <c r="G70" t="s">
         <v>5</v>
       </c>
       <c r="H70" s="3">
-        <v>6987.50</v>
+        <v>1598.51</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3571,13 +3571,13 @@
         <v>143</v>
       </c>
       <c r="F71" s="2">
-        <v>180.000</v>
+        <v>13.000</v>
       </c>
       <c r="G71" t="s">
         <v>5</v>
       </c>
       <c r="H71" s="3">
-        <v>1598.51</v>
+        <v>738.14</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3597,13 +3597,13 @@
         <v>145</v>
       </c>
       <c r="F72" s="2">
-        <v>13.000</v>
+        <v>6.000</v>
       </c>
       <c r="G72" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="3">
-        <v>738.14</v>
+        <v>344.01</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3623,13 +3623,13 @@
         <v>147</v>
       </c>
       <c r="F73" s="2">
-        <v>6.000</v>
+        <v>18.000</v>
       </c>
       <c r="G73" t="s">
         <v>5</v>
       </c>
       <c r="H73" s="3">
-        <v>344.01</v>
+        <v>1877.58</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3649,13 +3649,13 @@
         <v>149</v>
       </c>
       <c r="F74" s="2">
-        <v>18.000</v>
+        <v>46.000</v>
       </c>
       <c r="G74" t="s">
         <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>1877.58</v>
+        <v>4738.33</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3675,13 +3675,13 @@
         <v>151</v>
       </c>
       <c r="F75" s="2">
-        <v>46.000</v>
+        <v>2.000</v>
       </c>
       <c r="G75" t="s">
         <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>4738.33</v>
+        <v>495.95</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3701,13 +3701,13 @@
         <v>153</v>
       </c>
       <c r="F76" s="2">
-        <v>2.000</v>
+        <v>46.000</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
       </c>
       <c r="H76" s="3">
-        <v>495.95</v>
+        <v>854.65</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3727,13 +3727,13 @@
         <v>155</v>
       </c>
       <c r="F77" s="2">
-        <v>71.000</v>
+        <v>1.000</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>1319.15</v>
+        <v>86.93</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3753,13 +3753,13 @@
         <v>157</v>
       </c>
       <c r="F78" s="2">
-        <v>1.000</v>
+        <v>1084.000</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>86.93</v>
+        <v>6662.40</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3779,13 +3779,13 @@
         <v>159</v>
       </c>
       <c r="F79" s="2">
-        <v>1148.000</v>
+        <v>19.000</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>7055.88</v>
+        <v>207.19</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3805,13 +3805,13 @@
         <v>161</v>
       </c>
       <c r="F80" s="2">
-        <v>19.000</v>
+        <v>2923.000</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>207.19</v>
+        <v>76136.43</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3831,13 +3831,13 @@
         <v>163</v>
       </c>
       <c r="F81" s="2">
-        <v>2865.000</v>
+        <v>3.000</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
       </c>
       <c r="H81" s="3">
-        <v>74626.01</v>
+        <v>229.84</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3863,7 +3863,7 @@
         <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>229.84</v>
+        <v>651.71</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3889,7 +3889,7 @@
         <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>651.71</v>
+        <v>1263.43</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -3909,13 +3909,13 @@
         <v>169</v>
       </c>
       <c r="F84" s="2">
-        <v>3.000</v>
+        <v>1.000</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>1263.43</v>
+        <v>158.11</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -3961,13 +3961,13 @@
         <v>173</v>
       </c>
       <c r="F86" s="2">
-        <v>4.000</v>
+        <v>6.000</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>1008.05</v>
+        <v>1512.07</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4065,13 +4065,13 @@
         <v>181</v>
       </c>
       <c r="F90" s="2">
-        <v>134.000</v>
+        <v>132.000</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>5051.13</v>
+        <v>4975.74</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4195,13 +4195,13 @@
         <v>191</v>
       </c>
       <c r="F95" s="2">
-        <v>223.000</v>
+        <v>213.000</v>
       </c>
       <c r="G95" t="s">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>18877.36</v>
+        <v>18030.86</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4221,13 +4221,13 @@
         <v>193</v>
       </c>
       <c r="F96" s="2">
-        <v>2248.000</v>
+        <v>2627.000</v>
       </c>
       <c r="G96" t="s">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>316120.96</v>
+        <v>369417.52</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4305,7 +4305,7 @@
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>1598.30</v>
+        <v>1604.59</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -4565,7 +4565,7 @@
         <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>2825.06</v>
+        <v>2651.55</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4637,13 +4637,13 @@
         <v>225</v>
       </c>
       <c r="F112" s="2">
-        <v>651.000</v>
+        <v>633.000</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>24159.17</v>
+        <v>23491.18</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -4663,13 +4663,13 @@
         <v>227</v>
       </c>
       <c r="F113" s="2">
-        <v>349.000</v>
+        <v>340.000</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>22813.65</v>
+        <v>22225.32</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -4689,13 +4689,13 @@
         <v>229</v>
       </c>
       <c r="F114" s="2">
-        <v>920.000</v>
+        <v>855.000</v>
       </c>
       <c r="G114" t="s">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>30310.68</v>
+        <v>28169.05</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -4741,13 +4741,13 @@
         <v>233</v>
       </c>
       <c r="F116" s="2">
-        <v>24.000</v>
+        <v>22.000</v>
       </c>
       <c r="G116" t="s">
         <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>2538.29</v>
+        <v>2326.77</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -4767,13 +4767,13 @@
         <v>235</v>
       </c>
       <c r="F117" s="2">
-        <v>49.000</v>
+        <v>57.000</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>1654.46</v>
+        <v>1924.58</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -4793,13 +4793,13 @@
         <v>237</v>
       </c>
       <c r="F118" s="2">
-        <v>9.000</v>
+        <v>15.000</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>1675.75</v>
+        <v>2792.92</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -4819,13 +4819,13 @@
         <v>239</v>
       </c>
       <c r="F119" s="2">
-        <v>11810.000</v>
+        <v>11274.000</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>45886.97</v>
+        <v>43802.99</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -5105,13 +5105,13 @@
         <v>261</v>
       </c>
       <c r="F130" s="2">
-        <v>554.000</v>
+        <v>547.000</v>
       </c>
       <c r="G130" t="s">
         <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>3136.11</v>
+        <v>3096.49</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5131,13 +5131,13 @@
         <v>263</v>
       </c>
       <c r="F131" s="2">
-        <v>171.000</v>
+        <v>151.000</v>
       </c>
       <c r="G131" t="s">
         <v>5</v>
       </c>
       <c r="H131" s="3">
-        <v>1405.96</v>
+        <v>1241.52</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5157,13 +5157,13 @@
         <v>265</v>
       </c>
       <c r="F132" s="2">
-        <v>91.000</v>
+        <v>90.000</v>
       </c>
       <c r="G132" t="s">
         <v>5</v>
       </c>
       <c r="H132" s="3">
-        <v>1426.69</v>
+        <v>1411.01</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -5209,13 +5209,13 @@
         <v>269</v>
       </c>
       <c r="F134" s="2">
-        <v>78.000</v>
+        <v>86.000</v>
       </c>
       <c r="G134" t="s">
         <v>5</v>
       </c>
       <c r="H134" s="3">
-        <v>2380.78</v>
+        <v>2624.96</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -5235,13 +5235,13 @@
         <v>271</v>
       </c>
       <c r="F135" s="2">
-        <v>26.000</v>
+        <v>34.000</v>
       </c>
       <c r="G135" t="s">
         <v>5</v>
       </c>
       <c r="H135" s="3">
-        <v>3249.51</v>
+        <v>4249.36</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -5267,7 +5267,7 @@
         <v>5</v>
       </c>
       <c r="H136" s="3">
-        <v>194.13</v>
+        <v>191.28</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5859,13 +5859,13 @@
         <v>319</v>
       </c>
       <c r="F159" s="2">
-        <v>47.000</v>
+        <v>51.000</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
       </c>
       <c r="H159" s="3">
-        <v>6275.29</v>
+        <v>6809.36</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -6223,13 +6223,13 @@
         <v>346</v>
       </c>
       <c r="F173" s="2">
-        <v>2456.000</v>
+        <v>2473.000</v>
       </c>
       <c r="G173" t="s">
         <v>5</v>
       </c>
       <c r="H173" s="3">
-        <v>45988.60</v>
+        <v>46306.92</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6249,13 +6249,13 @@
         <v>348</v>
       </c>
       <c r="F174" s="2">
-        <v>215651.000</v>
+        <v>213936.000</v>
       </c>
       <c r="G174" t="s">
         <v>349</v>
       </c>
       <c r="H174" s="3">
-        <v>327871.67</v>
+        <v>324779.95</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -6301,13 +6301,13 @@
         <v>353</v>
       </c>
       <c r="F176" s="2">
-        <v>615.000</v>
+        <v>577.000</v>
       </c>
       <c r="G176" t="s">
         <v>5</v>
       </c>
       <c r="H176" s="3">
-        <v>107389.35</v>
+        <v>100753.90</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6405,13 +6405,13 @@
         <v>361</v>
       </c>
       <c r="F180" s="2">
-        <v>84.000</v>
+        <v>56.000</v>
       </c>
       <c r="G180" t="s">
         <v>5</v>
       </c>
       <c r="H180" s="3">
-        <v>38976.93</v>
+        <v>25984.62</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6431,13 +6431,13 @@
         <v>363</v>
       </c>
       <c r="F181" s="2">
-        <v>46.000</v>
+        <v>47.000</v>
       </c>
       <c r="G181" t="s">
         <v>5</v>
       </c>
       <c r="H181" s="3">
-        <v>2809.22</v>
+        <v>2870.29</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6457,13 +6457,13 @@
         <v>365</v>
       </c>
       <c r="F182" s="2">
-        <v>75.000</v>
+        <v>70.000</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
       </c>
       <c r="H182" s="3">
-        <v>10771.45</v>
+        <v>10053.35</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6593,7 +6593,7 @@
         <v>5</v>
       </c>
       <c r="H187" s="3">
-        <v>7566.20</v>
+        <v>7566.25</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6639,13 +6639,13 @@
         <v>379</v>
       </c>
       <c r="F189" s="2">
-        <v>509.000</v>
+        <v>503.000</v>
       </c>
       <c r="G189" t="s">
         <v>5</v>
       </c>
       <c r="H189" s="3">
-        <v>10312.34</v>
+        <v>10190.78</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -7679,13 +7679,13 @@
         <v>460</v>
       </c>
       <c r="F229" s="2">
-        <v>19336.700</v>
+        <v>21197.200</v>
       </c>
       <c r="G229" t="s">
         <v>430</v>
       </c>
       <c r="H229" s="3">
-        <v>43875.97</v>
+        <v>48516.61</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7705,13 +7705,13 @@
         <v>462</v>
       </c>
       <c r="F230" s="2">
-        <v>3213.960</v>
+        <v>3192.960</v>
       </c>
       <c r="G230" t="s">
         <v>430</v>
       </c>
       <c r="H230" s="3">
-        <v>14105.06</v>
+        <v>14012.90</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -7783,13 +7783,13 @@
         <v>468</v>
       </c>
       <c r="F233" s="2">
-        <v>56.100</v>
+        <v>0.600</v>
       </c>
       <c r="G233" t="s">
         <v>430</v>
       </c>
       <c r="H233" s="3">
-        <v>559.85</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7809,13 +7809,13 @@
         <v>470</v>
       </c>
       <c r="F234" s="2">
-        <v>12.800</v>
+        <v>0.800</v>
       </c>
       <c r="G234" t="s">
         <v>430</v>
       </c>
       <c r="H234" s="3">
-        <v>286.57</v>
+        <v>17.91</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7835,13 +7835,13 @@
         <v>472</v>
       </c>
       <c r="F235" s="2">
-        <v>1824.020</v>
+        <v>1823.020</v>
       </c>
       <c r="G235" t="s">
         <v>430</v>
       </c>
       <c r="H235" s="3">
-        <v>57304.24</v>
+        <v>57272.82</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -7861,13 +7861,13 @@
         <v>474</v>
       </c>
       <c r="F236" s="2">
-        <v>211.090</v>
+        <v>319.090</v>
       </c>
       <c r="G236" t="s">
         <v>430</v>
       </c>
       <c r="H236" s="3">
-        <v>19367.87</v>
+        <v>29277.05</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -8017,13 +8017,13 @@
         <v>486</v>
       </c>
       <c r="F242" s="2">
-        <v>203.000</v>
+        <v>221.000</v>
       </c>
       <c r="G242" t="s">
         <v>5</v>
       </c>
       <c r="H242" s="3">
-        <v>1188.56</v>
+        <v>1293.95</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -8069,13 +8069,13 @@
         <v>490</v>
       </c>
       <c r="F244" s="2">
-        <v>5851.000</v>
+        <v>5879.000</v>
       </c>
       <c r="G244" t="s">
         <v>5</v>
       </c>
       <c r="H244" s="3">
-        <v>14688.16</v>
+        <v>14758.48</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -8433,13 +8433,13 @@
         <v>518</v>
       </c>
       <c r="F258" s="2">
-        <v>16.000</v>
+        <v>17.000</v>
       </c>
       <c r="G258" t="s">
         <v>5</v>
       </c>
       <c r="H258" s="3">
-        <v>7363.28</v>
+        <v>7823.48</v>
       </c>
     </row>
     <row r="259" spans="1:8">

</xml_diff>